<commit_message>
Updating BOM; there were some parts that were incorrect vs. what's actually used in the machines.
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -5,22 +5,33 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajohnson\GIT_Projects\ValpoFilamentRecycler09\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamj\Git Projects\ValpoFilamentRecycler09\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E5A90E-8A86-47E8-A86B-38515DEEF7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2328994-ADA5-4D16-ACDB-96EC6E1E63B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2880" yWindow="0" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="255">
   <si>
     <t>Quantity</t>
   </si>
@@ -100,9 +111,6 @@
     <t>GlobTek Inc</t>
   </si>
   <si>
-    <t>1866-5173-ND</t>
-  </si>
-  <si>
     <t>Mean Well USA</t>
   </si>
   <si>
@@ -439,16 +447,9 @@
     <t>3201776F6000(R)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 
-ERPF-400-24</t>
-  </si>
-  <si>
     <t>PQDE6W-Q24-S5-T</t>
   </si>
   <si>
-    <t>AC/DC Converter, 24V, 16.7A</t>
-  </si>
-  <si>
     <t>A000067</t>
   </si>
   <si>
@@ -786,6 +787,15 @@
   </si>
   <si>
     <t>SMPW-K-M</t>
+  </si>
+  <si>
+    <t>AC/DC Converter, 24V, 8.8A</t>
+  </si>
+  <si>
+    <t>SE-200-24-ND</t>
+  </si>
+  <si>
+    <t>SE-200-24</t>
   </si>
 </sst>
 </file>
@@ -1184,8 +1194,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6961DE25-1017-49FB-B58C-151DD971B349}" name="TableExtruder" displayName="TableExtruder" ref="A1:J77" totalsRowCount="1" dataCellStyle="Normal">
   <autoFilter ref="A1:J76" xr:uid="{6961DE25-1017-49FB-B58C-151DD971B349}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J51">
-    <sortCondition ref="D1:D51"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J50">
+    <sortCondition ref="D1:D50"/>
   </sortState>
   <tableColumns count="10">
     <tableColumn id="13" xr3:uid="{F1D7053F-785C-43EA-8460-9A24903A67E6}" name="Machine" totalsRowDxfId="9"/>
@@ -1408,50 +1418,50 @@
   </sheetPr>
   <dimension ref="A1:P80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.33203125" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="30.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
@@ -1460,30 +1470,30 @@
         <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
     </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="3">
@@ -1500,24 +1510,24 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="3">
@@ -1534,15 +1544,15 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>6</v>
@@ -1566,24 +1576,24 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="3">
@@ -1600,24 +1610,24 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>106</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="3">
@@ -1634,21 +1644,21 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="1"/>
@@ -1666,21 +1676,21 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="1"/>
@@ -1698,21 +1708,21 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>86</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="1"/>
@@ -1730,21 +1740,21 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="1"/>
@@ -1762,55 +1772,53 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>98</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="F11" s="3"/>
       <c r="G11" s="1"/>
       <c r="H11" s="3">
         <v>1</v>
       </c>
       <c r="I11" s="2">
-        <v>29.38</v>
+        <v>7.41</v>
       </c>
       <c r="J11" s="4">
         <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>29.38</v>
+        <v>7.41</v>
       </c>
       <c r="K11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>199</v>
+        <v>132</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="1"/>
@@ -1818,59 +1826,65 @@
         <v>1</v>
       </c>
       <c r="I12" s="2">
-        <v>15.1</v>
+        <v>5.66</v>
       </c>
       <c r="J12" s="4">
         <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>15.1</v>
+        <v>5.66</v>
       </c>
       <c r="K12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="B13" s="13"/>
+        <v>216</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>223</v>
+      </c>
       <c r="C13" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F13" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="3">
         <v>1</v>
       </c>
       <c r="I13" s="2">
-        <v>7.41</v>
+        <v>29.38</v>
       </c>
       <c r="J13" s="4">
         <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>7.41</v>
+        <v>29.38</v>
       </c>
       <c r="K13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="B14" s="13"/>
+        <v>216</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>223</v>
+      </c>
       <c r="C14" s="3" t="s">
-        <v>133</v>
+        <v>196</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="1"/>
@@ -1878,22 +1892,22 @@
         <v>1</v>
       </c>
       <c r="I14" s="2">
-        <v>5.66</v>
+        <v>15.1</v>
       </c>
       <c r="J14" s="4">
         <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>5.66</v>
+        <v>15.1</v>
       </c>
       <c r="K14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>19</v>
@@ -1924,24 +1938,24 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="G16" s="1">
         <v>108050</v>
@@ -1960,27 +1974,27 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="E17" s="1">
         <v>37769</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H17" s="1">
         <v>2</v>
@@ -1996,21 +2010,21 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1">
@@ -2027,27 +2041,27 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E19" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="G19" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H19" s="3">
         <v>2</v>
@@ -2063,21 +2077,21 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1">
@@ -2094,12 +2108,12 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>17</v>
@@ -2109,7 +2123,7 @@
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="3">
@@ -2126,27 +2140,27 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="H22" s="17">
         <v>2</v>
@@ -2160,21 +2174,21 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1">
@@ -2191,15 +2205,15 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
@@ -2217,21 +2231,21 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="1"/>
@@ -2249,15 +2263,15 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>24</v>
@@ -2269,7 +2283,7 @@
         <v>25</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H26" s="3">
         <v>1</v>
@@ -2285,27 +2299,27 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27" spans="1:16" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="H27" s="17">
         <v>2</v>
@@ -2316,15 +2330,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D28" s="17"/>
       <c r="E28" s="17"/>
@@ -2342,27 +2356,27 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
     </row>
-    <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>141</v>
+        <v>252</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E29" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="G29" s="6" t="s">
-        <v>139</v>
+        <v>254</v>
       </c>
       <c r="H29" s="3">
         <v>1</v>
@@ -2378,27 +2392,27 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
     </row>
-    <row r="30" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E30" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="G30" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H30" s="3">
         <v>1</v>
@@ -2414,24 +2428,24 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="H31" s="1">
         <v>1</v>
@@ -2447,27 +2461,27 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
     </row>
-    <row r="32" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H32" s="1">
         <v>2</v>
@@ -2483,11 +2497,13 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
     </row>
-    <row r="33" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="B33" s="13"/>
+        <v>216</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>239</v>
+      </c>
       <c r="C33" s="3" t="s">
         <v>4</v>
       </c>
@@ -2515,131 +2531,135 @@
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
     </row>
-    <row r="34" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>55</v>
+    <row r="34" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>157</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="H34" s="3">
-        <v>7</v>
-      </c>
-      <c r="I34" s="2">
-        <v>2.75</v>
+        <v>121</v>
+      </c>
+      <c r="H34" s="1">
+        <v>2</v>
+      </c>
+      <c r="I34" s="4">
+        <v>26.12</v>
       </c>
       <c r="J34" s="4">
         <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>19.25</v>
+        <v>52.24</v>
       </c>
       <c r="K34" s="1"/>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
     </row>
-    <row r="35" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="H35" s="1">
-        <v>2</v>
-      </c>
-      <c r="I35" s="4">
-        <v>26.12</v>
-      </c>
-      <c r="J35" s="4">
-        <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>52.24</v>
+    <row r="35" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="H35" s="3">
+        <v>1</v>
+      </c>
+      <c r="I35" s="5">
+        <v>38.5</v>
+      </c>
+      <c r="J35" s="5">
+        <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
+        <v>38.5</v>
       </c>
       <c r="K35" s="1"/>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
     </row>
-    <row r="36" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="H36" s="3">
-        <v>1</v>
-      </c>
-      <c r="I36" s="5">
-        <v>38.5</v>
-      </c>
-      <c r="J36" s="5">
-        <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>38.5</v>
+        <v>239</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G36" s="7">
+        <v>181</v>
+      </c>
+      <c r="H36" s="1">
+        <v>1</v>
+      </c>
+      <c r="I36" s="4">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="J36" s="4">
+        <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
+        <v>9.9499999999999993</v>
       </c>
       <c r="K36" s="1"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
     </row>
-    <row r="37" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>242</v>
+    <row r="37" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>239</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>143</v>
+        <v>171</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G37" s="7">
-        <v>181</v>
+        <v>110</v>
+      </c>
+      <c r="G37" s="1">
+        <v>292</v>
       </c>
       <c r="H37" s="1">
         <v>1</v>
@@ -2655,909 +2675,907 @@
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
     </row>
-    <row r="38" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>174</v>
+        <v>129</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G38" s="1">
-        <v>292</v>
+        <v>42</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>141</v>
       </c>
       <c r="H38" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I38" s="4">
-        <v>9.9499999999999993</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="J38" s="4">
         <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>9.9499999999999993</v>
+        <v>5.6499999999999995</v>
       </c>
       <c r="K38" s="1"/>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
     </row>
-    <row r="39" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>242</v>
-      </c>
+    <row r="39" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="B39" s="13"/>
       <c r="C39" s="1" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="H39" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I39" s="4">
-        <v>1.1299999999999999</v>
+        <v>0.63</v>
       </c>
       <c r="J39" s="4">
         <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>5.6499999999999995</v>
+        <v>2.52</v>
       </c>
       <c r="K39" s="1"/>
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
     </row>
-    <row r="40" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="B40" s="13"/>
+    <row r="40" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B40" s="8"/>
       <c r="C40" s="1" t="s">
-        <v>153</v>
+        <v>206</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>36</v>
+        <v>116</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>37</v>
+        <v>205</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>152</v>
+        <v>204</v>
       </c>
       <c r="H40" s="1">
-        <v>4</v>
-      </c>
-      <c r="I40" s="4">
-        <v>0.63</v>
+        <v>1</v>
+      </c>
+      <c r="I40" s="2">
+        <v>4.13</v>
       </c>
       <c r="J40" s="4">
         <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>2.52</v>
+        <v>4.13</v>
       </c>
       <c r="K40" s="1"/>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
     </row>
-    <row r="41" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="B41" s="8"/>
+    <row r="41" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="B41" s="13"/>
       <c r="C41" s="1" t="s">
-        <v>209</v>
+        <v>152</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>117</v>
+        <v>37</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>208</v>
+        <v>38</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>207</v>
+        <v>151</v>
       </c>
       <c r="H41" s="1">
         <v>1</v>
       </c>
-      <c r="I41" s="2">
-        <v>4.13</v>
+      <c r="I41" s="4">
+        <v>4.3</v>
       </c>
       <c r="J41" s="4">
         <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>4.13</v>
+        <v>4.3</v>
       </c>
       <c r="K41" s="1"/>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
     </row>
-    <row r="42" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B42" s="13"/>
       <c r="C42" s="1" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H42" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I42" s="4">
-        <v>4.3</v>
+        <v>0.47</v>
       </c>
       <c r="J42" s="4">
         <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>4.3</v>
+        <v>1.88</v>
       </c>
       <c r="K42" s="1"/>
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
     </row>
-    <row r="43" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B43" s="13"/>
       <c r="C43" s="1" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="H43" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I43" s="4">
-        <v>0.47</v>
+        <v>0.51</v>
       </c>
       <c r="J43" s="4">
         <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>1.88</v>
+        <v>1.02</v>
       </c>
       <c r="K43" s="1"/>
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
     </row>
-    <row r="44" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="B44" s="13"/>
+        <v>216</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>234</v>
+      </c>
       <c r="C44" s="1" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="H44" s="1">
         <v>2</v>
       </c>
       <c r="I44" s="4">
-        <v>0.51</v>
+        <v>1.2</v>
       </c>
       <c r="J44" s="4">
         <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>1.02</v>
+        <v>2.4</v>
       </c>
       <c r="K44" s="1"/>
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
     </row>
-    <row r="45" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="B45" s="13" t="s">
-        <v>237</v>
+    <row r="45" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>234</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="H45" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I45" s="4">
-        <v>1.2</v>
+        <v>2.56</v>
       </c>
       <c r="J45" s="4">
         <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>2.4</v>
+        <v>2.56</v>
       </c>
       <c r="K45" s="1"/>
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
     </row>
-    <row r="46" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>177</v>
+        <v>87</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>176</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="G46" s="1"/>
       <c r="H46" s="1">
         <v>1</v>
       </c>
       <c r="I46" s="4">
-        <v>2.56</v>
+        <v>43.8</v>
       </c>
       <c r="J46" s="4">
         <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>2.56</v>
+        <v>43.8</v>
       </c>
       <c r="K46" s="1"/>
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
     </row>
-    <row r="47" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>237</v>
+    <row r="47" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>234</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>78</v>
+        <v>24</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>89</v>
+        <v>118</v>
       </c>
       <c r="G47" s="1"/>
       <c r="H47" s="1">
         <v>1</v>
       </c>
-      <c r="I47" s="4">
-        <v>43.8</v>
+      <c r="I47" s="2">
+        <v>43.82</v>
       </c>
       <c r="J47" s="4">
         <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>43.8</v>
+        <v>43.82</v>
       </c>
       <c r="K47" s="1"/>
       <c r="O47" s="1"/>
       <c r="P47" s="1"/>
     </row>
-    <row r="48" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>237</v>
-      </c>
+    <row r="48" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
-        <v>118</v>
+        <v>221</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G48" s="1"/>
+        <v>122</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>209</v>
+      </c>
       <c r="H48" s="1">
         <v>1</v>
       </c>
       <c r="I48" s="2">
-        <v>43.82</v>
+        <v>13.88</v>
       </c>
       <c r="J48" s="4">
         <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>43.82</v>
+        <v>13.88</v>
       </c>
       <c r="K48" s="1"/>
       <c r="O48" s="1"/>
       <c r="P48" s="1"/>
     </row>
-    <row r="49" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="B49" s="1"/>
+    <row r="49" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B49" s="3"/>
       <c r="C49" s="1" t="s">
-        <v>224</v>
+        <v>144</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>212</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="G49" s="1"/>
       <c r="H49" s="1">
         <v>1</v>
       </c>
-      <c r="I49" s="2">
-        <v>13.88</v>
+      <c r="I49" s="4">
+        <v>13.77</v>
       </c>
       <c r="J49" s="4">
         <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>13.88</v>
+        <v>13.77</v>
       </c>
       <c r="K49" s="1"/>
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
     </row>
-    <row r="50" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="B50" s="3"/>
+    <row r="50" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G50" s="1"/>
+        <v>112</v>
+      </c>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="H50" s="1">
         <v>1</v>
       </c>
-      <c r="I50" s="4">
-        <v>13.77</v>
+      <c r="I50" s="2">
+        <v>32.1</v>
       </c>
       <c r="J50" s="4">
         <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>13.77</v>
+        <v>32.1</v>
       </c>
       <c r="K50" s="1"/>
       <c r="O50" s="1"/>
       <c r="P50" s="1"/>
     </row>
-    <row r="51" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="H51" s="1">
-        <v>1</v>
-      </c>
-      <c r="I51" s="2">
-        <v>32.1</v>
-      </c>
-      <c r="J51" s="4">
-        <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>32.1</v>
+    <row r="51" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="B51" s="16"/>
+      <c r="C51" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="17"/>
+      <c r="I51" s="18"/>
+      <c r="J51" s="18">
+        <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
+        <v>0</v>
       </c>
       <c r="K51" s="1"/>
+      <c r="L51" s="4"/>
+      <c r="M51" s="4"/>
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
     </row>
-    <row r="52" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="B52" s="16"/>
-      <c r="C52" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="D52" s="17"/>
-      <c r="E52" s="17"/>
-      <c r="F52" s="17"/>
-      <c r="G52" s="17"/>
-      <c r="H52" s="17"/>
-      <c r="I52" s="18"/>
-      <c r="J52" s="18">
-        <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>0</v>
+    <row r="52" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1">
+        <v>1</v>
+      </c>
+      <c r="I52" s="4">
+        <v>96.1</v>
+      </c>
+      <c r="J52" s="14">
+        <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
+        <v>96.1</v>
       </c>
       <c r="K52" s="1"/>
-      <c r="L52" s="4"/>
-      <c r="M52" s="4"/>
-      <c r="O52" s="1"/>
+      <c r="N52" s="4"/>
       <c r="P52" s="1"/>
     </row>
-    <row r="53" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>239</v>
+    <row r="53" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>242</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>200</v>
+        <v>154</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>78</v>
+        <v>24</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>95</v>
+        <v>39</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G53" s="1"/>
+        <v>40</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>153</v>
+      </c>
       <c r="H53" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I53" s="4">
-        <v>96.1</v>
+        <v>13.27</v>
       </c>
       <c r="J53" s="14">
         <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>96.1</v>
+        <v>26.54</v>
       </c>
       <c r="K53" s="1"/>
       <c r="N53" s="4"/>
       <c r="P53" s="1"/>
     </row>
-    <row r="54" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>157</v>
+        <v>202</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>40</v>
+        <v>115</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>41</v>
+        <v>201</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>156</v>
+        <v>203</v>
       </c>
       <c r="H54" s="1">
         <v>2</v>
       </c>
       <c r="I54" s="4">
-        <v>13.27</v>
+        <v>6.97</v>
       </c>
       <c r="J54" s="14">
         <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>26.54</v>
+        <v>13.94</v>
       </c>
       <c r="K54" s="1"/>
       <c r="N54" s="4"/>
       <c r="P54" s="1"/>
     </row>
-    <row r="55" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>205</v>
+        <v>134</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>116</v>
+        <v>6</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>204</v>
+        <v>9</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>206</v>
+        <v>8</v>
       </c>
       <c r="H55" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I55" s="4">
-        <v>6.97</v>
+        <v>44.45</v>
       </c>
       <c r="J55" s="14">
         <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>13.94</v>
+        <v>44.45</v>
       </c>
       <c r="K55" s="1"/>
       <c r="N55" s="4"/>
       <c r="P55" s="1"/>
     </row>
-    <row r="56" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>246</v>
+    <row r="56" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>243</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>135</v>
+        <v>10</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="E56" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="F56" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>8</v>
+        <v>165</v>
       </c>
       <c r="H56" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I56" s="4">
-        <v>44.45</v>
-      </c>
-      <c r="J56" s="14">
-        <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>44.45</v>
+        <v>8.09</v>
+      </c>
+      <c r="J56" s="2">
+        <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
+        <v>16.18</v>
       </c>
       <c r="K56" s="1"/>
-      <c r="N56" s="4"/>
+      <c r="L56" s="4"/>
+      <c r="M56" s="4"/>
+      <c r="O56" s="1"/>
       <c r="P56" s="1"/>
     </row>
-    <row r="57" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B57" s="13" t="s">
-        <v>246</v>
+    <row r="57" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>243</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>10</v>
+        <v>178</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="H57" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I57" s="4">
-        <v>8.09</v>
-      </c>
-      <c r="J57" s="2">
-        <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>16.18</v>
+        <v>5.04</v>
+      </c>
+      <c r="J57" s="14">
+        <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
+        <v>5.04</v>
       </c>
       <c r="K57" s="1"/>
-      <c r="L57" s="4"/>
-      <c r="M57" s="4"/>
-      <c r="O57" s="1"/>
+      <c r="N57" s="4"/>
       <c r="P57" s="1"/>
     </row>
-    <row r="58" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>65</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
       <c r="F58" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>180</v>
+        <v>110</v>
+      </c>
+      <c r="G58" s="1">
+        <v>3985</v>
       </c>
       <c r="H58" s="1">
         <v>1</v>
       </c>
-      <c r="I58" s="4">
-        <v>5.04</v>
+      <c r="I58" s="2">
+        <v>3.95</v>
       </c>
       <c r="J58" s="14">
         <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>5.04</v>
+        <v>3.95</v>
       </c>
       <c r="K58" s="1"/>
       <c r="N58" s="4"/>
       <c r="P58" s="1"/>
     </row>
-    <row r="59" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>244</v>
+        <v>217</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
+        <v>155</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F59" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G59" s="1">
-        <v>3985</v>
+        <v>4540</v>
       </c>
       <c r="H59" s="1">
-        <v>1</v>
-      </c>
-      <c r="I59" s="2">
+        <v>4</v>
+      </c>
+      <c r="I59" s="4">
         <v>3.95</v>
       </c>
       <c r="J59" s="14">
         <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>3.95</v>
+        <v>15.8</v>
       </c>
       <c r="K59" s="1"/>
       <c r="N59" s="4"/>
       <c r="P59" s="1"/>
     </row>
-    <row r="60" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>158</v>
+        <v>119</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G60" s="1">
-        <v>4540</v>
+        <v>207</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>208</v>
       </c>
       <c r="H60" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I60" s="4">
-        <v>3.95</v>
+        <v>22.51</v>
       </c>
       <c r="J60" s="14">
         <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>15.8</v>
+        <v>67.53</v>
       </c>
       <c r="K60" s="1"/>
       <c r="N60" s="4"/>
       <c r="P60" s="1"/>
     </row>
-    <row r="61" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>120</v>
+        <v>44</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>121</v>
+        <v>45</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>211</v>
+        <v>156</v>
+      </c>
+      <c r="G61" s="1">
+        <v>4685</v>
       </c>
       <c r="H61" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I61" s="4">
-        <v>22.51</v>
+        <v>24.95</v>
       </c>
       <c r="J61" s="14">
         <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>67.53</v>
+        <v>24.95</v>
       </c>
       <c r="K61" s="1"/>
       <c r="N61" s="4"/>
       <c r="P61" s="1"/>
     </row>
-    <row r="62" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>45</v>
+        <v>211</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>46</v>
+        <v>114</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="G62" s="1">
-        <v>4685</v>
+        <v>199</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>200</v>
       </c>
       <c r="H62" s="1">
-        <v>1</v>
-      </c>
-      <c r="I62" s="4">
-        <v>24.95</v>
-      </c>
-      <c r="J62" s="14">
-        <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>24.95</v>
+        <v>2</v>
+      </c>
+      <c r="I62" s="2">
+        <v>17.39</v>
+      </c>
+      <c r="J62" s="4">
+        <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
+        <v>34.78</v>
       </c>
       <c r="K62" s="1"/>
-      <c r="N62" s="4"/>
+      <c r="O62" s="1"/>
       <c r="P62" s="1"/>
     </row>
-    <row r="63" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>202</v>
+    <row r="63" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="B63" s="13"/>
+      <c r="C63" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="H63" s="1">
-        <v>2</v>
+        <v>168</v>
+      </c>
+      <c r="H63" s="3">
+        <v>7</v>
       </c>
       <c r="I63" s="2">
-        <v>17.39</v>
+        <v>2.75</v>
       </c>
       <c r="J63" s="4">
         <f>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</f>
-        <v>34.78</v>
+        <v>19.25</v>
       </c>
       <c r="K63" s="1"/>
       <c r="O63" s="1"/>
       <c r="P63" s="1"/>
     </row>
-    <row r="64" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H64" s="1">
         <v>1</v>
@@ -3573,12 +3591,12 @@
       <c r="N64" s="4"/>
       <c r="P64" s="1"/>
     </row>
-    <row r="65" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>13</v>
@@ -3604,27 +3622,27 @@
       <c r="N65" s="4"/>
       <c r="P65" s="1"/>
     </row>
-    <row r="66" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E66" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F66" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F66" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="G66" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H66" s="1">
         <v>1</v>
@@ -3640,27 +3658,27 @@
       <c r="N66" s="4"/>
       <c r="P66" s="1"/>
     </row>
-    <row r="67" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E67" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F67" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F67" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="G67" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="H67" s="1">
         <v>5</v>
@@ -3676,27 +3694,27 @@
       <c r="N67" s="4"/>
       <c r="P67" s="1"/>
     </row>
-    <row r="68" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E68" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F68" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F68" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="G68" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="H68" s="1">
         <v>7</v>
@@ -3712,27 +3730,27 @@
       <c r="N68" s="4"/>
       <c r="P68" s="1"/>
     </row>
-    <row r="69" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H69" s="3">
         <v>7</v>
@@ -3748,27 +3766,27 @@
       <c r="N69" s="4"/>
       <c r="P69" s="1"/>
     </row>
-    <row r="70" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H70" s="1">
         <v>4</v>
@@ -3784,27 +3802,27 @@
       <c r="N70" s="4"/>
       <c r="P70" s="1"/>
     </row>
-    <row r="71" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="H71" s="1">
         <v>4</v>
@@ -3820,27 +3838,27 @@
       <c r="N71" s="4"/>
       <c r="P71" s="1"/>
     </row>
-    <row r="72" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H72" s="1">
         <v>4</v>
@@ -3856,27 +3874,27 @@
       <c r="N72" s="4"/>
       <c r="P72" s="1"/>
     </row>
-    <row r="73" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H73" s="1">
         <v>4</v>
@@ -3892,27 +3910,27 @@
       <c r="N73" s="4"/>
       <c r="P73" s="1"/>
     </row>
-    <row r="74" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H74" s="1">
         <v>2</v>
@@ -3928,27 +3946,27 @@
       <c r="N74" s="4"/>
       <c r="P74" s="1"/>
     </row>
-    <row r="75" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H75" s="1">
         <v>2</v>
@@ -3964,12 +3982,12 @@
       <c r="N75" s="4"/>
       <c r="P75" s="1"/>
     </row>
-    <row r="76" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>15</v>
@@ -3995,13 +4013,13 @@
       <c r="N76" s="4"/>
       <c r="P76" s="1"/>
     </row>
-    <row r="77" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="9"/>
       <c r="B77" s="9"/>
       <c r="C77" s="10"/>
       <c r="D77" s="10"/>
       <c r="E77" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F77" s="10"/>
       <c r="G77" s="10"/>
@@ -4015,15 +4033,15 @@
       <c r="N77" s="4"/>
       <c r="P77" s="1"/>
     </row>
-    <row r="78" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
     </row>
-    <row r="79" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
     </row>
-    <row r="80" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
     </row>

</xml_diff>

<commit_message>
Added parts that we need to order to complete the machines.
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -5,24 +5,35 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajohnson\GIT_Projects\ValpoFilamentRecycler09\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamj\Git Projects\ValpoFilamentRecycler09\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB78D12-4DBD-4A6D-97A2-7EB647EBEB86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2BDD24E-0590-495F-8726-ED087699374F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Extruder" sheetId="1" r:id="rId1"/>
     <sheet name="Spooler" sheetId="2" r:id="rId2"/>
     <sheet name="NEED" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="275">
   <si>
     <t>Quantity</t>
   </si>
@@ -234,9 +245,6 @@
     <t>On Semiconductor</t>
   </si>
   <si>
-    <t>122095-84</t>
-  </si>
-  <si>
     <t>Dwyer</t>
   </si>
   <si>
@@ -762,18 +770,9 @@
     <t>Arduino UNO</t>
   </si>
   <si>
-    <t>Extruder</t>
-  </si>
-  <si>
     <t>EXTRA PARTS</t>
   </si>
   <si>
-    <t>Power Cord</t>
-  </si>
-  <si>
-    <t>General purpose type J thermocouple with #6 spade terminals</t>
-  </si>
-  <si>
     <t>SE-600-24</t>
   </si>
   <si>
@@ -822,7 +821,43 @@
     <t>DC/DC Converter, 24V input, 12V, 5A output</t>
   </si>
   <si>
-    <t>Double-check thermocouple type before ordering connectors!</t>
+    <t>General purpose type K thermocouple with #6 spade terminals</t>
+  </si>
+  <si>
+    <t>122095-01</t>
+  </si>
+  <si>
+    <t>IEC-C13 Power Connector</t>
+  </si>
+  <si>
+    <t>DC Power Wall Wort, 12V, 2A</t>
+  </si>
+  <si>
+    <t>Power Cord, C13</t>
+  </si>
+  <si>
+    <t>Barrel Jack Connector, Panel Mount</t>
+  </si>
+  <si>
+    <t>SparkFun Transceiver Breakout - RS-485</t>
+  </si>
+  <si>
+    <t>SparkFun</t>
+  </si>
+  <si>
+    <t>BOB-10124</t>
+  </si>
+  <si>
+    <t>Got it?</t>
+  </si>
+  <si>
+    <t>IEC-A-2</t>
+  </si>
+  <si>
+    <t>Adam Tech</t>
+  </si>
+  <si>
+    <t>2057-IEC-A-2-ND</t>
   </si>
 </sst>
 </file>
@@ -1210,6 +1245,9 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1228,6 +1266,9 @@
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -1473,6 +1514,9 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1491,6 +1535,9 @@
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -1715,18 +1762,6 @@
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1747,15 +1782,15 @@
     <sortCondition ref="C1:C35"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="12" xr3:uid="{C633C4DA-E9F1-49FB-8240-86247B964FE1}" name="Assembly" totalsRowDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{DAB1913A-18D2-4D9A-9708-032A60B6BC64}" name="Description" totalsRowDxfId="27" dataCellStyle="Normal"/>
-    <tableColumn id="7" xr3:uid="{EC3749CD-9468-4676-8AAA-2DE4FA028800}" name="Supplier" totalsRowDxfId="26" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{FBFB3CD0-7BF1-4266-8755-35F85270404A}" name="Supplier Part Number" totalsRowLabel="Total" totalsRowDxfId="25" dataCellStyle="Normal"/>
-    <tableColumn id="8" xr3:uid="{70763CA8-03EB-4064-9534-D2C0729DD10E}" name="Manufactuer" totalsRowDxfId="24" dataCellStyle="Normal"/>
-    <tableColumn id="9" xr3:uid="{9D792AB2-8329-471D-9251-7B5C39551B6D}" name="Manufacturer Part Number" totalsRowDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{6C81D9F0-6082-4928-8091-DA45D848F33F}" name="Quantity" totalsRowDxfId="22" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{D2BF7368-0F05-4426-9AF7-A4A54F97F689}" name="Unit Price" dataDxfId="30" totalsRowDxfId="21" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{816B8560-23EB-4218-8B09-04C10060E74B}" name="Total Price" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="20" dataCellStyle="Currency">
+    <tableColumn id="12" xr3:uid="{C633C4DA-E9F1-49FB-8240-86247B964FE1}" name="Assembly" totalsRowDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{DAB1913A-18D2-4D9A-9708-032A60B6BC64}" name="Description" totalsRowDxfId="31" dataCellStyle="Normal"/>
+    <tableColumn id="7" xr3:uid="{EC3749CD-9468-4676-8AAA-2DE4FA028800}" name="Supplier" totalsRowDxfId="30" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{FBFB3CD0-7BF1-4266-8755-35F85270404A}" name="Supplier Part Number" totalsRowLabel="Total" totalsRowDxfId="29" dataCellStyle="Normal"/>
+    <tableColumn id="8" xr3:uid="{70763CA8-03EB-4064-9534-D2C0729DD10E}" name="Manufactuer" totalsRowDxfId="28" dataCellStyle="Normal"/>
+    <tableColumn id="9" xr3:uid="{9D792AB2-8329-471D-9251-7B5C39551B6D}" name="Manufacturer Part Number" totalsRowDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{6C81D9F0-6082-4928-8091-DA45D848F33F}" name="Quantity" totalsRowDxfId="26" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{D2BF7368-0F05-4426-9AF7-A4A54F97F689}" name="Unit Price" dataDxfId="25" totalsRowDxfId="24" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{816B8560-23EB-4218-8B09-04C10060E74B}" name="Total Price" totalsRowFunction="sum" dataDxfId="23" totalsRowDxfId="22" dataCellStyle="Currency">
       <calculatedColumnFormula>TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1767,15 +1802,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9548DB7C-B8C9-46D9-9175-857AA71A03C3}" name="TableSpooler" displayName="TableSpooler" ref="A1:I24" totalsRowCount="1" dataCellStyle="Normal">
   <autoFilter ref="A1:I23" xr:uid="{9548DB7C-B8C9-46D9-9175-857AA71A03C3}"/>
   <tableColumns count="9">
-    <tableColumn id="12" xr3:uid="{02FE56AC-0EFC-42AA-8A79-A19D1265C334}" name="Assembly" totalsRowDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{6C7F5790-A2D7-49D5-98CC-5347EEBCB1ED}" name="Description" totalsRowDxfId="18" dataCellStyle="Normal"/>
-    <tableColumn id="7" xr3:uid="{FF40B9DA-8160-42B4-A04B-59C3988A3C5E}" name="Supplier" totalsRowDxfId="17" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{66B504B5-4CA8-4C40-909D-18E9AADA1F9D}" name="Supplier Part Number" totalsRowLabel="Total" totalsRowDxfId="16" dataCellStyle="Normal"/>
-    <tableColumn id="8" xr3:uid="{B1FBFAC4-450D-465B-8926-44EA92A1276B}" name="Manufactuer" totalsRowDxfId="15" dataCellStyle="Normal"/>
-    <tableColumn id="9" xr3:uid="{42F90968-E8D4-4DE3-8E2B-F702BB9EC99B}" name="Manufacturer Part Number" totalsRowDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{E176CC47-E8BA-4A8D-9C82-D7F685B8FC85}" name="Quantity" totalsRowDxfId="13" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{CECFF550-A5B4-494E-8824-FFDC20FE1F96}" name="Unit Price" dataDxfId="32" totalsRowDxfId="12" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{5C811821-7EC0-4CCE-ABD1-E409C90F00A8}" name="Total Price" totalsRowFunction="sum" dataDxfId="31" totalsRowDxfId="11" dataCellStyle="Currency">
+    <tableColumn id="12" xr3:uid="{02FE56AC-0EFC-42AA-8A79-A19D1265C334}" name="Assembly" totalsRowDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{6C7F5790-A2D7-49D5-98CC-5347EEBCB1ED}" name="Description" totalsRowDxfId="20" dataCellStyle="Normal"/>
+    <tableColumn id="7" xr3:uid="{FF40B9DA-8160-42B4-A04B-59C3988A3C5E}" name="Supplier" totalsRowDxfId="19" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{66B504B5-4CA8-4C40-909D-18E9AADA1F9D}" name="Supplier Part Number" totalsRowLabel="Total" totalsRowDxfId="18" dataCellStyle="Normal"/>
+    <tableColumn id="8" xr3:uid="{B1FBFAC4-450D-465B-8926-44EA92A1276B}" name="Manufactuer" totalsRowDxfId="17" dataCellStyle="Normal"/>
+    <tableColumn id="9" xr3:uid="{42F90968-E8D4-4DE3-8E2B-F702BB9EC99B}" name="Manufacturer Part Number" totalsRowDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{E176CC47-E8BA-4A8D-9C82-D7F685B8FC85}" name="Quantity" totalsRowDxfId="15" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{CECFF550-A5B4-494E-8824-FFDC20FE1F96}" name="Unit Price" dataDxfId="14" totalsRowDxfId="13" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{5C811821-7EC0-4CCE-ABD1-E409C90F00A8}" name="Total Price" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="11" dataCellStyle="Currency">
       <calculatedColumnFormula>TableSpooler[[#This Row],[Quantity]]*TableSpooler[[#This Row],[Unit Price]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1784,13 +1819,13 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DB8F8FC9-89F7-4F5F-A0A1-985E1699572D}" name="TableNeed" displayName="TableNeed" ref="A1:I12" totalsRowCount="1" dataCellStyle="Normal">
-  <autoFilter ref="A1:I11" xr:uid="{DB8F8FC9-89F7-4F5F-A0A1-985E1699572D}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I8">
-    <sortCondition ref="C1:C8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DB8F8FC9-89F7-4F5F-A0A1-985E1699572D}" name="TableNeed" displayName="TableNeed" ref="A1:I14" totalsRowCount="1" dataCellStyle="Normal">
+  <autoFilter ref="A1:I13" xr:uid="{DB8F8FC9-89F7-4F5F-A0A1-985E1699572D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I9">
+    <sortCondition ref="C1:C9"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="12" xr3:uid="{2B5E4D02-1DE1-4D79-9E55-192E36B3EA77}" name="Assembly" totalsRowDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{2B5E4D02-1DE1-4D79-9E55-192E36B3EA77}" name="Got it?" totalsRowDxfId="8"/>
     <tableColumn id="2" xr3:uid="{E6F3A558-4A17-4A36-B2DB-42B6CC1D4C39}" name="Description" totalsRowDxfId="7" dataCellStyle="Normal"/>
     <tableColumn id="7" xr3:uid="{B387B6B1-B163-41DB-A8A1-86EF869C85DF}" name="Supplier" totalsRowDxfId="6" dataCellStyle="Normal"/>
     <tableColumn id="3" xr3:uid="{C6D04B3B-2A8B-436B-89D6-8B449FADB069}" name="Supplier Part Number" totalsRowLabel="Total" totalsRowDxfId="5" dataCellStyle="Normal"/>
@@ -1799,7 +1834,7 @@
     <tableColumn id="4" xr3:uid="{5967AF1C-97BD-47B7-A930-6C2111F8E15C}" name="Quantity" totalsRowDxfId="2" dataCellStyle="Normal"/>
     <tableColumn id="5" xr3:uid="{17C58ECF-F320-4E4E-B49F-27F8753AC79E}" name="Unit Price" dataDxfId="10" totalsRowDxfId="1" dataCellStyle="Currency"/>
     <tableColumn id="6" xr3:uid="{F9DFD496-D9A7-4553-8507-8E6AA33D3D67}" name="Total Price" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="0" dataCellStyle="Currency">
-      <calculatedColumnFormula>TableNeed[[#This Row],[Quantity]]*TableNeed[[#This Row],[Unit Price]]</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(TableNeed[[#This Row],[Got it?]]=FALSE, TableNeed[[#This Row],[Unit Price]]*TableNeed[[#This Row],[Quantity]], "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2010,46 +2045,46 @@
   <dimension ref="A1:P48"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="90" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="27.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>0</v>
@@ -2058,28 +2093,28 @@
         <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
     </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G2" s="3">
         <v>1</v>
@@ -2096,21 +2131,21 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G3" s="3">
         <v>1</v>
@@ -2127,12 +2162,12 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -2156,21 +2191,21 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -2187,21 +2222,21 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="G6" s="3">
         <v>1</v>
@@ -2218,18 +2253,18 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G7" s="1">
         <v>1</v>
@@ -2246,18 +2281,18 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G8" s="1">
         <v>1</v>
@@ -2274,18 +2309,18 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E9" s="3"/>
       <c r="G9" s="3">
@@ -2303,18 +2338,18 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="E10" s="3"/>
       <c r="G10" s="3">
@@ -2332,18 +2367,18 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="E11" s="3"/>
       <c r="G11" s="3">
@@ -2361,18 +2396,18 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E12" s="3"/>
       <c r="G12" s="3">
@@ -2390,18 +2425,18 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>92</v>
       </c>
       <c r="E13" s="3"/>
       <c r="G13" s="3">
@@ -2419,18 +2454,18 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E14" s="3"/>
       <c r="G14" s="3">
@@ -2448,21 +2483,21 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="G15" s="3">
         <v>1</v>
@@ -2479,18 +2514,18 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>90</v>
       </c>
       <c r="E16" s="3"/>
       <c r="G16" s="3">
@@ -2508,20 +2543,20 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G17" s="3">
         <v>1</v>
@@ -2536,21 +2571,21 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="F18" s="1">
         <v>108050</v>
@@ -2570,24 +2605,24 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="D19" s="1">
         <v>37769</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G19" s="1">
         <v>2</v>
@@ -2604,18 +2639,18 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="G20" s="1">
         <v>1</v>
@@ -2632,24 +2667,24 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D21" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="F21" s="3" t="s">
-        <v>70</v>
+        <v>263</v>
       </c>
       <c r="G21" s="3">
         <v>2</v>
@@ -2666,9 +2701,9 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>17</v>
@@ -2678,7 +2713,7 @@
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G22" s="3">
         <v>1</v>
@@ -2695,18 +2730,18 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E23" s="3"/>
       <c r="G23" s="3">
@@ -2724,24 +2759,24 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="G24" s="3">
         <v>1</v>
@@ -2758,12 +2793,12 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>23</v>
@@ -2775,7 +2810,7 @@
         <v>27</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G25" s="3">
         <v>1</v>
@@ -2792,24 +2827,24 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G26" s="1">
         <v>2</v>
@@ -2826,9 +2861,9 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>4</v>
@@ -2857,12 +2892,12 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
     </row>
-    <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>31</v>
@@ -2871,10 +2906,10 @@
         <v>30</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G28" s="1">
         <v>2</v>
@@ -2891,12 +2926,12 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
     </row>
-    <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>31</v>
@@ -2905,7 +2940,7 @@
         <v>32</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F29" s="7">
         <v>181</v>
@@ -2925,12 +2960,12 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
     </row>
-    <row r="30" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>31</v>
@@ -2939,7 +2974,7 @@
         <v>33</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F30" s="1">
         <v>292</v>
@@ -2959,12 +2994,12 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>23</v>
@@ -2976,7 +3011,7 @@
         <v>41</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G31" s="1">
         <v>5</v>
@@ -2993,10 +3028,10 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
     </row>
-    <row r="32" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>31</v>
@@ -3008,7 +3043,7 @@
         <v>35</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G32" s="1">
         <v>4</v>
@@ -3025,10 +3060,10 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
     </row>
-    <row r="33" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>31</v>
@@ -3040,7 +3075,7 @@
         <v>37</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G33" s="1">
         <v>1</v>
@@ -3057,10 +3092,10 @@
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
     </row>
-    <row r="34" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>23</v>
@@ -3072,7 +3107,7 @@
         <v>46</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G34" s="1">
         <v>4</v>
@@ -3089,10 +3124,10 @@
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
     </row>
-    <row r="35" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>31</v>
@@ -3104,7 +3139,7 @@
         <v>69</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G35" s="1">
         <v>2</v>
@@ -3121,12 +3156,12 @@
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
     </row>
-    <row r="36" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
@@ -3143,23 +3178,23 @@
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
     </row>
-    <row r="37" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
     </row>
-    <row r="38" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>23</v>
@@ -3171,7 +3206,7 @@
         <v>29</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G39" s="1">
         <v>1</v>
@@ -3180,22 +3215,22 @@
         <v>38.5</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G40" s="1">
         <v>1</v>
@@ -3204,10 +3239,10 @@
         <v>4.13</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>31</v>
@@ -3219,7 +3254,7 @@
         <v>51</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G41" s="1">
         <v>2</v>
@@ -3228,10 +3263,10 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>31</v>
@@ -3243,7 +3278,7 @@
         <v>65</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G42" s="1">
         <v>1</v>
@@ -3252,16 +3287,16 @@
         <v>2.56</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="G43" s="1">
         <v>1</v>
@@ -3270,16 +3305,16 @@
         <v>43.8</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G44" s="1">
         <v>1</v>
@@ -3288,10 +3323,10 @@
         <v>43.82</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>23</v>
@@ -3303,7 +3338,7 @@
         <v>24</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G45" s="1">
         <v>1</v>
@@ -3312,22 +3347,22 @@
         <v>19.54</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>211</v>
       </c>
       <c r="G46" s="1">
         <v>1</v>
@@ -3336,10 +3371,10 @@
         <v>368</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>20</v>
@@ -3360,15 +3395,15 @@
         <v>410</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="G48">
         <v>1</v>
@@ -3389,43 +3424,43 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC497086-9290-4C1D-9300-28557D6CEBE4}">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="96.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="96.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>0</v>
@@ -3434,24 +3469,24 @@
         <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1">
@@ -3465,12 +3500,12 @@
         <v>96.1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>23</v>
@@ -3482,7 +3517,7 @@
         <v>39</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G3" s="17">
         <v>2</v>
@@ -3495,24 +3530,24 @@
         <v>26.54</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G4" s="17">
         <v>2</v>
@@ -3525,12 +3560,12 @@
         <v>13.94</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
@@ -3553,9 +3588,9 @@
         <v>44.45</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>10</v>
@@ -3570,7 +3605,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G6" s="1">
         <v>2</v>
@@ -3583,12 +3618,12 @@
         <v>16.18</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>31</v>
@@ -3600,7 +3635,7 @@
         <v>51</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G7" s="1">
         <v>1</v>
@@ -3613,17 +3648,17 @@
         <v>5.04</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F8" s="1">
         <v>3985</v>
@@ -3639,12 +3674,12 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>23</v>
@@ -3653,7 +3688,7 @@
         <v>42</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F9" s="1">
         <v>4540</v>
@@ -3669,20 +3704,20 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="F10" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="G10" s="3">
         <v>1</v>
@@ -3690,12 +3725,12 @@
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>31</v>
@@ -3707,7 +3742,7 @@
         <v>53</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G11" s="3">
         <v>7</v>
@@ -3715,17 +3750,17 @@
       <c r="H11" s="2">
         <v>2.75</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="2">
         <f>TableSpooler[[#This Row],[Quantity]]*TableSpooler[[#This Row],[Unit Price]]</f>
         <v>19.25</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>23</v>
@@ -3737,7 +3772,7 @@
         <v>29</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G12" s="1">
         <v>1</v>
@@ -3750,12 +3785,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>31</v>
@@ -3767,7 +3802,7 @@
         <v>49</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G13" s="1">
         <v>1</v>
@@ -3780,12 +3815,12 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>31</v>
@@ -3797,7 +3832,7 @@
         <v>67</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G14" s="1">
         <v>5</v>
@@ -3810,12 +3845,12 @@
         <v>2.5499999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>31</v>
@@ -3827,7 +3862,7 @@
         <v>55</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G15" s="1">
         <v>7</v>
@@ -3840,12 +3875,12 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>31</v>
@@ -3857,7 +3892,7 @@
         <v>55</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G16" s="3">
         <v>7</v>
@@ -3870,12 +3905,12 @@
         <v>0.70000000000000007</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>31</v>
@@ -3887,7 +3922,7 @@
         <v>55</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G17" s="1">
         <v>4</v>
@@ -3900,12 +3935,12 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>31</v>
@@ -3917,7 +3952,7 @@
         <v>55</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G18" s="1">
         <v>4</v>
@@ -3930,12 +3965,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>31</v>
@@ -3947,7 +3982,7 @@
         <v>55</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G19" s="1">
         <v>4</v>
@@ -3960,12 +3995,12 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>31</v>
@@ -3977,7 +4012,7 @@
         <v>55</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G20" s="1">
         <v>4</v>
@@ -3990,12 +4025,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>31</v>
@@ -4007,7 +4042,7 @@
         <v>55</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G21" s="1">
         <v>2</v>
@@ -4020,12 +4055,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>31</v>
@@ -4037,7 +4072,7 @@
         <v>55</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G22" s="1">
         <v>2</v>
@@ -4050,9 +4085,9 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>15</v>
@@ -4076,12 +4111,12 @@
         <v>14.99</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
@@ -4092,27 +4127,27 @@
         <v>286.19999999999993</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>206</v>
       </c>
       <c r="G27" s="1">
         <v>3</v>
@@ -4123,22 +4158,22 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>198</v>
       </c>
       <c r="G28" s="1">
         <v>2</v>
@@ -4149,9 +4184,9 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>43</v>
@@ -4163,7 +4198,7 @@
         <v>44</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F29" s="1">
         <v>4685</v>
@@ -4177,9 +4212,9 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>13</v>
@@ -4187,19 +4222,38 @@
       <c r="C30" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="1"/>
       <c r="G30" s="1">
         <v>1</v>
       </c>
       <c r="H30" s="1">
         <v>9.99</v>
       </c>
-      <c r="I30" s="1"/>
-    </row>
+    </row>
+    <row r="31" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1</v>
+      </c>
+      <c r="H31" s="1">
+        <v>32.1</v>
+      </c>
+      <c r="I31" s="1" t="e">
+        <f>TableNeed[[#This Row],[Quantity]]*TableNeed[[#This Row],[Unit Price]]</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -4210,43 +4264,43 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8CF5BD-F5CF-420A-AD2A-E11B010BEA1F}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="73.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>213</v>
+        <v>271</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>0</v>
@@ -4255,13 +4309,15 @@
         <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="8"/>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="b">
+        <v>1</v>
+      </c>
       <c r="B2" s="3" t="s">
-        <v>248</v>
+        <v>265</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -4271,162 +4327,216 @@
         <v>1</v>
       </c>
       <c r="H2" s="2"/>
-      <c r="I2" s="2">
-        <f>TableNeed[[#This Row],[Quantity]]*TableNeed[[#This Row],[Unit Price]]</f>
+      <c r="I2" s="2" t="str">
+        <f>IF(TableNeed[[#This Row],[Got it?]]=FALSE, TableNeed[[#This Row],[Unit Price]]*TableNeed[[#This Row],[Quantity]], "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2">
+        <f>IF(TableNeed[[#This Row],[Got it?]]=FALSE, TableNeed[[#This Row],[Unit Price]]*TableNeed[[#This Row],[Quantity]], "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2">
+        <f>IF(TableNeed[[#This Row],[Got it?]]=FALSE, TableNeed[[#This Row],[Unit Price]]*TableNeed[[#This Row],[Quantity]], "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1.03</v>
+      </c>
+      <c r="I5" s="2">
+        <f>IF(TableNeed[[#This Row],[Got it?]]=FALSE, TableNeed[[#This Row],[Unit Price]]*TableNeed[[#This Row],[Quantity]], "")</f>
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E6" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="G6" s="1">
+        <v>2</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="I6" s="4">
+        <f>IF(TableNeed[[#This Row],[Got it?]]=FALSE, TableNeed[[#This Row],[Unit Price]]*TableNeed[[#This Row],[Quantity]], "")</f>
+        <v>4.8600000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="C7" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="G3" s="1">
+      <c r="G7" s="1">
         <v>2</v>
       </c>
-      <c r="I3" s="4">
-        <f>TableNeed[[#This Row],[Quantity]]*TableNeed[[#This Row],[Unit Price]]</f>
+      <c r="H7" s="1">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="I7" s="4">
+        <f>IF(TableNeed[[#This Row],[Got it?]]=FALSE, TableNeed[[#This Row],[Unit Price]]*TableNeed[[#This Row],[Quantity]], "")</f>
+        <v>5.0199999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="G4" s="1">
-        <v>2</v>
-      </c>
-      <c r="I4" s="4">
-        <f>TableNeed[[#This Row],[Quantity]]*TableNeed[[#This Row],[Unit Price]]</f>
+      <c r="B8" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="G8" s="1">
+        <v>3</v>
+      </c>
+      <c r="I8" s="4">
+        <f>IF(TableNeed[[#This Row],[Got it?]]=FALSE, TableNeed[[#This Row],[Unit Price]]*TableNeed[[#This Row],[Quantity]], "")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
+    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>222</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="G5" s="1">
-        <v>3</v>
-      </c>
-      <c r="I5" s="4">
-        <f>TableNeed[[#This Row],[Quantity]]*TableNeed[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="G6" s="3">
-        <v>3</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2">
-        <f>TableNeed[[#This Row],[Quantity]]*TableNeed[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="G7" s="1">
-        <v>3</v>
-      </c>
-      <c r="I7" s="4">
-        <f>TableNeed[[#This Row],[Quantity]]*TableNeed[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G8" s="1">
-        <v>1</v>
-      </c>
-      <c r="H8" s="2">
-        <v>32.1</v>
-      </c>
-      <c r="I8" s="4">
-        <f>TableNeed[[#This Row],[Quantity]]*TableNeed[[#This Row],[Unit Price]]</f>
-        <v>32.1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="3" t="s">
-        <v>241</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14">
-        <f>TableNeed[[#This Row],[Quantity]]*TableNeed[[#This Row],[Unit Price]]</f>
+      <c r="E9" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="G9" s="3">
+        <v>3</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2">
+        <f>IF(TableNeed[[#This Row],[Got it?]]=FALSE, TableNeed[[#This Row],[Unit Price]]*TableNeed[[#This Row],[Quantity]], "")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14">
-        <f>TableNeed[[#This Row],[Quantity]]*TableNeed[[#This Row],[Unit Price]]</f>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
+        <v>10.95</v>
+      </c>
+      <c r="I10" s="2" t="str">
+        <f>IF(TableNeed[[#This Row],[Got it?]]=FALSE, TableNeed[[#This Row],[Unit Price]]*TableNeed[[#This Row],[Quantity]], "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>246</v>
-      </c>
       <c r="B11" s="3" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -4434,100 +4544,132 @@
       <c r="G11" s="3"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14">
-        <f>TableNeed[[#This Row],[Quantity]]*TableNeed[[#This Row],[Unit Price]]</f>
+        <f>IF(TableNeed[[#This Row],[Got it?]]=FALSE, TableNeed[[#This Row],[Unit Price]]*TableNeed[[#This Row],[Quantity]], "")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="12">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14">
+        <f>IF(TableNeed[[#This Row],[Got it?]]=FALSE, TableNeed[[#This Row],[Unit Price]]*TableNeed[[#This Row],[Quantity]], "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="b">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="G13" s="3">
+        <v>2</v>
+      </c>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14" t="str">
+        <f>IF(TableNeed[[#This Row],[Got it?]]=FALSE, TableNeed[[#This Row],[Unit Price]]*TableNeed[[#This Row],[Quantity]], "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="12">
         <f>SUBTOTAL(109,TableNeed[Total Price])</f>
-        <v>32.1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="C15" s="1" t="s">
+        <v>10.91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="D17" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="G15" s="1">
-        <v>1</v>
-      </c>
-      <c r="H15" s="1">
+      <c r="F17" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1">
         <v>13.88</v>
       </c>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1">
-        <v>1</v>
-      </c>
-      <c r="H16" s="1">
-        <v>13.77</v>
-      </c>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>266</v>
-      </c>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1">
+        <v>13.77</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made a note of connector type needed.
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajohnson\GIT_Projects\ValpoFilamentRecycler09\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamj\Git Projects\ValpoFilamentRecycler09\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CBE11A-6828-44B7-B8BD-19E543A4F293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E63EE2-A00B-4E68-90CD-7F08D7BD2D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-165" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Extruder" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,23 @@
     <sheet name="Controller" sheetId="5" r:id="rId3"/>
     <sheet name="NEED" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="284">
   <si>
     <t>Quantity</t>
   </si>
@@ -872,6 +883,9 @@
   </si>
   <si>
     <t>Toggle Switch On-Off-(ON)</t>
+  </si>
+  <si>
+    <t>Need circular crimp connectors that can handle 16 and 18 gauge wire.</t>
   </si>
 </sst>
 </file>
@@ -993,6 +1007,9 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1011,6 +1028,9 @@
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -1234,12 +1254,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -1930,21 +1944,21 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DB8F8FC9-89F7-4F5F-A0A1-985E1699572D}" name="TableNeed" displayName="TableNeed" ref="A1:I19" totalsRowCount="1" dataCellStyle="Normal">
-  <autoFilter ref="A1:I18" xr:uid="{DB8F8FC9-89F7-4F5F-A0A1-985E1699572D}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I13">
-    <sortCondition ref="C1:C13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DB8F8FC9-89F7-4F5F-A0A1-985E1699572D}" name="TableNeed" displayName="TableNeed" ref="A1:I21" totalsRowCount="1" dataCellStyle="Normal">
+  <autoFilter ref="A1:I20" xr:uid="{DB8F8FC9-89F7-4F5F-A0A1-985E1699572D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I15">
+    <sortCondition ref="C1:C15"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="12" xr3:uid="{2B5E4D02-1DE1-4D79-9E55-192E36B3EA77}" name="Got it?" totalsRowDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{E6F3A558-4A17-4A36-B2DB-42B6CC1D4C39}" name="Description" totalsRowDxfId="7" dataCellStyle="Normal"/>
-    <tableColumn id="7" xr3:uid="{B387B6B1-B163-41DB-A8A1-86EF869C85DF}" name="Supplier" totalsRowDxfId="6" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{C6D04B3B-2A8B-436B-89D6-8B449FADB069}" name="Supplier Part Number" totalsRowLabel="Total" totalsRowDxfId="5" dataCellStyle="Normal"/>
-    <tableColumn id="8" xr3:uid="{FE34EFDD-6631-41FE-B1FB-5DA4EA7CE799}" name="Manufactuer" totalsRowDxfId="4" dataCellStyle="Normal"/>
-    <tableColumn id="9" xr3:uid="{BC7120C6-C05C-42E5-9B07-28CBA3BB206C}" name="Manufacturer Part Number" totalsRowDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{5967AF1C-97BD-47B7-A930-6C2111F8E15C}" name="Quantity" totalsRowDxfId="2" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{17C58ECF-F320-4E4E-B49F-27F8753AC79E}" name="Unit Price" dataDxfId="10" totalsRowDxfId="1" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{F9DFD496-D9A7-4553-8507-8E6AA33D3D67}" name="Total Price" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="0" dataCellStyle="Currency">
+    <tableColumn id="12" xr3:uid="{2B5E4D02-1DE1-4D79-9E55-192E36B3EA77}" name="Got it?" totalsRowDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{E6F3A558-4A17-4A36-B2DB-42B6CC1D4C39}" name="Description" totalsRowDxfId="9" dataCellStyle="Normal"/>
+    <tableColumn id="7" xr3:uid="{B387B6B1-B163-41DB-A8A1-86EF869C85DF}" name="Supplier" totalsRowDxfId="8" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{C6D04B3B-2A8B-436B-89D6-8B449FADB069}" name="Supplier Part Number" totalsRowLabel="Total" totalsRowDxfId="7" dataCellStyle="Normal"/>
+    <tableColumn id="8" xr3:uid="{FE34EFDD-6631-41FE-B1FB-5DA4EA7CE799}" name="Manufactuer" totalsRowDxfId="6" dataCellStyle="Normal"/>
+    <tableColumn id="9" xr3:uid="{BC7120C6-C05C-42E5-9B07-28CBA3BB206C}" name="Manufacturer Part Number" totalsRowDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{5967AF1C-97BD-47B7-A930-6C2111F8E15C}" name="Quantity" totalsRowDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{17C58ECF-F320-4E4E-B49F-27F8753AC79E}" name="Unit Price" dataDxfId="3" totalsRowDxfId="2" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{F9DFD496-D9A7-4553-8507-8E6AA33D3D67}" name="Total Price" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(TableNeed[[#This Row],[Got it?]]=FALSE, TableNeed[[#This Row],[Unit Price]]*TableNeed[[#This Row],[Quantity]], "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2155,30 +2169,30 @@
   </sheetPr>
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="90" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="27.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>212</v>
       </c>
@@ -2211,7 +2225,7 @@
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
     </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>227</v>
       </c>
@@ -2242,7 +2256,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>226</v>
       </c>
@@ -2273,7 +2287,7 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>226</v>
       </c>
@@ -2302,7 +2316,7 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>217</v>
       </c>
@@ -2333,7 +2347,7 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>217</v>
       </c>
@@ -2364,7 +2378,7 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>217</v>
       </c>
@@ -2392,7 +2406,7 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>217</v>
       </c>
@@ -2420,7 +2434,7 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>215</v>
       </c>
@@ -2449,7 +2463,7 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>215</v>
       </c>
@@ -2478,7 +2492,7 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>215</v>
       </c>
@@ -2507,7 +2521,7 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>215</v>
       </c>
@@ -2536,7 +2550,7 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>215</v>
       </c>
@@ -2565,7 +2579,7 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>215</v>
       </c>
@@ -2594,7 +2608,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>216</v>
       </c>
@@ -2625,7 +2639,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>216</v>
       </c>
@@ -2654,7 +2668,7 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>216</v>
       </c>
@@ -2676,7 +2690,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>218</v>
       </c>
@@ -2704,7 +2718,7 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>242</v>
       </c>
@@ -2738,7 +2752,7 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>242</v>
       </c>
@@ -2772,7 +2786,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>242</v>
       </c>
@@ -2800,7 +2814,7 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>242</v>
       </c>
@@ -2834,7 +2848,7 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>242</v>
       </c>
@@ -2863,7 +2877,7 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>242</v>
       </c>
@@ -2892,7 +2906,7 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>242</v>
       </c>
@@ -2926,7 +2940,7 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>242</v>
       </c>
@@ -2960,7 +2974,7 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>242</v>
       </c>
@@ -2991,7 +3005,7 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
     </row>
-    <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>242</v>
       </c>
@@ -3025,7 +3039,7 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
     </row>
-    <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="1" t="s">
         <v>156</v>
@@ -3057,7 +3071,7 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
     </row>
-    <row r="30" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="1" t="s">
         <v>173</v>
@@ -3089,7 +3103,7 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
@@ -3111,11 +3125,11 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
     </row>
-    <row r="32" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
     </row>
-    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
         <v>249</v>
@@ -3124,7 +3138,7 @@
       <c r="D33" s="1"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
         <v>126</v>
@@ -3148,7 +3162,7 @@
         <v>38.5</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
         <v>203</v>
@@ -3172,7 +3186,7 @@
         <v>4.13</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
         <v>164</v>
@@ -3196,7 +3210,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
         <v>171</v>
@@ -3220,7 +3234,7 @@
         <v>2.56</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
         <v>85</v>
@@ -3238,7 +3252,7 @@
         <v>43.8</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
         <v>115</v>
@@ -3256,7 +3270,7 @@
         <v>43.82</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
         <v>125</v>
@@ -3280,7 +3294,7 @@
         <v>19.54</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
         <v>211</v>
@@ -3304,7 +3318,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
         <v>257</v>
@@ -3328,7 +3342,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>260</v>
       </c>
@@ -3342,7 +3356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
         <v>128</v>
@@ -3387,20 +3401,20 @@
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="96.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="96.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>212</v>
       </c>
@@ -3429,7 +3443,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>227</v>
       </c>
@@ -3457,7 +3471,7 @@
         <v>96.1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>229</v>
       </c>
@@ -3487,7 +3501,7 @@
         <v>26.54</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>229</v>
       </c>
@@ -3517,7 +3531,7 @@
         <v>13.94</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>230</v>
       </c>
@@ -3545,7 +3559,7 @@
         <v>44.45</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>230</v>
       </c>
@@ -3575,7 +3589,7 @@
         <v>16.18</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>230</v>
       </c>
@@ -3605,7 +3619,7 @@
         <v>5.04</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>228</v>
       </c>
@@ -3631,7 +3645,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>213</v>
       </c>
@@ -3661,7 +3675,7 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>213</v>
       </c>
@@ -3682,7 +3696,7 @@
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>242</v>
       </c>
@@ -3712,7 +3726,7 @@
         <v>19.25</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>242</v>
       </c>
@@ -3742,7 +3756,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>242</v>
       </c>
@@ -3772,7 +3786,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>242</v>
       </c>
@@ -3802,7 +3816,7 @@
         <v>2.5499999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>242</v>
       </c>
@@ -3832,7 +3846,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>242</v>
       </c>
@@ -3862,7 +3876,7 @@
         <v>0.70000000000000007</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>242</v>
       </c>
@@ -3892,7 +3906,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>242</v>
       </c>
@@ -3922,7 +3936,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>242</v>
       </c>
@@ -3952,7 +3966,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>242</v>
       </c>
@@ -3982,7 +3996,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>242</v>
       </c>
@@ -4012,7 +4026,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>242</v>
       </c>
@@ -4042,7 +4056,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>242</v>
       </c>
@@ -4068,7 +4082,7 @@
         <v>14.99</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
@@ -4084,12 +4098,12 @@
         <v>286.19999999999993</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
         <v>117</v>
@@ -4115,7 +4129,7 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
         <v>208</v>
@@ -4141,7 +4155,7 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
         <v>43</v>
@@ -4167,7 +4181,7 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>13</v>
       </c>
@@ -4184,7 +4198,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>110</v>
       </c>
@@ -4205,7 +4219,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -4222,20 +4236,20 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>212</v>
       </c>
@@ -4264,7 +4278,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" s="1" t="s">
         <v>272</v>
@@ -4282,7 +4296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="1" t="s">
         <v>271</v>
@@ -4300,7 +4314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="1" t="s">
         <v>137</v>
@@ -4328,7 +4342,7 @@
         <v>19.899999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="1" t="s">
         <v>168</v>
@@ -4356,7 +4370,7 @@
         <v>19.899999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="1" t="s">
         <v>127</v>
@@ -4384,7 +4398,7 @@
         <v>5.6499999999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="1" t="s">
         <v>147</v>
@@ -4412,7 +4426,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="1" t="s">
         <v>149</v>
@@ -4440,7 +4454,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" t="s">
         <v>273</v>
@@ -4462,7 +4476,7 @@
         <v>2.95</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>107</v>
       </c>
@@ -4487,26 +4501,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8CF5BD-F5CF-420A-AD2A-E11B010BEA1F}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="73.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>269</v>
       </c>
@@ -4535,7 +4549,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="b">
         <v>1</v>
       </c>
@@ -4555,7 +4569,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="b">
         <v>0</v>
       </c>
@@ -4579,7 +4593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="b">
         <v>0</v>
       </c>
@@ -4603,7 +4617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="b">
         <v>0</v>
       </c>
@@ -4621,7 +4635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="b">
         <v>0</v>
       </c>
@@ -4645,7 +4659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="b">
         <v>0</v>
       </c>
@@ -4669,7 +4683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="b">
         <v>0</v>
       </c>
@@ -4693,7 +4707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="b">
         <v>0</v>
       </c>
@@ -4711,7 +4725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="b">
         <v>0</v>
       </c>
@@ -4741,257 +4755,286 @@
         <v>4.8600000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="b">
+    <row r="11" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2">
+        <f>IF(TableNeed[[#This Row],[Got it?]]=FALSE, TableNeed[[#This Row],[Unit Price]]*TableNeed[[#This Row],[Quantity]], "")</f>
         <v>0</v>
       </c>
-      <c r="B11" s="1" t="s">
+    </row>
+    <row r="12" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G12" s="1">
         <v>2</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H12" s="1">
         <v>2.5099999999999998</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I12" s="4">
         <f>IF(TableNeed[[#This Row],[Got it?]]=FALSE, TableNeed[[#This Row],[Unit Price]]*TableNeed[[#This Row],[Quantity]], "")</f>
         <v>5.0199999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="B12" s="1" t="s">
+    <row r="13" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2">
+        <f>IF(TableNeed[[#This Row],[Got it?]]=FALSE, TableNeed[[#This Row],[Unit Price]]*TableNeed[[#This Row],[Quantity]], "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G14" s="1">
         <v>3</v>
       </c>
-      <c r="I12" s="4" t="str">
+      <c r="I14" s="4" t="str">
         <f>IF(TableNeed[[#This Row],[Got it?]]=FALSE, TableNeed[[#This Row],[Unit Price]]*TableNeed[[#This Row],[Quantity]], "")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="B13" s="3" t="s">
+    <row r="15" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3" t="s">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G15" s="3">
         <v>3</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2" t="str">
-        <f>IF(TableNeed[[#This Row],[Got it?]]=FALSE, TableNeed[[#This Row],[Unit Price]]*TableNeed[[#This Row],[Quantity]], "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2">
-        <f>IF(TableNeed[[#This Row],[Got it?]]=FALSE, TableNeed[[#This Row],[Unit Price]]*TableNeed[[#This Row],[Quantity]], "")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>266</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>267</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>267</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="G15" s="3">
-        <v>1</v>
-      </c>
-      <c r="H15" s="2">
-        <v>10.95</v>
-      </c>
+      <c r="H15" s="2"/>
       <c r="I15" s="2" t="str">
         <f>IF(TableNeed[[#This Row],[Got it?]]=FALSE, TableNeed[[#This Row],[Unit Price]]*TableNeed[[#This Row],[Quantity]], "")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" t="b">
+    <row r="16" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="C16" s="3"/>
+        <v>282</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>233</v>
+      </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="G16" s="3"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14">
+      <c r="H16" s="2"/>
+      <c r="I16" s="2">
         <f>IF(TableNeed[[#This Row],[Got it?]]=FALSE, TableNeed[[#This Row],[Unit Price]]*TableNeed[[#This Row],[Quantity]], "")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" t="b">
+    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1</v>
+      </c>
+      <c r="H17" s="2">
+        <v>10.95</v>
+      </c>
+      <c r="I17" s="2" t="str">
+        <f>IF(TableNeed[[#This Row],[Got it?]]=FALSE, TableNeed[[#This Row],[Unit Price]]*TableNeed[[#This Row],[Quantity]], "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="b">
         <v>0</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14">
-        <f>IF(TableNeed[[#This Row],[Got it?]]=FALSE, TableNeed[[#This Row],[Unit Price]]*TableNeed[[#This Row],[Quantity]], "")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" t="b">
-        <v>1</v>
-      </c>
       <c r="B18" s="3" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="G18" s="3">
+      <c r="G18" s="3"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14">
+        <f>IF(TableNeed[[#This Row],[Got it?]]=FALSE, TableNeed[[#This Row],[Unit Price]]*TableNeed[[#This Row],[Quantity]], "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="b">
+        <v>0</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14">
+        <f>IF(TableNeed[[#This Row],[Got it?]]=FALSE, TableNeed[[#This Row],[Unit Price]]*TableNeed[[#This Row],[Quantity]], "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="b">
+        <v>1</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="G20" s="3">
         <v>2</v>
       </c>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14" t="str">
+      <c r="H20" s="14"/>
+      <c r="I20" s="14" t="str">
         <f>IF(TableNeed[[#This Row],[Got it?]]=FALSE, TableNeed[[#This Row],[Unit Price]]*TableNeed[[#This Row],[Quantity]], "")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="9"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10" t="s">
+    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="12">
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="12">
         <f>SUBTOTAL(109,TableNeed[Total Price])</f>
         <v>9.879999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
+    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1" t="s">
+    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="G22" s="1">
-        <v>1</v>
-      </c>
-      <c r="H22" s="1">
+      <c r="G24" s="1">
+        <v>1</v>
+      </c>
+      <c r="H24" s="1">
         <v>13.88</v>
       </c>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1">
-        <v>1</v>
-      </c>
-      <c r="H23" s="1">
-        <v>13.77</v>
-      </c>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1">
+        <v>1</v>
+      </c>
+      <c r="H25" s="1">
+        <v>13.77</v>
+      </c>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Spooler Updates to BOM, Schematic.
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajohnson\GIT_Projects\ValpoFilamentRecycler09\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamj\Git Projects\ValpoFilamentRecycler09\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A957BE5-7E9D-4CB0-85FA-264F80C1D90D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA53405-6112-4943-ABC0-A0DDF1218DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Extruder" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,23 @@
     <sheet name="Controller" sheetId="5" r:id="rId3"/>
     <sheet name="Helper" sheetId="6" state="hidden" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="361">
   <si>
     <t>Quantity</t>
   </si>
@@ -508,9 +519,6 @@
     <t>NTE2984</t>
   </si>
   <si>
-    <t>N-Channel Power MOSFET, 60V, 17A, Through Hole, TO-220</t>
-  </si>
-  <si>
     <t>B2B-XH-A(LF)(SN)</t>
   </si>
   <si>
@@ -1088,6 +1096,27 @@
   </si>
   <si>
     <t>CF14JT33K0</t>
+  </si>
+  <si>
+    <t>STP16NF06</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>497-2766-5-ND</t>
+  </si>
+  <si>
+    <t>MOSFET, Spooler</t>
+  </si>
+  <si>
+    <t>MOSFET, Fans</t>
+  </si>
+  <si>
+    <t>N-Channel Power MOSFET, 60V, 16A, Through Hole, TO-220 (for 12V DC motors)</t>
+  </si>
+  <si>
+    <t>N-Channel Power MOSFET, 60V, 17A, Through Hole, TO-220 (for 5V DC motors)</t>
   </si>
 </sst>
 </file>
@@ -1180,308 +1209,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="30">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1798,6 +1525,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1821,12 +1554,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -1858,6 +1585,308 @@
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1875,16 +1904,16 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6961DE25-1017-49FB-B58C-151DD971B349}" name="TableExtruder" displayName="TableExtruder" ref="A1:J50" totalsRowCount="1" dataCellStyle="Normal">
   <autoFilter ref="A1:J49" xr:uid="{6961DE25-1017-49FB-B58C-151DD971B349}"/>
   <tableColumns count="10">
-    <tableColumn id="12" xr3:uid="{C633C4DA-E9F1-49FB-8240-86247B964FE1}" name="Part" totalsRowDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{DAB1913A-18D2-4D9A-9708-032A60B6BC64}" name="Description" totalsRowDxfId="8" dataCellStyle="Normal"/>
-    <tableColumn id="1" xr3:uid="{F1A65BEB-7A95-468E-8FAE-B504744FDB1B}" name="Preference" dataDxfId="12" totalsRowDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{EC3749CD-9468-4676-8AAA-2DE4FA028800}" name="Supplier" totalsRowDxfId="6" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{FBFB3CD0-7BF1-4266-8755-35F85270404A}" name="Supplier Part Number" totalsRowLabel="Total" totalsRowDxfId="5" dataCellStyle="Normal"/>
-    <tableColumn id="8" xr3:uid="{70763CA8-03EB-4064-9534-D2C0729DD10E}" name="Manufactuer" totalsRowDxfId="4" dataCellStyle="Normal"/>
-    <tableColumn id="9" xr3:uid="{9D792AB2-8329-471D-9251-7B5C39551B6D}" name="Manufacturer Part Number" totalsRowDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{6C81D9F0-6082-4928-8091-DA45D848F33F}" name="Quantity" totalsRowDxfId="2" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{D2BF7368-0F05-4426-9AF7-A4A54F97F689}" name="Unit Price" dataDxfId="11" totalsRowDxfId="1" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{816B8560-23EB-4218-8B09-04C10060E74B}" name="Total Price" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="0" dataCellStyle="Currency">
+    <tableColumn id="12" xr3:uid="{C633C4DA-E9F1-49FB-8240-86247B964FE1}" name="Part" totalsRowDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{DAB1913A-18D2-4D9A-9708-032A60B6BC64}" name="Description" totalsRowDxfId="28" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{F1A65BEB-7A95-468E-8FAE-B504744FDB1B}" name="Preference" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{EC3749CD-9468-4676-8AAA-2DE4FA028800}" name="Supplier" totalsRowDxfId="25" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{FBFB3CD0-7BF1-4266-8755-35F85270404A}" name="Supplier Part Number" totalsRowLabel="Total" totalsRowDxfId="24" dataCellStyle="Normal"/>
+    <tableColumn id="8" xr3:uid="{70763CA8-03EB-4064-9534-D2C0729DD10E}" name="Manufactuer" totalsRowDxfId="23" dataCellStyle="Normal"/>
+    <tableColumn id="9" xr3:uid="{9D792AB2-8329-471D-9251-7B5C39551B6D}" name="Manufacturer Part Number" totalsRowDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{6C81D9F0-6082-4928-8091-DA45D848F33F}" name="Quantity" totalsRowDxfId="21" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{D2BF7368-0F05-4426-9AF7-A4A54F97F689}" name="Unit Price" dataDxfId="20" totalsRowDxfId="19" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{816B8560-23EB-4218-8B09-04C10060E74B}" name="Total Price" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="17" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1893,19 +1922,19 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9548DB7C-B8C9-46D9-9175-857AA71A03C3}" name="TableSpooler" displayName="TableSpooler" ref="A1:J24" totalsRowCount="1" dataCellStyle="Normal">
-  <autoFilter ref="A1:J23" xr:uid="{9548DB7C-B8C9-46D9-9175-857AA71A03C3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9548DB7C-B8C9-46D9-9175-857AA71A03C3}" name="TableSpooler" displayName="TableSpooler" ref="A1:J25" totalsRowCount="1" dataCellStyle="Normal">
+  <autoFilter ref="A1:J24" xr:uid="{9548DB7C-B8C9-46D9-9175-857AA71A03C3}"/>
   <tableColumns count="10">
-    <tableColumn id="12" xr3:uid="{02FE56AC-0EFC-42AA-8A79-A19D1265C334}" name="Part" totalsRowDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{6C7F5790-A2D7-49D5-98CC-5347EEBCB1ED}" name="Description" totalsRowDxfId="21" dataCellStyle="Normal"/>
-    <tableColumn id="1" xr3:uid="{76A9DB35-CA2E-42DE-8502-AF8BEE0A03C6}" name="Preference" totalsRowDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{FF40B9DA-8160-42B4-A04B-59C3988A3C5E}" name="Supplier" totalsRowDxfId="19" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{66B504B5-4CA8-4C40-909D-18E9AADA1F9D}" name="Supplier Part Number" totalsRowLabel="Total" totalsRowDxfId="18" dataCellStyle="Normal"/>
-    <tableColumn id="8" xr3:uid="{B1FBFAC4-450D-465B-8926-44EA92A1276B}" name="Manufactuer" totalsRowDxfId="17" dataCellStyle="Normal"/>
-    <tableColumn id="9" xr3:uid="{42F90968-E8D4-4DE3-8E2B-F702BB9EC99B}" name="Manufacturer Part Number" totalsRowDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{E176CC47-E8BA-4A8D-9C82-D7F685B8FC85}" name="Quantity" totalsRowDxfId="15" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{CECFF550-A5B4-494E-8824-FFDC20FE1F96}" name="Unit Price" dataDxfId="29" totalsRowDxfId="14" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{5C811821-7EC0-4CCE-ABD1-E409C90F00A8}" name="Total Price" totalsRowFunction="sum" dataDxfId="28" totalsRowDxfId="13" dataCellStyle="Currency">
+    <tableColumn id="12" xr3:uid="{02FE56AC-0EFC-42AA-8A79-A19D1265C334}" name="Part" totalsRowDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{6C7F5790-A2D7-49D5-98CC-5347EEBCB1ED}" name="Description" totalsRowDxfId="8" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{76A9DB35-CA2E-42DE-8502-AF8BEE0A03C6}" name="Preference" totalsRowDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{FF40B9DA-8160-42B4-A04B-59C3988A3C5E}" name="Supplier" totalsRowDxfId="6" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{66B504B5-4CA8-4C40-909D-18E9AADA1F9D}" name="Supplier Part Number" totalsRowLabel="Total" totalsRowDxfId="5" dataCellStyle="Normal"/>
+    <tableColumn id="8" xr3:uid="{B1FBFAC4-450D-465B-8926-44EA92A1276B}" name="Manufactuer" totalsRowDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="9" xr3:uid="{42F90968-E8D4-4DE3-8E2B-F702BB9EC99B}" name="Manufacturer Part Number" totalsRowDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{E176CC47-E8BA-4A8D-9C82-D7F685B8FC85}" name="Quantity" totalsRowDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{CECFF550-A5B4-494E-8824-FFDC20FE1F96}" name="Unit Price" dataDxfId="16" totalsRowDxfId="1" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{5C811821-7EC0-4CCE-ABD1-E409C90F00A8}" name="Total Price" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="0" dataCellStyle="Currency">
       <calculatedColumnFormula>TableSpooler[[#This Row],[Quantity]]*TableSpooler[[#This Row],[Unit Price]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1917,7 +1946,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{463B6967-B750-4F73-A588-9468E22D51C2}" name="TableController" displayName="TableController" ref="A1:J7" totalsRowCount="1">
   <autoFilter ref="A1:J6" xr:uid="{463B6967-B750-4F73-A588-9468E22D51C2}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{CC3FED35-0EF5-4A38-A244-2A16695FE8EF}" name="Part" totalsRowLabel="Total" dataDxfId="27" totalsRowDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{CC3FED35-0EF5-4A38-A244-2A16695FE8EF}" name="Part" totalsRowLabel="Total" dataDxfId="14" totalsRowDxfId="13"/>
     <tableColumn id="2" xr3:uid="{1873956F-859F-45C7-922E-A53ECC0CA3FD}" name="Description"/>
     <tableColumn id="10" xr3:uid="{4A3A649F-92F0-4C18-81CA-5B9D728DF405}" name="Preference"/>
     <tableColumn id="3" xr3:uid="{9697BE2D-FF87-4863-A96E-7898B6D0C8A9}" name="Supplier"/>
@@ -1925,8 +1954,8 @@
     <tableColumn id="5" xr3:uid="{E99B851A-67A7-490F-8E43-FCDDABF1F182}" name="Manufactuer"/>
     <tableColumn id="6" xr3:uid="{667ECAC5-D1EB-455C-B5F6-C393586B5D5F}" name="Manufacturer Part Number"/>
     <tableColumn id="7" xr3:uid="{DE0B06EE-7D26-4607-A86C-770AACE90A28}" name="Quantity"/>
-    <tableColumn id="8" xr3:uid="{40503977-B40C-4B6F-9DEA-6C725C85FC01}" name="Unit Price" dataDxfId="26"/>
-    <tableColumn id="9" xr3:uid="{15925615-B9B9-4B30-90D7-656911F22DE7}" name="Total Price" totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="23">
+    <tableColumn id="8" xr3:uid="{40503977-B40C-4B6F-9DEA-6C725C85FC01}" name="Unit Price" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{15925615-B9B9-4B30-90D7-656911F22DE7}" name="Total Price" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10">
       <calculatedColumnFormula>TableController[[#This Row],[Unit Price]]*TableController[[#This Row],[Quantity]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2147,8 +2176,8 @@
   </sheetPr>
   <dimension ref="A1:R68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2173,13 +2202,13 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>120</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -2209,13 +2238,13 @@
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>93</v>
@@ -2243,13 +2272,13 @@
     </row>
     <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>93</v>
@@ -2277,13 +2306,13 @@
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>96</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>98</v>
@@ -2311,13 +2340,13 @@
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>93</v>
@@ -2345,13 +2374,13 @@
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>89</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>91</v>
@@ -2379,13 +2408,13 @@
     </row>
     <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
@@ -2408,13 +2437,13 @@
     </row>
     <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>84</v>
@@ -2440,13 +2469,13 @@
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>71</v>
@@ -2472,13 +2501,13 @@
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>118</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>71</v>
@@ -2504,13 +2533,13 @@
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>71</v>
@@ -2536,13 +2565,13 @@
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>71</v>
@@ -2568,13 +2597,13 @@
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>86</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>84</v>
@@ -2600,13 +2629,13 @@
     </row>
     <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>124</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>71</v>
@@ -2632,13 +2661,13 @@
     </row>
     <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>139</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>71</v>
@@ -2664,13 +2693,13 @@
     </row>
     <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>138</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>71</v>
@@ -2696,13 +2725,13 @@
     </row>
     <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>137</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>71</v>
@@ -2728,20 +2757,20 @@
     </row>
     <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H18" s="3">
         <v>1</v>
@@ -2760,13 +2789,13 @@
     </row>
     <row r="19" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>6</v>
@@ -2792,13 +2821,13 @@
     </row>
     <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>71</v>
@@ -2824,16 +2853,16 @@
     </row>
     <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>68</v>
@@ -2861,13 +2890,13 @@
     </row>
     <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>6</v>
@@ -2895,13 +2924,13 @@
     </row>
     <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>151</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>21</v>
@@ -2932,25 +2961,25 @@
     </row>
     <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>67</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H24" s="3">
         <v>2</v>
@@ -2969,13 +2998,13 @@
     </row>
     <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>135</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>67</v>
@@ -3006,13 +3035,13 @@
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>140</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>29</v>
@@ -3043,23 +3072,23 @@
     </row>
     <row r="27" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D27" s="13" t="s">
         <v>18</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="13" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H27" s="3">
         <v>2</v>
@@ -3078,25 +3107,25 @@
     </row>
     <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E28" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>227</v>
       </c>
       <c r="H28" s="3">
         <v>2</v>
@@ -3115,23 +3144,23 @@
     </row>
     <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D29" s="13" t="s">
         <v>18</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="G29" s="8" t="s">
         <v>324</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>325</v>
       </c>
       <c r="H29" s="3">
         <v>2</v>
@@ -3150,25 +3179,25 @@
     </row>
     <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D30" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>225</v>
-      </c>
       <c r="F30" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>223</v>
       </c>
       <c r="H30" s="3">
         <v>2</v>
@@ -3187,21 +3216,21 @@
     </row>
     <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H31" s="3">
         <v>2</v>
@@ -3220,21 +3249,21 @@
     </row>
     <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H32" s="3">
         <v>8</v>
@@ -3253,21 +3282,21 @@
     </row>
     <row r="33" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H33" s="1">
         <v>2</v>
@@ -3286,21 +3315,21 @@
     </row>
     <row r="34" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H34" s="3">
         <v>8</v>
@@ -3319,13 +3348,13 @@
     </row>
     <row r="35" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>100</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>101</v>
@@ -3337,7 +3366,7 @@
         <v>102</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H35" s="1">
         <v>2</v>
@@ -3356,21 +3385,21 @@
     </row>
     <row r="36" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C36" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H36" s="3">
         <v>1</v>
@@ -3389,25 +3418,25 @@
     </row>
     <row r="37" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>23</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H37" s="3">
         <v>1</v>
@@ -3426,19 +3455,19 @@
     </row>
     <row r="38" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B38" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C38" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F38" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>242</v>
       </c>
       <c r="H38">
         <v>1</v>
@@ -3457,13 +3486,13 @@
     </row>
     <row r="39" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>148</v>
@@ -3494,25 +3523,25 @@
     </row>
     <row r="40" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E40" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="F40" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="G40" s="1" t="s">
         <v>353</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>354</v>
       </c>
       <c r="H40" s="3">
         <v>1</v>
@@ -3531,13 +3560,13 @@
     </row>
     <row r="41" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>148</v>
@@ -3563,25 +3592,25 @@
     </row>
     <row r="42" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E42" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="F42" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="G42" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>273</v>
       </c>
       <c r="H42" s="3">
         <v>1</v>
@@ -3600,25 +3629,25 @@
     </row>
     <row r="43" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>117</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H43" s="1">
         <v>1</v>
@@ -3637,25 +3666,25 @@
     </row>
     <row r="44" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F44" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="G44" s="3" t="s">
         <v>254</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>255</v>
       </c>
       <c r="H44" s="3">
         <v>1</v>
@@ -3674,22 +3703,22 @@
     </row>
     <row r="45" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G45" s="3">
         <v>4301.1409000000003</v>
@@ -3711,22 +3740,22 @@
     </row>
     <row r="46" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G46" s="3">
         <v>34.3127</v>
@@ -3748,25 +3777,25 @@
     </row>
     <row r="47" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E47" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="G47" s="1" t="s">
         <v>342</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>343</v>
       </c>
       <c r="H47" s="3">
         <v>1</v>
@@ -3785,13 +3814,13 @@
     </row>
     <row r="48" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>104</v>
@@ -3817,13 +3846,13 @@
     </row>
     <row r="49" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>29</v>
@@ -3835,7 +3864,7 @@
         <v>66</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H49" s="1">
         <v>2</v>
@@ -3876,7 +3905,7 @@
     <row r="51" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="9"/>
       <c r="B51" s="10" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C51" s="9"/>
       <c r="D51" s="10"/>
@@ -3894,7 +3923,7 @@
     <row r="52" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="9"/>
       <c r="B52" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C52" s="9"/>
       <c r="D52" s="10"/>
@@ -3912,7 +3941,7 @@
     <row r="53" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="9"/>
       <c r="B53" s="10" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C53" s="9"/>
       <c r="D53" s="10"/>
@@ -3942,7 +3971,7 @@
     <row r="55" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="B55" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -4001,7 +4030,7 @@
     <row r="58" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
       <c r="B58" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1" t="s">
@@ -4043,7 +4072,7 @@
     <row r="60" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
       <c r="B60" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -4100,7 +4129,7 @@
     <row r="63" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
       <c r="B63" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -4115,7 +4144,7 @@
     <row r="64" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
       <c r="B64" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1" t="s">
@@ -4152,20 +4181,20 @@
     </row>
     <row r="66" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G66"/>
       <c r="H66"/>
     </row>
     <row r="67" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F67" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G67" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H67">
         <v>1</v>
@@ -4176,19 +4205,19 @@
     </row>
     <row r="68" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
+        <v>316</v>
+      </c>
+      <c r="D68" t="s">
+        <v>223</v>
+      </c>
+      <c r="E68" t="s">
+        <v>315</v>
+      </c>
+      <c r="F68" t="s">
+        <v>318</v>
+      </c>
+      <c r="G68" t="s">
         <v>317</v>
-      </c>
-      <c r="D68" t="s">
-        <v>224</v>
-      </c>
-      <c r="E68" t="s">
-        <v>316</v>
-      </c>
-      <c r="F68" t="s">
-        <v>319</v>
-      </c>
-      <c r="G68" t="s">
-        <v>318</v>
       </c>
       <c r="H68">
         <v>1</v>
@@ -4236,15 +4265,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC497086-9290-4C1D-9300-28557D6CEBE4}">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="96.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
@@ -4258,13 +4287,13 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>120</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -4290,13 +4319,13 @@
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>71</v>
@@ -4321,7 +4350,7 @@
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>146</v>
@@ -4352,7 +4381,7 @@
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>126</v>
@@ -4381,7 +4410,7 @@
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
@@ -4412,10 +4441,10 @@
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
@@ -4428,7 +4457,7 @@
         <v>48</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H6" s="1">
         <v>1</v>
@@ -4443,7 +4472,7 @@
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>105</v>
@@ -4470,7 +4499,7 @@
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>147</v>
@@ -4501,19 +4530,19 @@
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H9" s="3">
         <v>1</v>
@@ -4523,10 +4552,10 @@
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>229</v>
+        <v>358</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>161</v>
+        <v>360</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
@@ -4553,565 +4582,577 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="A11" s="13" t="s">
+        <v>357</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2">
+        <f>TableSpooler[[#This Row],[Quantity]]*TableSpooler[[#This Row],[Unit Price]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1" t="s">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H11" s="1">
-        <v>1</v>
-      </c>
-      <c r="I11" s="4">
+      <c r="H12" s="1">
+        <v>1</v>
+      </c>
+      <c r="I12" s="4">
         <v>22</v>
       </c>
-      <c r="J11" s="14">
+      <c r="J12" s="14">
         <f>TableSpooler[[#This Row],[Quantity]]*TableSpooler[[#This Row],[Unit Price]]</f>
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="H12" s="1">
-        <v>1</v>
-      </c>
-      <c r="I12" s="4">
-        <v>0.48</v>
-      </c>
-      <c r="J12" s="14">
-        <f>TableSpooler[[#This Row],[Quantity]]*TableSpooler[[#This Row],[Unit Price]]</f>
-        <v>0.48</v>
-      </c>
-    </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="H13" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I13" s="4">
-        <v>0.51</v>
+        <v>0.48</v>
       </c>
       <c r="J13" s="14">
         <f>TableSpooler[[#This Row],[Quantity]]*TableSpooler[[#This Row],[Unit Price]]</f>
-        <v>2.5499999999999998</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="H14" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I14" s="4">
-        <v>0.15</v>
+        <v>0.51</v>
       </c>
       <c r="J14" s="14">
         <f>TableSpooler[[#This Row],[Quantity]]*TableSpooler[[#This Row],[Unit Price]]</f>
-        <v>1.05</v>
+        <v>2.5499999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" s="3" t="s">
+      <c r="E15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="H15" s="3">
+      <c r="G15" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H15" s="1">
         <v>7</v>
       </c>
-      <c r="I15" s="5">
-        <v>0.1</v>
+      <c r="I15" s="4">
+        <v>0.15</v>
       </c>
       <c r="J15" s="14">
         <f>TableSpooler[[#This Row],[Quantity]]*TableSpooler[[#This Row],[Unit Price]]</f>
-        <v>0.70000000000000007</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="B16" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1" t="s">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="E16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="H16" s="1">
-        <v>4</v>
-      </c>
-      <c r="I16" s="4">
-        <v>0.19</v>
+      <c r="G16" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="H16" s="3">
+        <v>7</v>
+      </c>
+      <c r="I16" s="5">
+        <v>0.1</v>
       </c>
       <c r="J16" s="14">
         <f>TableSpooler[[#This Row],[Quantity]]*TableSpooler[[#This Row],[Unit Price]]</f>
-        <v>0.76</v>
+        <v>0.70000000000000007</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="H17" s="1">
         <v>4</v>
       </c>
       <c r="I17" s="4">
-        <v>0.1</v>
+        <v>0.19</v>
       </c>
       <c r="J17" s="14">
         <f>TableSpooler[[#This Row],[Quantity]]*TableSpooler[[#This Row],[Unit Price]]</f>
-        <v>0.4</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="H18" s="1">
         <v>4</v>
       </c>
       <c r="I18" s="4">
-        <v>0.21</v>
+        <v>0.1</v>
       </c>
       <c r="J18" s="14">
         <f>TableSpooler[[#This Row],[Quantity]]*TableSpooler[[#This Row],[Unit Price]]</f>
-        <v>0.84</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="H19" s="1">
         <v>4</v>
       </c>
       <c r="I19" s="4">
-        <v>0.1</v>
+        <v>0.21</v>
       </c>
       <c r="J19" s="14">
         <f>TableSpooler[[#This Row],[Quantity]]*TableSpooler[[#This Row],[Unit Price]]</f>
-        <v>0.4</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="H20" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I20" s="4">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="J20" s="14">
         <f>TableSpooler[[#This Row],[Quantity]]*TableSpooler[[#This Row],[Unit Price]]</f>
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="H21" s="1">
         <v>2</v>
       </c>
       <c r="I21" s="4">
-        <v>0.14000000000000001</v>
+        <v>0.25</v>
       </c>
       <c r="J21" s="14">
         <f>TableSpooler[[#This Row],[Quantity]]*TableSpooler[[#This Row],[Unit Price]]</f>
-        <v>0.28000000000000003</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="8" t="s">
-        <v>229</v>
+      <c r="A22" s="1" t="s">
+        <v>228</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>15</v>
+        <v>181</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="F22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G22" s="1"/>
+        <v>52</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>178</v>
+      </c>
       <c r="H22" s="1">
-        <v>1</v>
-      </c>
-      <c r="I22" s="1">
-        <v>14.99</v>
+        <v>2</v>
+      </c>
+      <c r="I22" s="4">
+        <v>0.14000000000000001</v>
       </c>
       <c r="J22" s="14">
         <f>TableSpooler[[#This Row],[Quantity]]*TableSpooler[[#This Row],[Unit Price]]</f>
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
+      <c r="I23" s="1">
         <v>14.99</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>246</v>
-      </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="16">
-        <v>1</v>
-      </c>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18">
+      <c r="J23" s="14">
+        <f>TableSpooler[[#This Row],[Quantity]]*TableSpooler[[#This Row],[Unit Price]]</f>
+        <v>14.99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="22" t="s">
+        <v>346</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="C24" s="22"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="16">
+        <v>1</v>
+      </c>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18">
         <f>TableSpooler[[#This Row],[Quantity]]*TableSpooler[[#This Row],[Unit Price]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="9"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10" t="s">
+    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="9"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="12">
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="12">
         <f>SUBTOTAL(109,TableSpooler[Total Price])</f>
         <v>272.25999999999993</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
+    <row r="26" spans="1:11" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="H26" s="1">
-        <v>2</v>
-      </c>
-      <c r="I26" s="1">
-        <v>6.97</v>
-      </c>
-      <c r="J26" s="1"/>
+        <v>266</v>
+      </c>
     </row>
     <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
+      <c r="B27" s="1" t="s">
+        <v>193</v>
+      </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
+      <c r="D27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H27" s="1">
+        <v>2</v>
+      </c>
+      <c r="I27" s="1">
+        <v>6.97</v>
+      </c>
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>262</v>
-      </c>
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
     </row>
     <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1" t="s">
+      <c r="C30" s="1"/>
+      <c r="D30" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F30" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="H29" s="1">
+      <c r="H30" s="1">
         <v>3</v>
       </c>
-      <c r="I29" s="1">
+      <c r="I30" s="1">
         <v>22.51</v>
       </c>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-    </row>
-    <row r="30" spans="1:11" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="1" t="s">
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+    </row>
+    <row r="31" spans="1:11" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="H30" s="1">
-        <v>1</v>
-      </c>
-      <c r="I30" s="1">
+      <c r="H31" s="1">
+        <v>1</v>
+      </c>
+      <c r="I31" s="1">
         <v>32.1</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1" t="s">
+    <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G32" s="1">
         <v>4685</v>
       </c>
-      <c r="H31" s="1">
-        <v>1</v>
-      </c>
-      <c r="I31" s="1">
+      <c r="H32" s="1">
+        <v>1</v>
+      </c>
+      <c r="I32" s="1">
         <v>24.95</v>
       </c>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-    </row>
-    <row r="32" spans="1:11" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="1" t="s">
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+    </row>
+    <row r="33" spans="1:11" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H32" s="1">
-        <v>1</v>
-      </c>
-      <c r="I32" s="1">
+      <c r="H33" s="1">
+        <v>1</v>
+      </c>
+      <c r="I33" s="1">
         <v>9.99</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
     </row>
     <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
-      <c r="B34" s="1" t="s">
-        <v>263</v>
-      </c>
+      <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -5125,75 +5166,90 @@
     <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
-        <v>203</v>
+        <v>262</v>
       </c>
       <c r="C35" s="1"/>
-      <c r="D35" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="H35" s="1">
-        <v>2</v>
-      </c>
-      <c r="I35" s="1">
-        <v>17.39</v>
-      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:11" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" t="s">
-        <v>230</v>
-      </c>
-    </row>
+    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H36" s="1">
+        <v>2</v>
+      </c>
+      <c r="I36" s="1">
+        <v>17.39</v>
+      </c>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+    </row>
+    <row r="37" spans="1:11" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="H38" s="1">
-        <v>1</v>
-      </c>
-      <c r="I38" s="1">
-        <v>13.88</v>
+      <c r="B38" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="H39" s="1">
+        <v>1</v>
+      </c>
+      <c r="I39" s="1">
+        <v>13.88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1">
-        <v>1</v>
-      </c>
-      <c r="I39" s="1">
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1">
+        <v>1</v>
+      </c>
+      <c r="I40" s="1">
         <v>13.77</v>
       </c>
     </row>
@@ -5234,7 +5290,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5253,13 +5309,13 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>120</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -5289,7 +5345,7 @@
         <v>132</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>29</v>
@@ -5317,10 +5373,10 @@
     <row r="3" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>29</v>
@@ -5404,17 +5460,17 @@
     <row r="6" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="B6" s="13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>248</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>249</v>
       </c>
       <c r="H6" s="3">
         <v>1</v>
@@ -5453,7 +5509,7 @@
     <row r="9" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9"/>
       <c r="B9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C9"/>
       <c r="D9"/>
@@ -5471,7 +5527,7 @@
     <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
@@ -5481,10 +5537,10 @@
         <v>110</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H10" s="1">
         <v>1</v>
@@ -5520,7 +5576,7 @@
     </row>
     <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5552,16 +5608,16 @@
     <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H15" s="1">
         <v>1</v>
@@ -5599,7 +5655,7 @@
     </row>
     <row r="17" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>29</v>
@@ -5611,7 +5667,7 @@
         <v>62</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H17" s="1">
         <v>1</v>
@@ -5689,22 +5745,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 12V to 5V DC/DC Converter.
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamj\Git Projects\ValpoFilamentRecycler09\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA53405-6112-4943-ABC0-A0DDF1218DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3CE320-40AF-4BFE-B683-8742E1FD8165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Extruder" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="381">
   <si>
     <t>Quantity</t>
   </si>
@@ -654,9 +654,6 @@
     <t>DC Speed Control, Chassis, 0 to 48V DC Voltage Output, 20 A Max. Amps</t>
   </si>
   <si>
-    <t>Spooler</t>
-  </si>
-  <si>
     <t>Linear Optical Array Sensor I2C, SPI Output</t>
   </si>
   <si>
@@ -690,9 +687,6 @@
     <t>Fixture</t>
   </si>
   <si>
-    <t>Slack Sensor</t>
-  </si>
-  <si>
     <t>Fan</t>
   </si>
   <si>
@@ -720,9 +714,6 @@
     <t>TE Connectivity</t>
   </si>
   <si>
-    <t>Electronics</t>
-  </si>
-  <si>
     <t>EXTRA PARTS</t>
   </si>
   <si>
@@ -1117,6 +1108,75 @@
   </si>
   <si>
     <t>N-Channel Power MOSFET, 60V, 17A, Through Hole, TO-220 (for 5V DC motors)</t>
+  </si>
+  <si>
+    <t>1N5819</t>
+  </si>
+  <si>
+    <t>DC/DC Converter</t>
+  </si>
+  <si>
+    <t>945-2201-ND</t>
+  </si>
+  <si>
+    <t>Recom Power</t>
+  </si>
+  <si>
+    <t>R-78E5.0-1.0</t>
+  </si>
+  <si>
+    <t>Linear Regulator DC DC Converter, 8V - 28V Input, 5V, 1A Output</t>
+  </si>
+  <si>
+    <t>Bearing</t>
+  </si>
+  <si>
+    <t>USB Cable</t>
+  </si>
+  <si>
+    <t>Photo Interrupter</t>
+  </si>
+  <si>
+    <t>Load Cell</t>
+  </si>
+  <si>
+    <t>Spooler Motor</t>
+  </si>
+  <si>
+    <t>Arduino Uno</t>
+  </si>
+  <si>
+    <t>USB-A Connector</t>
+  </si>
+  <si>
+    <t>Headers, Male</t>
+  </si>
+  <si>
+    <t>Connector, 2 position</t>
+  </si>
+  <si>
+    <t>Plug, 2 position</t>
+  </si>
+  <si>
+    <t>Connector, 3 position</t>
+  </si>
+  <si>
+    <t>Plug, 3 position</t>
+  </si>
+  <si>
+    <t>Connector, 4 position</t>
+  </si>
+  <si>
+    <t>Plug, 4 position</t>
+  </si>
+  <si>
+    <t>Connector, 5 position</t>
+  </si>
+  <si>
+    <t>Plug, 6 position</t>
+  </si>
+  <si>
+    <t>Wire</t>
   </si>
 </sst>
 </file>
@@ -1177,7 +1237,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -1197,7 +1257,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1525,12 +1584,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1554,6 +1607,12 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -1901,8 +1960,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6961DE25-1017-49FB-B58C-151DD971B349}" name="TableExtruder" displayName="TableExtruder" ref="A1:J50" totalsRowCount="1" dataCellStyle="Normal">
-  <autoFilter ref="A1:J49" xr:uid="{6961DE25-1017-49FB-B58C-151DD971B349}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6961DE25-1017-49FB-B58C-151DD971B349}" name="TableExtruder" displayName="TableExtruder" ref="A1:J51" totalsRowCount="1" dataCellStyle="Normal">
+  <autoFilter ref="A1:J50" xr:uid="{6961DE25-1017-49FB-B58C-151DD971B349}"/>
   <tableColumns count="10">
     <tableColumn id="12" xr3:uid="{C633C4DA-E9F1-49FB-8240-86247B964FE1}" name="Part" totalsRowDxfId="29"/>
     <tableColumn id="2" xr3:uid="{DAB1913A-18D2-4D9A-9708-032A60B6BC64}" name="Description" totalsRowDxfId="28" dataCellStyle="Normal"/>
@@ -1943,10 +2002,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{463B6967-B750-4F73-A588-9468E22D51C2}" name="TableController" displayName="TableController" ref="A1:J7" totalsRowCount="1">
-  <autoFilter ref="A1:J6" xr:uid="{463B6967-B750-4F73-A588-9468E22D51C2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{463B6967-B750-4F73-A588-9468E22D51C2}" name="TableController" displayName="TableController" ref="A1:J8" totalsRowCount="1">
+  <autoFilter ref="A1:J7" xr:uid="{463B6967-B750-4F73-A588-9468E22D51C2}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{CC3FED35-0EF5-4A38-A244-2A16695FE8EF}" name="Part" totalsRowLabel="Total" dataDxfId="14" totalsRowDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{CC3FED35-0EF5-4A38-A244-2A16695FE8EF}" name="Part" totalsRowLabel="Total" dataDxfId="14" totalsRowDxfId="11"/>
     <tableColumn id="2" xr3:uid="{1873956F-859F-45C7-922E-A53ECC0CA3FD}" name="Description"/>
     <tableColumn id="10" xr3:uid="{4A3A649F-92F0-4C18-81CA-5B9D728DF405}" name="Preference"/>
     <tableColumn id="3" xr3:uid="{9697BE2D-FF87-4863-A96E-7898B6D0C8A9}" name="Supplier"/>
@@ -1954,8 +2013,8 @@
     <tableColumn id="5" xr3:uid="{E99B851A-67A7-490F-8E43-FCDDABF1F182}" name="Manufactuer"/>
     <tableColumn id="6" xr3:uid="{667ECAC5-D1EB-455C-B5F6-C393586B5D5F}" name="Manufacturer Part Number"/>
     <tableColumn id="7" xr3:uid="{DE0B06EE-7D26-4607-A86C-770AACE90A28}" name="Quantity"/>
-    <tableColumn id="8" xr3:uid="{40503977-B40C-4B6F-9DEA-6C725C85FC01}" name="Unit Price" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{15925615-B9B9-4B30-90D7-656911F22DE7}" name="Total Price" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10">
+    <tableColumn id="8" xr3:uid="{40503977-B40C-4B6F-9DEA-6C725C85FC01}" name="Unit Price" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{15925615-B9B9-4B30-90D7-656911F22DE7}" name="Total Price" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="10">
       <calculatedColumnFormula>TableController[[#This Row],[Unit Price]]*TableController[[#This Row],[Quantity]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2174,10 +2233,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:R68"/>
+  <dimension ref="A1:R69"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2202,13 +2261,13 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>120</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -2238,13 +2297,13 @@
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>93</v>
@@ -2272,13 +2331,13 @@
     </row>
     <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>93</v>
@@ -2306,13 +2365,13 @@
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>96</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>98</v>
@@ -2340,13 +2399,13 @@
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>93</v>
@@ -2374,13 +2433,13 @@
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>89</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>91</v>
@@ -2407,14 +2466,14 @@
       <c r="R6" s="1"/>
     </row>
     <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
-        <v>292</v>
+      <c r="A7" s="19" t="s">
+        <v>289</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>249</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>277</v>
+        <v>246</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>274</v>
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
@@ -2423,8 +2482,8 @@
       <c r="H7" s="16">
         <v>1</v>
       </c>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21">
+      <c r="I7" s="20"/>
+      <c r="J7" s="20">
         <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
         <v>0</v>
       </c>
@@ -2437,13 +2496,13 @@
     </row>
     <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>187</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>84</v>
@@ -2469,13 +2528,13 @@
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>71</v>
@@ -2501,13 +2560,13 @@
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>118</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>71</v>
@@ -2533,13 +2592,13 @@
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>71</v>
@@ -2565,13 +2624,13 @@
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>71</v>
@@ -2597,13 +2656,13 @@
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>86</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>84</v>
@@ -2629,13 +2688,13 @@
     </row>
     <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>124</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>71</v>
@@ -2661,13 +2720,13 @@
     </row>
     <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>139</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>71</v>
@@ -2693,13 +2752,13 @@
     </row>
     <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>138</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>71</v>
@@ -2725,13 +2784,13 @@
     </row>
     <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>137</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>71</v>
@@ -2757,20 +2816,20 @@
     </row>
     <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="H18" s="3">
         <v>1</v>
@@ -2789,13 +2848,13 @@
     </row>
     <row r="19" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>6</v>
@@ -2821,13 +2880,13 @@
     </row>
     <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>186</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>71</v>
@@ -2853,13 +2912,13 @@
     </row>
     <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>203</v>
@@ -2890,13 +2949,13 @@
     </row>
     <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>6</v>
@@ -2924,13 +2983,13 @@
     </row>
     <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>151</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>21</v>
@@ -2961,25 +3020,25 @@
     </row>
     <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>67</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="H24" s="3">
         <v>2</v>
@@ -2998,13 +3057,13 @@
     </row>
     <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>135</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>67</v>
@@ -3035,13 +3094,13 @@
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>140</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>29</v>
@@ -3072,23 +3131,23 @@
     </row>
     <row r="27" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D27" s="13" t="s">
         <v>18</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="13" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="H27" s="3">
         <v>2</v>
@@ -3107,25 +3166,25 @@
     </row>
     <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D28" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>225</v>
-      </c>
       <c r="F28" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H28" s="3">
         <v>2</v>
@@ -3144,23 +3203,23 @@
     </row>
     <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D29" s="13" t="s">
         <v>18</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="13" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="H29" s="3">
         <v>2</v>
@@ -3179,25 +3238,25 @@
     </row>
     <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H30" s="3">
         <v>2</v>
@@ -3216,21 +3275,21 @@
     </row>
     <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="H31" s="3">
         <v>2</v>
@@ -3249,21 +3308,21 @@
     </row>
     <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>339</v>
-      </c>
       <c r="C32" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="H32" s="3">
         <v>8</v>
@@ -3282,21 +3341,21 @@
     </row>
     <row r="33" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="H33" s="1">
         <v>2</v>
@@ -3315,21 +3374,21 @@
     </row>
     <row r="34" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="H34" s="3">
         <v>8</v>
@@ -3348,13 +3407,13 @@
     </row>
     <row r="35" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>100</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>101</v>
@@ -3385,21 +3444,21 @@
     </row>
     <row r="36" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C36" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H36" s="3">
         <v>1</v>
@@ -3418,25 +3477,25 @@
     </row>
     <row r="37" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="13" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>23</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H37" s="3">
         <v>1</v>
@@ -3455,19 +3514,19 @@
     </row>
     <row r="38" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B38" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C38" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="H38">
         <v>1</v>
@@ -3486,13 +3545,13 @@
     </row>
     <row r="39" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>148</v>
@@ -3523,25 +3582,25 @@
     </row>
     <row r="40" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H40" s="3">
         <v>1</v>
@@ -3560,13 +3619,13 @@
     </row>
     <row r="41" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>148</v>
@@ -3592,25 +3651,25 @@
     </row>
     <row r="42" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="H42" s="3">
         <v>1</v>
@@ -3629,13 +3688,13 @@
     </row>
     <row r="43" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>205</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>203</v>
@@ -3644,7 +3703,7 @@
         <v>117</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>204</v>
@@ -3666,25 +3725,25 @@
     </row>
     <row r="44" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="H44" s="3">
         <v>1</v>
@@ -3703,22 +3762,22 @@
     </row>
     <row r="45" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G45" s="3">
         <v>4301.1409000000003</v>
@@ -3740,22 +3799,22 @@
     </row>
     <row r="46" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G46" s="3">
         <v>34.3127</v>
@@ -3777,25 +3836,25 @@
     </row>
     <row r="47" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="13" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="H47" s="3">
         <v>1</v>
@@ -3814,13 +3873,13 @@
     </row>
     <row r="48" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="13" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>104</v>
@@ -3846,13 +3905,13 @@
     </row>
     <row r="49" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="13" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>167</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>29</v>
@@ -3882,20 +3941,24 @@
       <c r="R49" s="1"/>
     </row>
     <row r="50" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="9"/>
-      <c r="B50" s="10"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
-      <c r="H50" s="10"/>
-      <c r="I50" s="11"/>
-      <c r="J50" s="12">
-        <f>SUBTOTAL(109,TableExtruder[Total Price])</f>
-        <v>2236.4799999999996</v>
+      <c r="A50" s="13"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="H50" s="3">
+        <v>4</v>
+      </c>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2">
+        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
+        <v>0</v>
       </c>
       <c r="K50"/>
       <c r="M50" s="1"/>
@@ -3904,17 +3967,20 @@
     </row>
     <row r="51" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="9"/>
-      <c r="B51" s="10" t="s">
-        <v>330</v>
-      </c>
+      <c r="B51" s="10"/>
       <c r="C51" s="9"/>
       <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
+      <c r="E51" s="10" t="s">
+        <v>103</v>
+      </c>
       <c r="F51" s="10"/>
       <c r="G51" s="10"/>
       <c r="H51" s="10"/>
       <c r="I51" s="11"/>
-      <c r="J51" s="12"/>
+      <c r="J51" s="12">
+        <f>SUBTOTAL(109,TableExtruder[Total Price])</f>
+        <v>2236.4799999999996</v>
+      </c>
       <c r="K51"/>
       <c r="M51" s="1"/>
       <c r="P51" s="4"/>
@@ -3923,7 +3989,7 @@
     <row r="52" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="9"/>
       <c r="B52" s="10" t="s">
-        <v>289</v>
+        <v>327</v>
       </c>
       <c r="C52" s="9"/>
       <c r="D52" s="10"/>
@@ -3941,7 +4007,7 @@
     <row r="53" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="9"/>
       <c r="B53" s="10" t="s">
-        <v>309</v>
+        <v>286</v>
       </c>
       <c r="C53" s="9"/>
       <c r="D53" s="10"/>
@@ -3958,7 +4024,9 @@
     </row>
     <row r="54" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="9"/>
-      <c r="B54" s="10"/>
+      <c r="B54" s="10" t="s">
+        <v>306</v>
+      </c>
       <c r="C54" s="9"/>
       <c r="D54" s="10"/>
       <c r="E54" s="10"/>
@@ -3969,35 +4037,27 @@
       <c r="J54" s="12"/>
     </row>
     <row r="55" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="I55" s="1"/>
+      <c r="A55" s="9"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
+      <c r="H55" s="10"/>
+      <c r="I55" s="11"/>
+      <c r="J55" s="12"/>
     </row>
     <row r="56" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
       <c r="B56" s="1" t="s">
-        <v>81</v>
+        <v>265</v>
       </c>
       <c r="C56" s="1"/>
-      <c r="D56" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
       <c r="F56" s="1"/>
-      <c r="H56" s="1">
-        <v>1</v>
-      </c>
-      <c r="I56" s="1">
-        <v>43.8</v>
-      </c>
+      <c r="I56" s="1"/>
       <c r="K56"/>
       <c r="M56" s="1"/>
       <c r="P56" s="4"/>
@@ -4006,21 +4066,21 @@
     <row r="57" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
       <c r="B57" s="1" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="F57" s="1"/>
       <c r="H57" s="1">
         <v>1</v>
       </c>
       <c r="I57" s="1">
-        <v>43.82</v>
+        <v>43.8</v>
       </c>
       <c r="K57"/>
       <c r="M57" s="1"/>
@@ -4030,26 +4090,21 @@
     <row r="58" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
       <c r="B58" s="1" t="s">
-        <v>264</v>
+        <v>111</v>
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>130</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="F58" s="1"/>
       <c r="H58" s="1">
         <v>1</v>
       </c>
       <c r="I58" s="1">
-        <v>20.25</v>
+        <v>43.82</v>
       </c>
       <c r="K58"/>
       <c r="M58" s="1"/>
@@ -4058,12 +4113,28 @@
     </row>
     <row r="59" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
+      <c r="B59" s="1" t="s">
+        <v>261</v>
+      </c>
       <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-      <c r="I59" s="1"/>
+      <c r="D59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H59" s="1">
+        <v>1</v>
+      </c>
+      <c r="I59" s="1">
+        <v>20.25</v>
+      </c>
       <c r="K59"/>
       <c r="M59" s="1"/>
       <c r="P59" s="4"/>
@@ -4071,9 +4142,7 @@
     </row>
     <row r="60" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
-      <c r="B60" s="1" t="s">
-        <v>265</v>
-      </c>
+      <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
@@ -4087,27 +4156,13 @@
     <row r="61" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
       <c r="B61" s="1" t="s">
-        <v>121</v>
+        <v>262</v>
       </c>
       <c r="C61" s="1"/>
-      <c r="D61" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="H61" s="1">
-        <v>1</v>
-      </c>
-      <c r="I61" s="1">
-        <v>19.54</v>
-      </c>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="I61" s="1"/>
       <c r="K61"/>
       <c r="M61" s="1"/>
       <c r="P61" s="4"/>
@@ -4115,12 +4170,28 @@
     </row>
     <row r="62" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
+      <c r="B62" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-      <c r="I62" s="1"/>
+      <c r="D62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="H62" s="1">
+        <v>1</v>
+      </c>
+      <c r="I62" s="1">
+        <v>19.54</v>
+      </c>
       <c r="K62"/>
       <c r="M62" s="1"/>
       <c r="P62" s="4"/>
@@ -4128,9 +4199,7 @@
     </row>
     <row r="63" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
-      <c r="B63" s="1" t="s">
-        <v>261</v>
-      </c>
+      <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
@@ -4144,27 +4213,13 @@
     <row r="64" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
       <c r="B64" s="1" t="s">
-        <v>239</v>
+        <v>258</v>
       </c>
       <c r="C64" s="1"/>
-      <c r="D64" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H64" s="1">
-        <v>1</v>
-      </c>
-      <c r="I64" s="1">
-        <v>410</v>
-      </c>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="I64" s="1"/>
       <c r="K64"/>
       <c r="M64" s="1"/>
       <c r="P64" s="4"/>
@@ -4172,57 +4227,82 @@
     </row>
     <row r="65" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
+      <c r="B65" s="1" t="s">
+        <v>236</v>
+      </c>
       <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-      <c r="I65" s="1"/>
+      <c r="D65" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H65" s="1">
+        <v>1</v>
+      </c>
+      <c r="I65" s="1">
+        <v>410</v>
+      </c>
     </row>
     <row r="66" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B66" t="s">
-        <v>273</v>
-      </c>
-      <c r="G66"/>
-      <c r="H66"/>
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="I66" s="1"/>
     </row>
     <row r="67" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
-        <v>275</v>
-      </c>
-      <c r="F67" t="s">
-        <v>227</v>
-      </c>
-      <c r="G67" t="s">
-        <v>274</v>
-      </c>
-      <c r="H67">
-        <v>1</v>
-      </c>
-      <c r="I67">
-        <v>19.32</v>
-      </c>
+        <v>270</v>
+      </c>
+      <c r="G67"/>
+      <c r="H67"/>
     </row>
     <row r="68" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
-        <v>316</v>
-      </c>
-      <c r="D68" t="s">
-        <v>223</v>
-      </c>
-      <c r="E68" t="s">
+        <v>272</v>
+      </c>
+      <c r="F68" t="s">
+        <v>225</v>
+      </c>
+      <c r="G68" t="s">
+        <v>271</v>
+      </c>
+      <c r="H68">
+        <v>1</v>
+      </c>
+      <c r="I68">
+        <v>19.32</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B69" t="s">
+        <v>313</v>
+      </c>
+      <c r="D69" t="s">
+        <v>221</v>
+      </c>
+      <c r="E69" t="s">
+        <v>312</v>
+      </c>
+      <c r="F69" t="s">
         <v>315</v>
       </c>
-      <c r="F68" t="s">
-        <v>318</v>
-      </c>
-      <c r="G68" t="s">
-        <v>317</v>
-      </c>
-      <c r="H68">
-        <v>1</v>
-      </c>
-      <c r="I68">
+      <c r="G69" t="s">
+        <v>314</v>
+      </c>
+      <c r="H69">
+        <v>1</v>
+      </c>
+      <c r="I69">
         <v>14.65</v>
       </c>
     </row>
@@ -4255,7 +4335,7 @@
           <x14:formula1>
             <xm:f>Helper!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C49</xm:sqref>
+          <xm:sqref>C2:C50</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4268,12 +4348,12 @@
   <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="96.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
@@ -4287,13 +4367,13 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>120</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -4319,13 +4399,13 @@
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>188</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>71</v>
@@ -4348,40 +4428,39 @@
         <v>96.1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="B3" s="16" t="s">
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="1">
         <v>2</v>
       </c>
-      <c r="I3" s="17">
+      <c r="I3" s="1">
         <v>13.27</v>
       </c>
-      <c r="J3" s="18">
+      <c r="J3" s="1">
         <f>TableSpooler[[#This Row],[Quantity]]*TableSpooler[[#This Row],[Unit Price]]</f>
         <v>26.54</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>126</v>
@@ -4410,7 +4489,7 @@
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>220</v>
+        <v>364</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
@@ -4441,7 +4520,7 @@
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>220</v>
+        <v>365</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>169</v>
@@ -4472,7 +4551,7 @@
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>218</v>
+        <v>366</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>105</v>
@@ -4499,7 +4578,7 @@
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>206</v>
+        <v>367</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>147</v>
@@ -4530,19 +4609,19 @@
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>206</v>
+        <v>368</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G9" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="H9" s="3">
         <v>1</v>
@@ -4552,10 +4631,10 @@
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
@@ -4583,23 +4662,23 @@
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="2"/>
@@ -4610,7 +4689,7 @@
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>228</v>
+        <v>369</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>153</v>
@@ -4641,7 +4720,7 @@
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>228</v>
+        <v>370</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>155</v>
@@ -4672,7 +4751,7 @@
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>228</v>
+        <v>371</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>171</v>
@@ -4703,7 +4782,7 @@
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>228</v>
+        <v>372</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>172</v>
@@ -4734,7 +4813,7 @@
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>228</v>
+        <v>373</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>175</v>
@@ -4765,7 +4844,7 @@
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>228</v>
+        <v>374</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>174</v>
@@ -4796,7 +4875,7 @@
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>228</v>
+        <v>375</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>179</v>
@@ -4827,7 +4906,7 @@
     </row>
     <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>228</v>
+        <v>376</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>185</v>
@@ -4858,7 +4937,7 @@
     </row>
     <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>228</v>
+        <v>377</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>180</v>
@@ -4889,7 +4968,7 @@
     </row>
     <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>228</v>
+        <v>378</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>184</v>
@@ -4920,7 +4999,7 @@
     </row>
     <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>228</v>
+        <v>379</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>181</v>
@@ -4951,7 +5030,7 @@
     </row>
     <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>228</v>
+        <v>380</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>15</v>
@@ -4977,22 +5056,22 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="22" t="s">
-        <v>346</v>
+      <c r="A24" s="21" t="s">
+        <v>343</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>245</v>
-      </c>
-      <c r="C24" s="22"/>
+        <v>242</v>
+      </c>
+      <c r="C24" s="21"/>
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
       <c r="F24" s="16"/>
-      <c r="G24" s="22"/>
+      <c r="G24" s="21"/>
       <c r="H24" s="16">
         <v>1</v>
       </c>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18">
+      <c r="I24" s="17"/>
+      <c r="J24" s="17">
         <f>TableSpooler[[#This Row],[Quantity]]*TableSpooler[[#This Row],[Unit Price]]</f>
         <v>0</v>
       </c>
@@ -5016,7 +5095,7 @@
     </row>
     <row r="26" spans="1:11" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5059,7 +5138,7 @@
     </row>
     <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5109,7 +5188,7 @@
     <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1" t="s">
@@ -5166,7 +5245,7 @@
     <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -5208,12 +5287,12 @@
     <row r="37" spans="1:11" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>21</v>
@@ -5290,12 +5369,12 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
@@ -5309,13 +5388,13 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>120</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -5345,7 +5424,7 @@
         <v>132</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>29</v>
@@ -5376,7 +5455,7 @@
         <v>162</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>29</v>
@@ -5460,17 +5539,17 @@
     <row r="6" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="B6" s="13" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="13" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="H6" s="3">
         <v>1</v>
@@ -5485,12 +5564,35 @@
     </row>
     <row r="7" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="I7"/>
-      <c r="J7" s="19">
-        <f>SUBTOTAL(109,TableController[Total Price])</f>
-        <v>58.92</v>
+        <v>359</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+      <c r="I7" s="18">
+        <v>2.52</v>
+      </c>
+      <c r="J7" s="18">
+        <f>TableController[[#This Row],[Unit Price]]*TableController[[#This Row],[Quantity]]</f>
+        <v>2.52</v>
       </c>
       <c r="K7"/>
       <c r="L7"/>
@@ -5498,9 +5600,14 @@
       <c r="Q7" s="4"/>
     </row>
     <row r="8" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
+      <c r="A8" s="9" t="s">
+        <v>103</v>
+      </c>
       <c r="I8"/>
-      <c r="J8" s="19"/>
+      <c r="J8" s="18">
+        <f>SUBTOTAL(109,TableController[Total Price])</f>
+        <v>61.440000000000005</v>
+      </c>
       <c r="K8"/>
       <c r="L8"/>
       <c r="P8" s="4"/>
@@ -5509,7 +5616,7 @@
     <row r="9" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9"/>
       <c r="B9" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C9"/>
       <c r="D9"/>
@@ -5576,7 +5683,7 @@
     </row>
     <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5608,16 +5715,16 @@
     <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="H15" s="1">
         <v>1</v>
@@ -5724,7 +5831,7 @@
           <x14:formula1>
             <xm:f>Helper!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C6</xm:sqref>
+          <xm:sqref>C2:C8</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5745,22 +5852,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating schematics for spooling machine.
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajohnson\GIT_Projects\ValpoFilamentRecycler09\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C538A9B1-817F-451B-BE73-C5F8938FF15D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A27E386-FDDF-4C7C-8A33-D0228281F7EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-165" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Extruder" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="383">
   <si>
     <t>Quantity</t>
   </si>
@@ -1177,6 +1178,12 @@
   </si>
   <si>
     <t>Wire</t>
+  </si>
+  <si>
+    <t>Gearbox Machine Key</t>
+  </si>
+  <si>
+    <t>OBSOLETE:</t>
   </si>
 </sst>
 </file>
@@ -1237,7 +1244,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -1262,6 +1269,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -2235,8 +2245,8 @@
   </sheetPr>
   <dimension ref="A1:R69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2528,7 +2538,7 @@
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>285</v>
+        <v>381</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>212</v>
@@ -4347,8 +4357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC497086-9290-4C1D-9300-28557D6CEBE4}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5099,7 +5109,9 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1"/>
+      <c r="A27" s="22" t="s">
+        <v>382</v>
+      </c>
       <c r="B27" s="1" t="s">
         <v>193</v>
       </c>

</xml_diff>

<commit_message>
Added enclosure manufacturer info.
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajohnson\GIT_Projects\ValpoFilamentRecycler09\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamj\Git Projects\ValpoFilamentRecycler09\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126EDACF-F3F4-4DAE-8A4A-EC14E5B00524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49ACDB76-AFF9-44E1-ADE8-408BA977D38D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Extruder" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="383">
   <si>
     <t>Quantity</t>
   </si>
@@ -1178,6 +1178,12 @@
   </si>
   <si>
     <t>C2 Fab LLC</t>
+  </si>
+  <si>
+    <t>Hoffman Enclosures</t>
+  </si>
+  <si>
+    <t>AHE12X12X6</t>
   </si>
 </sst>
 </file>
@@ -1443,20 +1449,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1834,6 +1826,20 @@
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1853,14 +1859,14 @@
   <tableColumns count="10">
     <tableColumn id="12" xr3:uid="{C633C4DA-E9F1-49FB-8240-86247B964FE1}" name="Part" totalsRowDxfId="9"/>
     <tableColumn id="2" xr3:uid="{DAB1913A-18D2-4D9A-9708-032A60B6BC64}" name="Description" totalsRowDxfId="8" dataCellStyle="Normal"/>
-    <tableColumn id="1" xr3:uid="{F1A65BEB-7A95-468E-8FAE-B504744FDB1B}" name="Preference" dataDxfId="12" totalsRowDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{F1A65BEB-7A95-468E-8FAE-B504744FDB1B}" name="Preference" dataDxfId="29" totalsRowDxfId="7"/>
     <tableColumn id="7" xr3:uid="{EC3749CD-9468-4676-8AAA-2DE4FA028800}" name="Supplier" totalsRowDxfId="6" dataCellStyle="Normal"/>
     <tableColumn id="3" xr3:uid="{FBFB3CD0-7BF1-4266-8755-35F85270404A}" name="Supplier Part Number" totalsRowLabel="Total" totalsRowDxfId="5" dataCellStyle="Normal"/>
     <tableColumn id="8" xr3:uid="{70763CA8-03EB-4064-9534-D2C0729DD10E}" name="Manufactuer" totalsRowDxfId="4" dataCellStyle="Normal"/>
     <tableColumn id="9" xr3:uid="{9D792AB2-8329-471D-9251-7B5C39551B6D}" name="Manufacturer Part Number" totalsRowDxfId="3"/>
     <tableColumn id="4" xr3:uid="{6C81D9F0-6082-4928-8091-DA45D848F33F}" name="Quantity" totalsRowDxfId="2" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{D2BF7368-0F05-4426-9AF7-A4A54F97F689}" name="Unit Price" dataDxfId="11" totalsRowDxfId="1" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{816B8560-23EB-4218-8B09-04C10060E74B}" name="Total Price" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="0" dataCellStyle="Currency">
+    <tableColumn id="5" xr3:uid="{D2BF7368-0F05-4426-9AF7-A4A54F97F689}" name="Unit Price" dataDxfId="28" totalsRowDxfId="1" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{816B8560-23EB-4218-8B09-04C10060E74B}" name="Total Price" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="0" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1872,16 +1878,16 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9548DB7C-B8C9-46D9-9175-857AA71A03C3}" name="TableSpooler" displayName="TableSpooler" ref="A1:J25" totalsRowCount="1" dataCellStyle="Normal">
   <autoFilter ref="A1:J24" xr:uid="{9548DB7C-B8C9-46D9-9175-857AA71A03C3}"/>
   <tableColumns count="10">
-    <tableColumn id="12" xr3:uid="{02FE56AC-0EFC-42AA-8A79-A19D1265C334}" name="Part" totalsRowDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{6C7F5790-A2D7-49D5-98CC-5347EEBCB1ED}" name="Description" totalsRowDxfId="28" dataCellStyle="Normal"/>
-    <tableColumn id="1" xr3:uid="{76A9DB35-CA2E-42DE-8502-AF8BEE0A03C6}" name="Preference" totalsRowDxfId="27"/>
-    <tableColumn id="7" xr3:uid="{FF40B9DA-8160-42B4-A04B-59C3988A3C5E}" name="Supplier" totalsRowDxfId="26" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{66B504B5-4CA8-4C40-909D-18E9AADA1F9D}" name="Supplier Part Number" totalsRowLabel="Total" totalsRowDxfId="25" dataCellStyle="Normal"/>
-    <tableColumn id="8" xr3:uid="{B1FBFAC4-450D-465B-8926-44EA92A1276B}" name="Manufactuer" totalsRowDxfId="24" dataCellStyle="Normal"/>
-    <tableColumn id="9" xr3:uid="{42F90968-E8D4-4DE3-8E2B-F702BB9EC99B}" name="Manufacturer Part Number" totalsRowDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{E176CC47-E8BA-4A8D-9C82-D7F685B8FC85}" name="Quantity" totalsRowDxfId="22" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{CECFF550-A5B4-494E-8824-FFDC20FE1F96}" name="Unit Price" dataDxfId="21" totalsRowDxfId="20" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{5C811821-7EC0-4CCE-ABD1-E409C90F00A8}" name="Total Price" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="18" dataCellStyle="Currency">
+    <tableColumn id="12" xr3:uid="{02FE56AC-0EFC-42AA-8A79-A19D1265C334}" name="Part" totalsRowDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{6C7F5790-A2D7-49D5-98CC-5347EEBCB1ED}" name="Description" totalsRowDxfId="25" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{76A9DB35-CA2E-42DE-8502-AF8BEE0A03C6}" name="Preference" totalsRowDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{FF40B9DA-8160-42B4-A04B-59C3988A3C5E}" name="Supplier" totalsRowDxfId="23" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{66B504B5-4CA8-4C40-909D-18E9AADA1F9D}" name="Supplier Part Number" totalsRowLabel="Total" totalsRowDxfId="22" dataCellStyle="Normal"/>
+    <tableColumn id="8" xr3:uid="{B1FBFAC4-450D-465B-8926-44EA92A1276B}" name="Manufactuer" totalsRowDxfId="21" dataCellStyle="Normal"/>
+    <tableColumn id="9" xr3:uid="{42F90968-E8D4-4DE3-8E2B-F702BB9EC99B}" name="Manufacturer Part Number" totalsRowDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{E176CC47-E8BA-4A8D-9C82-D7F685B8FC85}" name="Quantity" totalsRowDxfId="19" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{CECFF550-A5B4-494E-8824-FFDC20FE1F96}" name="Unit Price" dataDxfId="18" totalsRowDxfId="17" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{5C811821-7EC0-4CCE-ABD1-E409C90F00A8}" name="Total Price" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="15" dataCellStyle="Currency">
       <calculatedColumnFormula>TableSpooler[[#This Row],[Quantity]]*TableSpooler[[#This Row],[Unit Price]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1893,7 +1899,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{463B6967-B750-4F73-A588-9468E22D51C2}" name="TableController" displayName="TableController" ref="A1:J8" totalsRowCount="1">
   <autoFilter ref="A1:J7" xr:uid="{463B6967-B750-4F73-A588-9468E22D51C2}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{CC3FED35-0EF5-4A38-A244-2A16695FE8EF}" name="Part" totalsRowLabel="Total" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{CC3FED35-0EF5-4A38-A244-2A16695FE8EF}" name="Part" totalsRowLabel="Total" dataDxfId="14" totalsRowDxfId="13"/>
     <tableColumn id="2" xr3:uid="{1873956F-859F-45C7-922E-A53ECC0CA3FD}" name="Description"/>
     <tableColumn id="10" xr3:uid="{4A3A649F-92F0-4C18-81CA-5B9D728DF405}" name="Preference"/>
     <tableColumn id="3" xr3:uid="{9697BE2D-FF87-4863-A96E-7898B6D0C8A9}" name="Supplier"/>
@@ -1901,8 +1907,8 @@
     <tableColumn id="5" xr3:uid="{E99B851A-67A7-490F-8E43-FCDDABF1F182}" name="Manufactuer"/>
     <tableColumn id="6" xr3:uid="{667ECAC5-D1EB-455C-B5F6-C393586B5D5F}" name="Manufacturer Part Number"/>
     <tableColumn id="7" xr3:uid="{DE0B06EE-7D26-4607-A86C-770AACE90A28}" name="Quantity"/>
-    <tableColumn id="8" xr3:uid="{40503977-B40C-4B6F-9DEA-6C725C85FC01}" name="Unit Price" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{15925615-B9B9-4B30-90D7-656911F22DE7}" name="Total Price" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="13">
+    <tableColumn id="8" xr3:uid="{40503977-B40C-4B6F-9DEA-6C725C85FC01}" name="Unit Price" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{15925615-B9B9-4B30-90D7-656911F22DE7}" name="Total Price" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10">
       <calculatedColumnFormula>TableController[[#This Row],[Unit Price]]*TableController[[#This Row],[Quantity]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2123,28 +2129,28 @@
   </sheetPr>
   <dimension ref="A1:R68"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="90" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="15" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="15" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>275</v>
       </c>
@@ -2178,7 +2184,7 @@
       <c r="Q1"/>
       <c r="R1"/>
     </row>
-    <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>378</v>
       </c>
@@ -2202,7 +2208,7 @@
       <c r="Q2"/>
       <c r="R2"/>
     </row>
-    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>211</v>
       </c>
@@ -2234,7 +2240,7 @@
       <c r="Q3"/>
       <c r="R3"/>
     </row>
-    <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>289</v>
       </c>
@@ -2266,7 +2272,7 @@
       <c r="Q4"/>
       <c r="R4"/>
     </row>
-    <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>288</v>
       </c>
@@ -2298,7 +2304,7 @@
       <c r="Q5"/>
       <c r="R5"/>
     </row>
-    <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>283</v>
       </c>
@@ -2330,7 +2336,7 @@
       <c r="Q6"/>
       <c r="R6"/>
     </row>
-    <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>285</v>
       </c>
@@ -2357,7 +2363,7 @@
       <c r="Q7"/>
       <c r="R7"/>
     </row>
-    <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>284</v>
       </c>
@@ -2386,7 +2392,7 @@
       <c r="Q8"/>
       <c r="R8"/>
     </row>
-    <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>376</v>
       </c>
@@ -2415,7 +2421,7 @@
       <c r="Q9"/>
       <c r="R9"/>
     </row>
-    <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>278</v>
       </c>
@@ -2444,7 +2450,7 @@
       <c r="Q10"/>
       <c r="R10"/>
     </row>
-    <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>279</v>
       </c>
@@ -2473,7 +2479,7 @@
       <c r="Q11"/>
       <c r="R11"/>
     </row>
-    <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>280</v>
       </c>
@@ -2502,7 +2508,7 @@
       <c r="Q12"/>
       <c r="R12"/>
     </row>
-    <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>321</v>
       </c>
@@ -2531,7 +2537,7 @@
       <c r="Q13"/>
       <c r="R13"/>
     </row>
-    <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>322</v>
       </c>
@@ -2560,7 +2566,7 @@
       <c r="Q14"/>
       <c r="R14"/>
     </row>
-    <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>277</v>
       </c>
@@ -2589,7 +2595,7 @@
       <c r="Q15"/>
       <c r="R15"/>
     </row>
-    <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>276</v>
       </c>
@@ -2618,7 +2624,7 @@
       <c r="Q16"/>
       <c r="R16"/>
     </row>
-    <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>295</v>
       </c>
@@ -2647,7 +2653,7 @@
       <c r="Q17"/>
       <c r="R17"/>
     </row>
-    <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>294</v>
       </c>
@@ -2676,7 +2682,7 @@
       <c r="Q18"/>
       <c r="R18"/>
     </row>
-    <row r="19" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>297</v>
       </c>
@@ -2705,7 +2711,7 @@
       <c r="Q19"/>
       <c r="R19"/>
     </row>
-    <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>298</v>
       </c>
@@ -2720,6 +2726,12 @@
       </c>
       <c r="E20" t="s">
         <v>81</v>
+      </c>
+      <c r="F20" t="s">
+        <v>381</v>
+      </c>
+      <c r="G20" t="s">
+        <v>382</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2734,7 +2746,7 @@
       <c r="Q20"/>
       <c r="R20"/>
     </row>
-    <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>204</v>
       </c>
@@ -2769,7 +2781,7 @@
       <c r="Q21"/>
       <c r="R21"/>
     </row>
-    <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>290</v>
       </c>
@@ -2801,7 +2813,7 @@
       <c r="Q22"/>
       <c r="R22"/>
     </row>
-    <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>293</v>
       </c>
@@ -2836,7 +2848,7 @@
       <c r="Q23"/>
       <c r="R23"/>
     </row>
-    <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>296</v>
       </c>
@@ -2871,7 +2883,7 @@
       <c r="Q24"/>
       <c r="R24"/>
     </row>
-    <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>300</v>
       </c>
@@ -2906,7 +2918,7 @@
       <c r="Q25"/>
       <c r="R25"/>
     </row>
-    <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>292</v>
       </c>
@@ -2941,7 +2953,7 @@
       <c r="Q26"/>
       <c r="R26"/>
     </row>
-    <row r="27" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>306</v>
       </c>
@@ -2973,7 +2985,7 @@
       <c r="Q27"/>
       <c r="R27"/>
     </row>
-    <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>306</v>
       </c>
@@ -3008,7 +3020,7 @@
       <c r="Q28"/>
       <c r="R28"/>
     </row>
-    <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>307</v>
       </c>
@@ -3040,7 +3052,7 @@
       <c r="Q29"/>
       <c r="R29"/>
     </row>
-    <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>307</v>
       </c>
@@ -3075,7 +3087,7 @@
       <c r="Q30"/>
       <c r="R30"/>
     </row>
-    <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>208</v>
       </c>
@@ -3104,7 +3116,7 @@
       <c r="Q31"/>
       <c r="R31"/>
     </row>
-    <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>328</v>
       </c>
@@ -3133,7 +3145,7 @@
       <c r="Q32"/>
       <c r="R32"/>
     </row>
-    <row r="33" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>207</v>
       </c>
@@ -3162,7 +3174,7 @@
       <c r="Q33"/>
       <c r="R33"/>
     </row>
-    <row r="34" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>327</v>
       </c>
@@ -3191,7 +3203,7 @@
       <c r="Q34"/>
       <c r="R34"/>
     </row>
-    <row r="35" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>287</v>
       </c>
@@ -3226,7 +3238,7 @@
       <c r="P35" s="2"/>
       <c r="R35"/>
     </row>
-    <row r="36" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>286</v>
       </c>
@@ -3255,7 +3267,7 @@
       <c r="P36" s="2"/>
       <c r="R36"/>
     </row>
-    <row r="37" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>299</v>
       </c>
@@ -3290,7 +3302,7 @@
       <c r="Q37"/>
       <c r="R37"/>
     </row>
-    <row r="38" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>303</v>
       </c>
@@ -3319,7 +3331,7 @@
       <c r="P38" s="2"/>
       <c r="R38"/>
     </row>
-    <row r="39" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>301</v>
       </c>
@@ -3354,7 +3366,7 @@
       <c r="Q39"/>
       <c r="R39"/>
     </row>
-    <row r="40" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>313</v>
       </c>
@@ -3389,7 +3401,7 @@
       <c r="P40" s="2"/>
       <c r="R40"/>
     </row>
-    <row r="41" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>291</v>
       </c>
@@ -3418,7 +3430,7 @@
       <c r="Q41"/>
       <c r="R41"/>
     </row>
-    <row r="42" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>291</v>
       </c>
@@ -3453,7 +3465,7 @@
       <c r="Q42"/>
       <c r="R42"/>
     </row>
-    <row r="43" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>290</v>
       </c>
@@ -3488,7 +3500,7 @@
       <c r="Q43"/>
       <c r="R43"/>
     </row>
-    <row r="44" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>339</v>
       </c>
@@ -3523,7 +3535,7 @@
       <c r="Q44"/>
       <c r="R44"/>
     </row>
-    <row r="45" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>340</v>
       </c>
@@ -3558,7 +3570,7 @@
       <c r="Q45"/>
       <c r="R45"/>
     </row>
-    <row r="46" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>341</v>
       </c>
@@ -3593,7 +3605,7 @@
       <c r="Q46"/>
       <c r="R46"/>
     </row>
-    <row r="47" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>304</v>
       </c>
@@ -3628,7 +3640,7 @@
       <c r="Q47"/>
       <c r="R47"/>
     </row>
-    <row r="48" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>304</v>
       </c>
@@ -3657,7 +3669,7 @@
       <c r="Q48"/>
       <c r="R48"/>
     </row>
-    <row r="49" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>281</v>
       </c>
@@ -3692,7 +3704,7 @@
       <c r="Q49"/>
       <c r="R49"/>
     </row>
-    <row r="50" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
       <c r="C50" t="s">
         <v>270</v>
@@ -3711,7 +3723,7 @@
       <c r="P50" s="2"/>
       <c r="R50"/>
     </row>
-    <row r="51" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
@@ -3730,7 +3742,7 @@
       <c r="P51" s="2"/>
       <c r="R51"/>
     </row>
-    <row r="52" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="B52" s="5" t="s">
         <v>282</v>
@@ -3746,7 +3758,7 @@
       <c r="P52" s="2"/>
       <c r="R52"/>
     </row>
-    <row r="53" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="B53" s="5" t="s">
         <v>302</v>
@@ -3760,7 +3772,7 @@
       <c r="I53" s="5"/>
       <c r="J53" s="6"/>
     </row>
-    <row r="54" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
@@ -3772,14 +3784,14 @@
       <c r="I54" s="5"/>
       <c r="J54" s="6"/>
     </row>
-    <row r="55" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>261</v>
       </c>
       <c r="P55" s="2"/>
       <c r="R55"/>
     </row>
-    <row r="56" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>79</v>
       </c>
@@ -3798,7 +3810,7 @@
       <c r="P56" s="2"/>
       <c r="R56"/>
     </row>
-    <row r="57" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>108</v>
       </c>
@@ -3817,7 +3829,7 @@
       <c r="P57" s="2"/>
       <c r="R57"/>
     </row>
-    <row r="58" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>257</v>
       </c>
@@ -3842,18 +3854,18 @@
       <c r="P58" s="2"/>
       <c r="R58"/>
     </row>
-    <row r="59" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P59" s="2"/>
       <c r="R59"/>
     </row>
-    <row r="60" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>258</v>
       </c>
       <c r="P60" s="2"/>
       <c r="R60"/>
     </row>
-    <row r="61" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>118</v>
       </c>
@@ -3878,18 +3890,18 @@
       <c r="P61" s="2"/>
       <c r="R61"/>
     </row>
-    <row r="62" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P62" s="2"/>
       <c r="R62"/>
     </row>
-    <row r="63" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>254</v>
       </c>
       <c r="P63" s="2"/>
       <c r="R63"/>
     </row>
-    <row r="64" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>232</v>
       </c>
@@ -3912,12 +3924,12 @@
         <v>410</v>
       </c>
     </row>
-    <row r="66" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="67" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>268</v>
       </c>
@@ -3934,7 +3946,7 @@
         <v>19.32</v>
       </c>
     </row>
-    <row r="68" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>309</v>
       </c>
@@ -4002,21 +4014,21 @@
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="96.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="96.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>275</v>
       </c>
@@ -4048,7 +4060,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>212</v>
       </c>
@@ -4078,7 +4090,7 @@
         <v>96.1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>213</v>
       </c>
@@ -4108,7 +4120,7 @@
         <v>26.54</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>214</v>
       </c>
@@ -4135,7 +4147,7 @@
         <v>44.45</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>359</v>
       </c>
@@ -4165,7 +4177,7 @@
         <v>16.18</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>360</v>
       </c>
@@ -4195,7 +4207,7 @@
         <v>5.04</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>361</v>
       </c>
@@ -4219,7 +4231,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>362</v>
       </c>
@@ -4249,7 +4261,7 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>363</v>
       </c>
@@ -4268,7 +4280,7 @@
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>350</v>
       </c>
@@ -4298,7 +4310,7 @@
         <v>19.25</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>349</v>
       </c>
@@ -4323,7 +4335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>364</v>
       </c>
@@ -4353,7 +4365,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>365</v>
       </c>
@@ -4383,7 +4395,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>366</v>
       </c>
@@ -4413,7 +4425,7 @@
         <v>2.5499999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>367</v>
       </c>
@@ -4443,7 +4455,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>368</v>
       </c>
@@ -4473,7 +4485,7 @@
         <v>0.70000000000000007</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>369</v>
       </c>
@@ -4503,7 +4515,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>370</v>
       </c>
@@ -4533,7 +4545,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>371</v>
       </c>
@@ -4563,7 +4575,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>372</v>
       </c>
@@ -4593,7 +4605,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>373</v>
       </c>
@@ -4623,7 +4635,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>374</v>
       </c>
@@ -4653,7 +4665,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>375</v>
       </c>
@@ -4677,7 +4689,7 @@
         <v>14.99</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>338</v>
       </c>
@@ -4698,7 +4710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -4715,12 +4727,12 @@
         <v>272.25999999999993</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>377</v>
       </c>
@@ -4746,12 +4758,12 @@
         <v>6.97</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>110</v>
       </c>
@@ -4774,7 +4786,7 @@
         <v>22.51</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>103</v>
       </c>
@@ -4791,7 +4803,7 @@
         <v>32.1</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>253</v>
       </c>
@@ -4814,12 +4826,12 @@
         <v>24.95</v>
       </c>
     </row>
-    <row r="34" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="35" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>199</v>
       </c>
@@ -4842,12 +4854,12 @@
         <v>17.39</v>
       </c>
     </row>
-    <row r="37" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="38" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>203</v>
       </c>
@@ -4870,7 +4882,7 @@
         <v>13.88</v>
       </c>
     </row>
-    <row r="39" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>133</v>
       </c>
@@ -4923,25 +4935,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA7CB6E4-B302-45F6-B44D-AC8D3E41427A}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>275</v>
       </c>
@@ -4973,7 +4985,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" t="s">
         <v>129</v>
@@ -5004,7 +5016,7 @@
         <v>19.899999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>159</v>
       </c>
@@ -5034,7 +5046,7 @@
         <v>19.899999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>120</v>
       </c>
@@ -5061,7 +5073,7 @@
         <v>5.6499999999999995</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" t="s">
         <v>139</v>
@@ -5089,7 +5101,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5" t="s">
         <v>239</v>
@@ -5115,7 +5127,7 @@
         <v>10.95</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>354</v>
       </c>
@@ -5150,7 +5162,7 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
     </row>
-    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>100</v>
       </c>
@@ -5161,14 +5173,14 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>256</v>
       </c>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
     </row>
-    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>194</v>
       </c>
@@ -5191,7 +5203,7 @@
         <v>4.13</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>141</v>
       </c>
@@ -5214,12 +5226,12 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>119</v>
       </c>
@@ -5242,7 +5254,7 @@
         <v>38.5</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>243</v>
       </c>
@@ -5259,7 +5271,7 @@
         <v>2.95</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>156</v>
       </c>
@@ -5282,7 +5294,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>162</v>
       </c>
@@ -5343,27 +5355,27 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>271</v>
       </c>

</xml_diff>

<commit_message>
Unsure...it's been a while.
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamj\Git Projects\ValpoFilamentRecycler09\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49ACDB76-AFF9-44E1-ADE8-408BA977D38D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF82AC9-BA73-4629-B837-BCC3CB1BE4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="359">
   <si>
     <t>Quantity</t>
   </si>
@@ -49,18 +49,9 @@
     <t>Manufactuer</t>
   </si>
   <si>
-    <t xml:space="preserve">BCZAMD 3D Printer Heating Controller MKS MOSFET MOS </t>
-  </si>
-  <si>
-    <t>AiUS Mos Red</t>
-  </si>
-  <si>
     <t>Amazon</t>
   </si>
   <si>
-    <t>BCZAMD</t>
-  </si>
-  <si>
     <t>DITR-0055</t>
   </si>
   <si>
@@ -157,12 +148,6 @@
     <t>2183-4685-ND</t>
   </si>
   <si>
-    <t>1655-2316-1-ND</t>
-  </si>
-  <si>
-    <t>SMC Diode Solutions</t>
-  </si>
-  <si>
     <t>1050-1024-ND</t>
   </si>
   <si>
@@ -226,12 +211,6 @@
     <t>Sullins Connector Solutions</t>
   </si>
   <si>
-    <t>1N5337BRLGOSCT-ND</t>
-  </si>
-  <si>
-    <t>On Semiconductor</t>
-  </si>
-  <si>
     <t>Dwyer</t>
   </si>
   <si>
@@ -289,12 +268,6 @@
     <t>85385T22</t>
   </si>
   <si>
-    <t>6-Point Standard Socket, 1/2" Square Drive, 12mm Size</t>
-  </si>
-  <si>
-    <t>7149A54</t>
-  </si>
-  <si>
     <t>47065T521</t>
   </si>
   <si>
@@ -385,9 +358,6 @@
     <t>High Torque Set Screw Flexible Shaft Coupling - Stainless Steel Hub</t>
   </si>
   <si>
-    <t>5549A13</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -400,9 +370,6 @@
     <t>Pushbutton, SPST, Normally Open, 0.1A, 32V</t>
   </si>
   <si>
-    <t>6-Point Impact Socket, Standard, 1/2" Square Drive, 1/2" Size, 1-1/2" Long</t>
-  </si>
-  <si>
     <t>Total Price</t>
   </si>
   <si>
@@ -478,12 +445,6 @@
     <t>Panasonic</t>
   </si>
   <si>
-    <t>SB2060TA</t>
-  </si>
-  <si>
-    <t>Diode Schottky, 60V, 20A, Through Hole, DO-201AD</t>
-  </si>
-  <si>
     <t>A000066</t>
   </si>
   <si>
@@ -526,12 +487,6 @@
     <t>RJ45 (Ethernet) Cable, Unshielded, 3.00' (914.4mm)</t>
   </si>
   <si>
-    <t>1N5337BRLG</t>
-  </si>
-  <si>
-    <t>Zener Diode, 4.7V, 5W, ±5%, Through Hole, Axial</t>
-  </si>
-  <si>
     <t>AK67421-2</t>
   </si>
   <si>
@@ -673,9 +628,6 @@
     <t>Nozzle</t>
   </si>
   <si>
-    <t>Fixture</t>
-  </si>
-  <si>
     <t>Fan</t>
   </si>
   <si>
@@ -880,12 +832,6 @@
     <t>Coupler Cover</t>
   </si>
   <si>
-    <t>**</t>
-  </si>
-  <si>
-    <t>** Unsure what this is for.</t>
-  </si>
-  <si>
     <t>Hopper Wall</t>
   </si>
   <si>
@@ -913,12 +859,6 @@
     <t>Motor Driver, Capacitor</t>
   </si>
   <si>
-    <t>Heater, Relay</t>
-  </si>
-  <si>
-    <t>Motor Diode</t>
-  </si>
-  <si>
     <t>Nozzle Heater</t>
   </si>
   <si>
@@ -940,12 +880,6 @@
     <t>Temperature Controller</t>
   </si>
   <si>
-    <t>Motor Driver***</t>
-  </si>
-  <si>
-    <t>*** Requires capacitor and current-limiting resistor, also listed in this table.</t>
-  </si>
-  <si>
     <t>12V Power Supply</t>
   </si>
   <si>
@@ -1000,12 +934,6 @@
     <t>Electrolytic Capacitor, 330uF, 35V, Radial (for Pololu Motor Driver)</t>
   </si>
   <si>
-    <t>Coupler Socket*</t>
-  </si>
-  <si>
-    <t>Screw Socket*</t>
-  </si>
-  <si>
     <t>206060-1</t>
   </si>
   <si>
@@ -1096,9 +1024,6 @@
     <t>N-Channel Power MOSFET, 60V, 17A, Through Hole, TO-220 (for 5V DC motors)</t>
   </si>
   <si>
-    <t>1N5819</t>
-  </si>
-  <si>
     <t>DC/DC Converter</t>
   </si>
   <si>
@@ -1184,6 +1109,9 @@
   </si>
   <si>
     <t>AHE12X12X6</t>
+  </si>
+  <si>
+    <t>Solid State Relay</t>
   </si>
 </sst>
 </file>
@@ -1244,7 +1172,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1263,12 +1191,210 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="30">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1525,320 +1651,10 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1854,19 +1670,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6961DE25-1017-49FB-B58C-151DD971B349}" name="TableExtruder" displayName="TableExtruder" ref="A1:J51" totalsRowCount="1" dataCellStyle="Normal">
-  <autoFilter ref="A1:J50" xr:uid="{6961DE25-1017-49FB-B58C-151DD971B349}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6961DE25-1017-49FB-B58C-151DD971B349}" name="TableExtruder" displayName="TableExtruder" ref="A1:J47" totalsRowCount="1" dataCellStyle="Normal">
+  <autoFilter ref="A1:J46" xr:uid="{6961DE25-1017-49FB-B58C-151DD971B349}"/>
   <tableColumns count="10">
     <tableColumn id="12" xr3:uid="{C633C4DA-E9F1-49FB-8240-86247B964FE1}" name="Part" totalsRowDxfId="9"/>
     <tableColumn id="2" xr3:uid="{DAB1913A-18D2-4D9A-9708-032A60B6BC64}" name="Description" totalsRowDxfId="8" dataCellStyle="Normal"/>
-    <tableColumn id="1" xr3:uid="{F1A65BEB-7A95-468E-8FAE-B504744FDB1B}" name="Preference" dataDxfId="29" totalsRowDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{F1A65BEB-7A95-468E-8FAE-B504744FDB1B}" name="Preference" dataDxfId="12" totalsRowDxfId="7"/>
     <tableColumn id="7" xr3:uid="{EC3749CD-9468-4676-8AAA-2DE4FA028800}" name="Supplier" totalsRowDxfId="6" dataCellStyle="Normal"/>
     <tableColumn id="3" xr3:uid="{FBFB3CD0-7BF1-4266-8755-35F85270404A}" name="Supplier Part Number" totalsRowLabel="Total" totalsRowDxfId="5" dataCellStyle="Normal"/>
     <tableColumn id="8" xr3:uid="{70763CA8-03EB-4064-9534-D2C0729DD10E}" name="Manufactuer" totalsRowDxfId="4" dataCellStyle="Normal"/>
     <tableColumn id="9" xr3:uid="{9D792AB2-8329-471D-9251-7B5C39551B6D}" name="Manufacturer Part Number" totalsRowDxfId="3"/>
     <tableColumn id="4" xr3:uid="{6C81D9F0-6082-4928-8091-DA45D848F33F}" name="Quantity" totalsRowDxfId="2" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{D2BF7368-0F05-4426-9AF7-A4A54F97F689}" name="Unit Price" dataDxfId="28" totalsRowDxfId="1" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{816B8560-23EB-4218-8B09-04C10060E74B}" name="Total Price" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="0" dataCellStyle="Currency">
+    <tableColumn id="5" xr3:uid="{D2BF7368-0F05-4426-9AF7-A4A54F97F689}" name="Unit Price" dataDxfId="11" totalsRowDxfId="1" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{816B8560-23EB-4218-8B09-04C10060E74B}" name="Total Price" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="0" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1878,16 +1694,16 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9548DB7C-B8C9-46D9-9175-857AA71A03C3}" name="TableSpooler" displayName="TableSpooler" ref="A1:J25" totalsRowCount="1" dataCellStyle="Normal">
   <autoFilter ref="A1:J24" xr:uid="{9548DB7C-B8C9-46D9-9175-857AA71A03C3}"/>
   <tableColumns count="10">
-    <tableColumn id="12" xr3:uid="{02FE56AC-0EFC-42AA-8A79-A19D1265C334}" name="Part" totalsRowDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{6C7F5790-A2D7-49D5-98CC-5347EEBCB1ED}" name="Description" totalsRowDxfId="25" dataCellStyle="Normal"/>
-    <tableColumn id="1" xr3:uid="{76A9DB35-CA2E-42DE-8502-AF8BEE0A03C6}" name="Preference" totalsRowDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{FF40B9DA-8160-42B4-A04B-59C3988A3C5E}" name="Supplier" totalsRowDxfId="23" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{66B504B5-4CA8-4C40-909D-18E9AADA1F9D}" name="Supplier Part Number" totalsRowLabel="Total" totalsRowDxfId="22" dataCellStyle="Normal"/>
-    <tableColumn id="8" xr3:uid="{B1FBFAC4-450D-465B-8926-44EA92A1276B}" name="Manufactuer" totalsRowDxfId="21" dataCellStyle="Normal"/>
-    <tableColumn id="9" xr3:uid="{42F90968-E8D4-4DE3-8E2B-F702BB9EC99B}" name="Manufacturer Part Number" totalsRowDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{E176CC47-E8BA-4A8D-9C82-D7F685B8FC85}" name="Quantity" totalsRowDxfId="19" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{CECFF550-A5B4-494E-8824-FFDC20FE1F96}" name="Unit Price" dataDxfId="18" totalsRowDxfId="17" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{5C811821-7EC0-4CCE-ABD1-E409C90F00A8}" name="Total Price" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="15" dataCellStyle="Currency">
+    <tableColumn id="12" xr3:uid="{02FE56AC-0EFC-42AA-8A79-A19D1265C334}" name="Part" totalsRowDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{6C7F5790-A2D7-49D5-98CC-5347EEBCB1ED}" name="Description" totalsRowDxfId="21" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{76A9DB35-CA2E-42DE-8502-AF8BEE0A03C6}" name="Preference" totalsRowDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{FF40B9DA-8160-42B4-A04B-59C3988A3C5E}" name="Supplier" totalsRowDxfId="19" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{66B504B5-4CA8-4C40-909D-18E9AADA1F9D}" name="Supplier Part Number" totalsRowLabel="Total" totalsRowDxfId="18" dataCellStyle="Normal"/>
+    <tableColumn id="8" xr3:uid="{B1FBFAC4-450D-465B-8926-44EA92A1276B}" name="Manufactuer" totalsRowDxfId="17" dataCellStyle="Normal"/>
+    <tableColumn id="9" xr3:uid="{42F90968-E8D4-4DE3-8E2B-F702BB9EC99B}" name="Manufacturer Part Number" totalsRowDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{E176CC47-E8BA-4A8D-9C82-D7F685B8FC85}" name="Quantity" totalsRowDxfId="15" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{CECFF550-A5B4-494E-8824-FFDC20FE1F96}" name="Unit Price" dataDxfId="29" totalsRowDxfId="14" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{5C811821-7EC0-4CCE-ABD1-E409C90F00A8}" name="Total Price" totalsRowFunction="sum" dataDxfId="28" totalsRowDxfId="13" dataCellStyle="Currency">
       <calculatedColumnFormula>TableSpooler[[#This Row],[Quantity]]*TableSpooler[[#This Row],[Unit Price]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1899,7 +1715,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{463B6967-B750-4F73-A588-9468E22D51C2}" name="TableController" displayName="TableController" ref="A1:J8" totalsRowCount="1">
   <autoFilter ref="A1:J7" xr:uid="{463B6967-B750-4F73-A588-9468E22D51C2}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{CC3FED35-0EF5-4A38-A244-2A16695FE8EF}" name="Part" totalsRowLabel="Total" dataDxfId="14" totalsRowDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{CC3FED35-0EF5-4A38-A244-2A16695FE8EF}" name="Part" totalsRowLabel="Total" dataDxfId="27" totalsRowDxfId="26"/>
     <tableColumn id="2" xr3:uid="{1873956F-859F-45C7-922E-A53ECC0CA3FD}" name="Description"/>
     <tableColumn id="10" xr3:uid="{4A3A649F-92F0-4C18-81CA-5B9D728DF405}" name="Preference"/>
     <tableColumn id="3" xr3:uid="{9697BE2D-FF87-4863-A96E-7898B6D0C8A9}" name="Supplier"/>
@@ -1907,8 +1723,8 @@
     <tableColumn id="5" xr3:uid="{E99B851A-67A7-490F-8E43-FCDDABF1F182}" name="Manufactuer"/>
     <tableColumn id="6" xr3:uid="{667ECAC5-D1EB-455C-B5F6-C393586B5D5F}" name="Manufacturer Part Number"/>
     <tableColumn id="7" xr3:uid="{DE0B06EE-7D26-4607-A86C-770AACE90A28}" name="Quantity"/>
-    <tableColumn id="8" xr3:uid="{40503977-B40C-4B6F-9DEA-6C725C85FC01}" name="Unit Price" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{15925615-B9B9-4B30-90D7-656911F22DE7}" name="Total Price" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10">
+    <tableColumn id="8" xr3:uid="{40503977-B40C-4B6F-9DEA-6C725C85FC01}" name="Unit Price" dataDxfId="25"/>
+    <tableColumn id="9" xr3:uid="{15925615-B9B9-4B30-90D7-656911F22DE7}" name="Total Price" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="23">
       <calculatedColumnFormula>TableController[[#This Row],[Unit Price]]*TableController[[#This Row],[Quantity]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2127,10 +1943,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:R68"/>
+  <dimension ref="A1:R61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="B28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2152,25 +1968,25 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="B1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>272</v>
+        <v>256</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="H1" t="s">
         <v>0</v>
@@ -2179,23 +1995,23 @@
         <v>1</v>
       </c>
       <c r="J1" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="Q1"/>
       <c r="R1"/>
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>378</v>
+        <v>353</v>
       </c>
       <c r="B2" t="s">
-        <v>379</v>
+        <v>354</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="F2" t="s">
-        <v>380</v>
+        <v>355</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -2210,22 +2026,22 @@
     </row>
     <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="B3" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="E3" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F3" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -2242,22 +2058,22 @@
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>289</v>
+        <v>271</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="F4" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -2274,22 +2090,22 @@
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>288</v>
+        <v>270</v>
       </c>
       <c r="B5" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="E5" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="F5" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -2306,22 +2122,22 @@
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>283</v>
+        <v>265</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="D6" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="E6" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="F6" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2338,13 +2154,13 @@
     </row>
     <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>285</v>
+        <v>267</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
@@ -2365,19 +2181,19 @@
     </row>
     <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
       <c r="B8" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="D8" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E8" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -2394,19 +2210,19 @@
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>376</v>
+        <v>351</v>
       </c>
       <c r="B9" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2423,19 +2239,19 @@
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
       <c r="B10" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="D10" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2452,19 +2268,19 @@
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="D11" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -2481,19 +2297,19 @@
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>280</v>
+        <v>264</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="D12" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E12" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2509,1463 +2325,1304 @@
       <c r="R12"/>
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>321</v>
+      <c r="A13" t="s">
+        <v>261</v>
       </c>
       <c r="B13" t="s">
-        <v>84</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>270</v>
+        <v>125</v>
+      </c>
+      <c r="C13" t="s">
+        <v>254</v>
       </c>
       <c r="D13" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="E13" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="H13">
         <v>1</v>
       </c>
-      <c r="I13" s="1">
-        <v>7.41</v>
+      <c r="I13" s="2">
+        <v>15.2</v>
       </c>
       <c r="J13" s="2">
         <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>7.41</v>
+        <v>15.2</v>
       </c>
       <c r="Q13"/>
       <c r="R13"/>
     </row>
     <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>322</v>
+      <c r="A14" t="s">
+        <v>260</v>
       </c>
       <c r="B14" t="s">
-        <v>121</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>270</v>
+        <v>124</v>
+      </c>
+      <c r="C14" t="s">
+        <v>254</v>
       </c>
       <c r="D14" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E14" t="s">
-        <v>116</v>
+        <v>64</v>
       </c>
       <c r="H14">
         <v>1</v>
       </c>
-      <c r="I14" s="1">
-        <v>5.66</v>
+      <c r="I14" s="2">
+        <v>12.64</v>
       </c>
       <c r="J14" s="2">
         <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>5.66</v>
+        <v>12.64</v>
       </c>
       <c r="Q14"/>
       <c r="R14"/>
     </row>
     <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B15" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="C15" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="D15" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E15" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H15">
         <v>1</v>
       </c>
       <c r="I15" s="2">
-        <v>15.2</v>
+        <v>85.02</v>
       </c>
       <c r="J15" s="2">
         <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>15.2</v>
+        <v>85.02</v>
       </c>
       <c r="Q15"/>
       <c r="R15"/>
     </row>
     <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>276</v>
+      <c r="A16" s="5" t="s">
+        <v>274</v>
       </c>
       <c r="B16" t="s">
-        <v>135</v>
-      </c>
-      <c r="C16" t="s">
-        <v>270</v>
+        <v>191</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>254</v>
       </c>
       <c r="D16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" t="s">
-        <v>71</v>
+        <v>4</v>
+      </c>
+      <c r="F16" t="s">
+        <v>312</v>
       </c>
       <c r="H16">
         <v>1</v>
       </c>
-      <c r="I16" s="2">
-        <v>12.64</v>
+      <c r="I16" s="1">
+        <v>12.99</v>
       </c>
       <c r="J16" s="2">
         <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>12.64</v>
+        <v>12.99</v>
       </c>
       <c r="Q16"/>
       <c r="R16"/>
     </row>
     <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>295</v>
+      <c r="A17" s="5" t="s">
+        <v>277</v>
       </c>
       <c r="B17" t="s">
-        <v>134</v>
-      </c>
-      <c r="C17" t="s">
-        <v>270</v>
+        <v>313</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>254</v>
       </c>
       <c r="D17" t="s">
-        <v>69</v>
-      </c>
-      <c r="E17" t="s">
-        <v>70</v>
+        <v>4</v>
+      </c>
+      <c r="F17" t="s">
+        <v>142</v>
       </c>
       <c r="H17">
         <v>1</v>
       </c>
-      <c r="I17" s="2">
-        <v>85.02</v>
+      <c r="I17" s="1">
+        <v>12.49</v>
       </c>
       <c r="J17" s="2">
         <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>85.02</v>
+        <v>12.49</v>
       </c>
       <c r="Q17"/>
       <c r="R17"/>
     </row>
     <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>294</v>
+        <v>278</v>
       </c>
       <c r="B18" t="s">
-        <v>206</v>
+        <v>168</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="D18" t="s">
-        <v>6</v>
+        <v>62</v>
+      </c>
+      <c r="E18" t="s">
+        <v>74</v>
       </c>
       <c r="F18" t="s">
-        <v>336</v>
+        <v>356</v>
+      </c>
+      <c r="G18" t="s">
+        <v>357</v>
       </c>
       <c r="H18">
         <v>1</v>
       </c>
       <c r="I18" s="1">
-        <v>12.99</v>
+        <v>53.76</v>
       </c>
       <c r="J18" s="2">
         <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>12.99</v>
+        <v>53.76</v>
       </c>
       <c r="Q18"/>
       <c r="R18"/>
     </row>
     <row r="19" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>297</v>
+      <c r="A19" t="s">
+        <v>189</v>
       </c>
       <c r="B19" t="s">
-        <v>337</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>270</v>
+        <v>290</v>
+      </c>
+      <c r="C19" t="s">
+        <v>254</v>
       </c>
       <c r="D19" t="s">
-        <v>6</v>
+        <v>185</v>
+      </c>
+      <c r="E19" t="s">
+        <v>59</v>
       </c>
       <c r="F19" t="s">
-        <v>155</v>
+        <v>60</v>
+      </c>
+      <c r="G19">
+        <v>108050</v>
       </c>
       <c r="H19">
         <v>1</v>
       </c>
-      <c r="I19" s="1">
-        <v>12.49</v>
+      <c r="I19" s="2">
+        <v>372</v>
       </c>
       <c r="J19" s="2">
         <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>12.49</v>
+        <v>372</v>
       </c>
       <c r="Q19"/>
       <c r="R19"/>
     </row>
     <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>298</v>
+        <v>276</v>
       </c>
       <c r="B20" t="s">
-        <v>183</v>
+        <v>220</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="D20" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="E20" t="s">
-        <v>81</v>
+        <v>221</v>
       </c>
       <c r="F20" t="s">
-        <v>381</v>
+        <v>58</v>
       </c>
       <c r="G20" t="s">
-        <v>382</v>
+        <v>221</v>
       </c>
       <c r="H20">
-        <v>1</v>
-      </c>
-      <c r="I20" s="1">
-        <v>53.76</v>
+        <v>2</v>
+      </c>
+      <c r="I20" s="8">
+        <v>31.85</v>
       </c>
       <c r="J20" s="2">
         <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>53.76</v>
+        <v>63.7</v>
       </c>
       <c r="Q20"/>
       <c r="R20"/>
     </row>
     <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>204</v>
+        <v>280</v>
       </c>
       <c r="B21" t="s">
-        <v>312</v>
+        <v>121</v>
       </c>
       <c r="C21" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="D21" t="s">
-        <v>200</v>
+        <v>58</v>
       </c>
       <c r="E21" t="s">
-        <v>66</v>
+        <v>120</v>
       </c>
       <c r="F21" t="s">
-        <v>67</v>
-      </c>
-      <c r="G21">
-        <v>108050</v>
+        <v>58</v>
+      </c>
+      <c r="G21" t="s">
+        <v>120</v>
       </c>
       <c r="H21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I21" s="2">
-        <v>372</v>
+        <v>102</v>
       </c>
       <c r="J21" s="2">
         <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>372</v>
+        <v>204</v>
       </c>
       <c r="Q21"/>
       <c r="R21"/>
     </row>
     <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>290</v>
+      <c r="A22" t="s">
+        <v>358</v>
       </c>
       <c r="B22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>271</v>
+        <v>126</v>
+      </c>
+      <c r="C22" t="s">
+        <v>254</v>
       </c>
       <c r="D22" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="E22" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="F22" t="s">
+        <v>135</v>
+      </c>
+      <c r="G22" t="s">
+        <v>103</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="I22" s="2">
+        <v>26.12</v>
+      </c>
+      <c r="J22" s="2">
+        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
+        <v>52.24</v>
+      </c>
+      <c r="Q22"/>
+      <c r="R22"/>
+    </row>
+    <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>284</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="C23" t="s">
+        <v>254</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="I23" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="J23" s="2">
+        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
         <v>7</v>
       </c>
-      <c r="H22">
-        <v>1</v>
-      </c>
-      <c r="I22" s="1">
-        <v>14.99</v>
-      </c>
-      <c r="J22" s="2" t="str">
+      <c r="Q23"/>
+      <c r="R23"/>
+    </row>
+    <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>284</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="C24" t="s">
+        <v>255</v>
+      </c>
+      <c r="D24" t="s">
+        <v>201</v>
+      </c>
+      <c r="E24" t="s">
+        <v>203</v>
+      </c>
+      <c r="F24" t="s">
+        <v>199</v>
+      </c>
+      <c r="G24" t="s">
+        <v>204</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+      <c r="I24" s="2">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="J24" s="2" t="str">
         <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
         <v/>
       </c>
-      <c r="Q22"/>
-      <c r="R22"/>
-    </row>
-    <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="B23" t="s">
-        <v>148</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="D23" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" t="s">
-        <v>40</v>
-      </c>
-      <c r="F23" t="s">
-        <v>41</v>
-      </c>
-      <c r="G23" t="s">
-        <v>147</v>
-      </c>
-      <c r="H23">
-        <v>4</v>
-      </c>
-      <c r="I23" s="2">
-        <v>0.47</v>
-      </c>
-      <c r="J23" s="2">
-        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>1.88</v>
-      </c>
-      <c r="Q23"/>
-      <c r="R23"/>
-    </row>
-    <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="B24" t="s">
-        <v>236</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="D24" t="s">
-        <v>65</v>
-      </c>
-      <c r="E24" t="s">
-        <v>237</v>
-      </c>
-      <c r="F24" t="s">
-        <v>65</v>
-      </c>
-      <c r="G24" t="s">
-        <v>237</v>
-      </c>
-      <c r="H24">
-        <v>2</v>
-      </c>
-      <c r="I24" s="8">
-        <v>31.85</v>
-      </c>
-      <c r="J24" s="2">
-        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>63.7</v>
-      </c>
       <c r="Q24"/>
       <c r="R24"/>
     </row>
     <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>300</v>
-      </c>
-      <c r="B25" t="s">
-        <v>132</v>
+        <v>285</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>297</v>
       </c>
       <c r="C25" t="s">
-        <v>270</v>
-      </c>
-      <c r="D25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E25" t="s">
-        <v>131</v>
-      </c>
-      <c r="F25" t="s">
-        <v>65</v>
-      </c>
-      <c r="G25" t="s">
-        <v>131</v>
+        <v>254</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>295</v>
       </c>
       <c r="H25">
         <v>2</v>
       </c>
-      <c r="I25" s="2">
-        <v>102</v>
+      <c r="I25" s="1">
+        <v>6</v>
       </c>
       <c r="J25" s="2">
         <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>204</v>
+        <v>12</v>
       </c>
       <c r="Q25"/>
       <c r="R25"/>
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>292</v>
-      </c>
-      <c r="B26" t="s">
-        <v>137</v>
+        <v>285</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>297</v>
       </c>
       <c r="C26" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="D26" t="s">
-        <v>27</v>
+        <v>201</v>
       </c>
       <c r="E26" t="s">
-        <v>26</v>
+        <v>202</v>
       </c>
       <c r="F26" t="s">
-        <v>146</v>
+        <v>199</v>
       </c>
       <c r="G26" t="s">
-        <v>112</v>
+        <v>200</v>
       </c>
       <c r="H26">
         <v>2</v>
       </c>
       <c r="I26" s="2">
-        <v>26.12</v>
-      </c>
-      <c r="J26" s="2">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="J26" s="2" t="str">
         <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>52.24</v>
+        <v/>
       </c>
       <c r="Q26"/>
       <c r="R26"/>
     </row>
     <row r="27" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>306</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>318</v>
+        <v>193</v>
+      </c>
+      <c r="B27" t="s">
+        <v>300</v>
       </c>
       <c r="C27" t="s">
-        <v>270</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>315</v>
+        <v>254</v>
+      </c>
+      <c r="F27" t="s">
+        <v>205</v>
+      </c>
+      <c r="G27" t="s">
+        <v>299</v>
       </c>
       <c r="H27">
         <v>2</v>
       </c>
       <c r="I27" s="1">
-        <v>3.5</v>
+        <v>7.33</v>
       </c>
       <c r="J27" s="2">
         <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>7</v>
+        <v>14.66</v>
       </c>
       <c r="Q27"/>
       <c r="R27"/>
     </row>
     <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>304</v>
+      </c>
+      <c r="B28" t="s">
+        <v>307</v>
+      </c>
+      <c r="C28" t="s">
+        <v>254</v>
+      </c>
+      <c r="F28" t="s">
+        <v>205</v>
+      </c>
+      <c r="G28" t="s">
+        <v>308</v>
+      </c>
+      <c r="H28">
+        <v>8</v>
+      </c>
+      <c r="I28" s="1">
+        <v>1.63</v>
+      </c>
+      <c r="J28" s="2">
+        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
+        <v>13.04</v>
+      </c>
+      <c r="Q28"/>
+      <c r="R28"/>
+    </row>
+    <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>192</v>
+      </c>
+      <c r="B29" t="s">
+        <v>301</v>
+      </c>
+      <c r="C29" t="s">
+        <v>254</v>
+      </c>
+      <c r="F29" t="s">
+        <v>205</v>
+      </c>
+      <c r="G29" t="s">
+        <v>302</v>
+      </c>
+      <c r="H29">
+        <v>2</v>
+      </c>
+      <c r="I29" s="1">
+        <v>5.73</v>
+      </c>
+      <c r="J29" s="2">
+        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
+        <v>11.46</v>
+      </c>
+      <c r="Q29"/>
+      <c r="R29"/>
+    </row>
+    <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>303</v>
+      </c>
+      <c r="B30" t="s">
+        <v>305</v>
+      </c>
+      <c r="C30" t="s">
+        <v>254</v>
+      </c>
+      <c r="F30" t="s">
+        <v>205</v>
+      </c>
+      <c r="G30" t="s">
         <v>306</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="H30">
+        <v>8</v>
+      </c>
+      <c r="I30" s="1">
+        <v>1.57</v>
+      </c>
+      <c r="J30" s="2">
+        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
+        <v>12.56</v>
+      </c>
+      <c r="Q30"/>
+      <c r="R30"/>
+    </row>
+    <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>269</v>
+      </c>
+      <c r="B31" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" t="s">
+        <v>254</v>
+      </c>
+      <c r="D31" t="s">
+        <v>89</v>
+      </c>
+      <c r="E31">
+        <v>37769</v>
+      </c>
+      <c r="F31" t="s">
+        <v>90</v>
+      </c>
+      <c r="G31" t="s">
+        <v>171</v>
+      </c>
+      <c r="H31">
+        <v>2</v>
+      </c>
+      <c r="I31" s="2">
+        <v>5.13</v>
+      </c>
+      <c r="J31" s="2">
+        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
+        <v>10.26</v>
+      </c>
+      <c r="P31" s="2"/>
+      <c r="R31"/>
+    </row>
+    <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>268</v>
+      </c>
+      <c r="B32" t="s">
+        <v>214</v>
+      </c>
+      <c r="C32" t="s">
+        <v>254</v>
+      </c>
+      <c r="F32" t="s">
+        <v>215</v>
+      </c>
+      <c r="G32" t="s">
+        <v>253</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32" s="1">
+        <v>808.75</v>
+      </c>
+      <c r="J32" s="2">
+        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
+        <v>808.75</v>
+      </c>
+      <c r="P32" s="2"/>
+      <c r="R32"/>
+    </row>
+    <row r="33" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="B33" t="s">
+        <v>209</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="D33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" t="s">
+        <v>208</v>
+      </c>
+      <c r="F33" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33" s="8">
+        <v>92.94</v>
+      </c>
+      <c r="J33" s="2">
+        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
+        <v>92.94</v>
+      </c>
+      <c r="Q33"/>
+      <c r="R33"/>
+    </row>
+    <row r="34" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>281</v>
+      </c>
+      <c r="B34" t="s">
+        <v>219</v>
+      </c>
+      <c r="C34" t="s">
+        <v>254</v>
+      </c>
+      <c r="F34" t="s">
+        <v>217</v>
+      </c>
+      <c r="G34" t="s">
+        <v>218</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34" s="8">
+        <v>12.98</v>
+      </c>
+      <c r="J34" s="2">
+        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
+        <v>12.98</v>
+      </c>
+      <c r="P34" s="2"/>
+      <c r="R34"/>
+    </row>
+    <row r="35" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>272</v>
+      </c>
+      <c r="B35" t="s">
+        <v>246</v>
+      </c>
+      <c r="C35" t="s">
+        <v>254</v>
+      </c>
+      <c r="D35" t="s">
+        <v>134</v>
+      </c>
+      <c r="E35">
+        <v>2991</v>
+      </c>
+      <c r="F35" t="s">
+        <v>134</v>
+      </c>
+      <c r="G35">
+        <v>2991</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35" s="1">
+        <v>29.95</v>
+      </c>
+      <c r="J35" s="2">
+        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
+        <v>29.95</v>
+      </c>
+      <c r="Q35"/>
+      <c r="R35"/>
+    </row>
+    <row r="36" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>291</v>
+      </c>
+      <c r="B36" t="s">
         <v>318</v>
       </c>
-      <c r="C28" t="s">
-        <v>271</v>
-      </c>
-      <c r="D28" t="s">
-        <v>217</v>
-      </c>
-      <c r="E28" t="s">
-        <v>219</v>
-      </c>
-      <c r="F28" t="s">
-        <v>215</v>
-      </c>
-      <c r="G28" t="s">
-        <v>220</v>
-      </c>
-      <c r="H28">
-        <v>2</v>
-      </c>
-      <c r="I28" s="2">
-        <v>2.4300000000000002</v>
-      </c>
-      <c r="J28" s="2" t="str">
+      <c r="C36" t="s">
+        <v>254</v>
+      </c>
+      <c r="D36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" t="s">
+        <v>319</v>
+      </c>
+      <c r="F36" t="s">
+        <v>320</v>
+      </c>
+      <c r="G36" t="s">
+        <v>321</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J36" s="2">
+        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
+        <v>0.1</v>
+      </c>
+      <c r="P36" s="2"/>
+      <c r="R36"/>
+    </row>
+    <row r="37" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>273</v>
+      </c>
+      <c r="B37" t="s">
+        <v>298</v>
+      </c>
+      <c r="C37" t="s">
+        <v>254</v>
+      </c>
+      <c r="D37" t="s">
+        <v>134</v>
+      </c>
+      <c r="E37">
+        <v>882</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37" s="1">
+        <v>0.49</v>
+      </c>
+      <c r="J37" s="2">
+        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
+        <v>0.49</v>
+      </c>
+      <c r="Q37"/>
+      <c r="R37"/>
+    </row>
+    <row r="38" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>273</v>
+      </c>
+      <c r="B38" t="s">
+        <v>292</v>
+      </c>
+      <c r="C38" t="s">
+        <v>255</v>
+      </c>
+      <c r="D38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" t="s">
+        <v>247</v>
+      </c>
+      <c r="F38" t="s">
+        <v>248</v>
+      </c>
+      <c r="G38" t="s">
+        <v>249</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="J38" s="2" t="str">
         <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
         <v/>
       </c>
-      <c r="Q28"/>
-      <c r="R28"/>
-    </row>
-    <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>307</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="C29" t="s">
-        <v>270</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="H29">
-        <v>2</v>
-      </c>
-      <c r="I29" s="1">
-        <v>6</v>
-      </c>
-      <c r="J29" s="2">
-        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>12</v>
-      </c>
-      <c r="Q29"/>
-      <c r="R29"/>
-    </row>
-    <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>307</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="C30" t="s">
-        <v>271</v>
-      </c>
-      <c r="D30" t="s">
-        <v>217</v>
-      </c>
-      <c r="E30" t="s">
-        <v>218</v>
-      </c>
-      <c r="F30" t="s">
-        <v>215</v>
-      </c>
-      <c r="G30" t="s">
-        <v>216</v>
-      </c>
-      <c r="H30">
-        <v>2</v>
-      </c>
-      <c r="I30" s="2">
-        <v>2.5099999999999998</v>
-      </c>
-      <c r="J30" s="2" t="str">
+      <c r="Q38"/>
+      <c r="R38"/>
+    </row>
+    <row r="39" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>272</v>
+      </c>
+      <c r="B39" t="s">
+        <v>187</v>
+      </c>
+      <c r="C39" t="s">
+        <v>255</v>
+      </c>
+      <c r="D39" t="s">
+        <v>185</v>
+      </c>
+      <c r="E39" t="s">
+        <v>105</v>
+      </c>
+      <c r="F39" t="s">
+        <v>210</v>
+      </c>
+      <c r="G39" t="s">
+        <v>186</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39" s="2">
+        <v>368</v>
+      </c>
+      <c r="J39" s="2" t="str">
         <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
         <v/>
       </c>
-      <c r="Q30"/>
-      <c r="R30"/>
-    </row>
-    <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>208</v>
-      </c>
-      <c r="B31" t="s">
-        <v>324</v>
-      </c>
-      <c r="C31" t="s">
-        <v>270</v>
-      </c>
-      <c r="F31" t="s">
-        <v>221</v>
-      </c>
-      <c r="G31" t="s">
-        <v>323</v>
-      </c>
-      <c r="H31">
-        <v>2</v>
-      </c>
-      <c r="I31" s="1">
-        <v>7.33</v>
-      </c>
-      <c r="J31" s="2">
-        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>14.66</v>
-      </c>
-      <c r="Q31"/>
-      <c r="R31"/>
-    </row>
-    <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>328</v>
-      </c>
-      <c r="B32" t="s">
-        <v>331</v>
-      </c>
-      <c r="C32" t="s">
-        <v>270</v>
-      </c>
-      <c r="F32" t="s">
-        <v>221</v>
-      </c>
-      <c r="G32" t="s">
-        <v>332</v>
-      </c>
-      <c r="H32">
-        <v>8</v>
-      </c>
-      <c r="I32" s="1">
-        <v>1.63</v>
-      </c>
-      <c r="J32" s="2">
-        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>13.04</v>
-      </c>
-      <c r="Q32"/>
-      <c r="R32"/>
-    </row>
-    <row r="33" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>207</v>
-      </c>
-      <c r="B33" t="s">
-        <v>325</v>
-      </c>
-      <c r="C33" t="s">
-        <v>270</v>
-      </c>
-      <c r="F33" t="s">
-        <v>221</v>
-      </c>
-      <c r="G33" t="s">
-        <v>326</v>
-      </c>
-      <c r="H33">
-        <v>2</v>
-      </c>
-      <c r="I33" s="1">
-        <v>5.73</v>
-      </c>
-      <c r="J33" s="2">
-        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>11.46</v>
-      </c>
-      <c r="Q33"/>
-      <c r="R33"/>
-    </row>
-    <row r="34" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>327</v>
-      </c>
-      <c r="B34" t="s">
-        <v>329</v>
-      </c>
-      <c r="C34" t="s">
-        <v>270</v>
-      </c>
-      <c r="F34" t="s">
-        <v>221</v>
-      </c>
-      <c r="G34" t="s">
-        <v>330</v>
-      </c>
-      <c r="H34">
-        <v>8</v>
-      </c>
-      <c r="I34" s="1">
-        <v>1.57</v>
-      </c>
-      <c r="J34" s="2">
-        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>12.56</v>
-      </c>
-      <c r="Q34"/>
-      <c r="R34"/>
-    </row>
-    <row r="35" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>287</v>
-      </c>
-      <c r="B35" t="s">
-        <v>97</v>
-      </c>
-      <c r="C35" t="s">
-        <v>270</v>
-      </c>
-      <c r="D35" t="s">
-        <v>98</v>
-      </c>
-      <c r="E35">
-        <v>37769</v>
-      </c>
-      <c r="F35" t="s">
-        <v>99</v>
-      </c>
-      <c r="G35" t="s">
-        <v>186</v>
-      </c>
-      <c r="H35">
-        <v>2</v>
-      </c>
-      <c r="I35" s="2">
-        <v>5.13</v>
-      </c>
-      <c r="J35" s="2">
-        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>10.26</v>
-      </c>
-      <c r="P35" s="2"/>
-      <c r="R35"/>
-    </row>
-    <row r="36" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>286</v>
-      </c>
-      <c r="B36" t="s">
-        <v>230</v>
-      </c>
-      <c r="C36" t="s">
-        <v>270</v>
-      </c>
-      <c r="F36" t="s">
-        <v>231</v>
-      </c>
-      <c r="G36" t="s">
-        <v>269</v>
-      </c>
-      <c r="H36">
-        <v>1</v>
-      </c>
-      <c r="I36" s="1">
-        <v>808.75</v>
-      </c>
-      <c r="J36" s="2">
-        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>808.75</v>
-      </c>
-      <c r="P36" s="2"/>
-      <c r="R36"/>
-    </row>
-    <row r="37" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="B37" t="s">
-        <v>225</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="D37" t="s">
-        <v>19</v>
-      </c>
-      <c r="E37" t="s">
-        <v>224</v>
-      </c>
-      <c r="F37" t="s">
-        <v>21</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="H37">
-        <v>1</v>
-      </c>
-      <c r="I37" s="8">
-        <v>92.94</v>
-      </c>
-      <c r="J37" s="2">
-        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>92.94</v>
-      </c>
-      <c r="Q37"/>
-      <c r="R37"/>
-    </row>
-    <row r="38" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>303</v>
-      </c>
-      <c r="B38" t="s">
-        <v>235</v>
-      </c>
-      <c r="C38" t="s">
-        <v>270</v>
-      </c>
-      <c r="F38" t="s">
-        <v>233</v>
-      </c>
-      <c r="G38" t="s">
-        <v>234</v>
-      </c>
-      <c r="H38">
-        <v>1</v>
-      </c>
-      <c r="I38" s="8">
-        <v>12.98</v>
-      </c>
-      <c r="J38" s="2">
-        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>12.98</v>
-      </c>
-      <c r="P38" s="2"/>
-      <c r="R38"/>
-    </row>
-    <row r="39" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>301</v>
-      </c>
-      <c r="B39" t="s">
-        <v>262</v>
-      </c>
-      <c r="C39" t="s">
-        <v>270</v>
-      </c>
-      <c r="D39" t="s">
-        <v>145</v>
-      </c>
-      <c r="E39">
-        <v>2991</v>
-      </c>
-      <c r="F39" t="s">
-        <v>145</v>
-      </c>
-      <c r="G39">
-        <v>2991</v>
-      </c>
-      <c r="H39">
-        <v>1</v>
-      </c>
-      <c r="I39" s="1">
-        <v>29.95</v>
-      </c>
-      <c r="J39" s="2">
-        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>29.95</v>
-      </c>
       <c r="Q39"/>
       <c r="R39"/>
     </row>
     <row r="40" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B40" t="s">
-        <v>342</v>
+        <v>229</v>
       </c>
       <c r="C40" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="D40" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E40" t="s">
-        <v>343</v>
+        <v>234</v>
       </c>
       <c r="F40" t="s">
-        <v>344</v>
+        <v>230</v>
       </c>
       <c r="G40" t="s">
-        <v>345</v>
+        <v>231</v>
       </c>
       <c r="H40">
         <v>1</v>
       </c>
       <c r="I40" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="J40" s="2">
+        <v>11.27</v>
+      </c>
+      <c r="J40" s="1">
         <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>0.1</v>
-      </c>
-      <c r="P40" s="2"/>
+        <v>11.27</v>
+      </c>
+      <c r="Q40"/>
       <c r="R40"/>
     </row>
     <row r="41" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>291</v>
+        <v>316</v>
       </c>
       <c r="B41" t="s">
-        <v>320</v>
+        <v>232</v>
       </c>
       <c r="C41" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="D41" t="s">
-        <v>145</v>
-      </c>
-      <c r="E41">
-        <v>882</v>
+        <v>16</v>
+      </c>
+      <c r="E41" t="s">
+        <v>235</v>
+      </c>
+      <c r="F41" t="s">
+        <v>230</v>
+      </c>
+      <c r="G41">
+        <v>4301.1409000000003</v>
       </c>
       <c r="H41">
         <v>1</v>
       </c>
       <c r="I41" s="1">
-        <v>0.49</v>
-      </c>
-      <c r="J41" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="J41" s="1">
         <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>0.49</v>
+        <v>4.7</v>
       </c>
       <c r="Q41"/>
       <c r="R41"/>
     </row>
     <row r="42" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>291</v>
+        <v>317</v>
       </c>
       <c r="B42" t="s">
-        <v>314</v>
+        <v>233</v>
       </c>
       <c r="C42" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="D42" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E42" t="s">
-        <v>263</v>
+        <v>236</v>
       </c>
       <c r="F42" t="s">
-        <v>264</v>
-      </c>
-      <c r="G42" t="s">
-        <v>265</v>
+        <v>230</v>
+      </c>
+      <c r="G42">
+        <v>34.3127</v>
       </c>
       <c r="H42">
         <v>1</v>
       </c>
       <c r="I42" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="J42" s="2" t="str">
+        <v>0.44</v>
+      </c>
+      <c r="J42" s="1">
+        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
+        <v>0.44</v>
+      </c>
+      <c r="Q42"/>
+      <c r="R42"/>
+    </row>
+    <row r="43" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="B43" t="s">
+        <v>311</v>
+      </c>
+      <c r="C43" t="s">
+        <v>254</v>
+      </c>
+      <c r="D43" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" t="s">
+        <v>309</v>
+      </c>
+      <c r="F43" t="s">
+        <v>283</v>
+      </c>
+      <c r="G43" t="s">
+        <v>310</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43" s="1">
+        <v>4.99</v>
+      </c>
+      <c r="J43" s="2">
+        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
+        <v>4.99</v>
+      </c>
+      <c r="Q43"/>
+      <c r="R43"/>
+    </row>
+    <row r="44" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="B44" t="s">
+        <v>311</v>
+      </c>
+      <c r="C44" t="s">
+        <v>255</v>
+      </c>
+      <c r="D44" t="s">
+        <v>92</v>
+      </c>
+      <c r="E44">
+        <v>3311</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44" s="1">
+        <v>5.95</v>
+      </c>
+      <c r="J44" s="1" t="str">
         <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
         <v/>
       </c>
-      <c r="Q42"/>
-      <c r="R42"/>
-    </row>
-    <row r="43" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>290</v>
-      </c>
-      <c r="B43" t="s">
-        <v>202</v>
-      </c>
-      <c r="C43" t="s">
-        <v>271</v>
-      </c>
-      <c r="D43" t="s">
-        <v>200</v>
-      </c>
-      <c r="E43" t="s">
-        <v>114</v>
-      </c>
-      <c r="F43" t="s">
-        <v>226</v>
-      </c>
-      <c r="G43" t="s">
-        <v>201</v>
-      </c>
-      <c r="H43">
-        <v>1</v>
-      </c>
-      <c r="I43" s="2">
-        <v>368</v>
-      </c>
-      <c r="J43" s="2" t="str">
-        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v/>
-      </c>
-      <c r="Q43"/>
-      <c r="R43"/>
-    </row>
-    <row r="44" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>339</v>
-      </c>
-      <c r="B44" t="s">
-        <v>245</v>
-      </c>
-      <c r="C44" t="s">
-        <v>270</v>
-      </c>
-      <c r="D44" t="s">
-        <v>19</v>
-      </c>
-      <c r="E44" t="s">
-        <v>250</v>
-      </c>
-      <c r="F44" t="s">
-        <v>246</v>
-      </c>
-      <c r="G44" t="s">
-        <v>247</v>
-      </c>
-      <c r="H44">
-        <v>1</v>
-      </c>
-      <c r="I44" s="1">
-        <v>11.27</v>
-      </c>
-      <c r="J44" s="1">
-        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>11.27</v>
-      </c>
       <c r="Q44"/>
       <c r="R44"/>
     </row>
     <row r="45" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>340</v>
-      </c>
-      <c r="B45" t="s">
-        <v>248</v>
-      </c>
-      <c r="C45" t="s">
-        <v>270</v>
-      </c>
-      <c r="D45" t="s">
-        <v>19</v>
-      </c>
-      <c r="E45" t="s">
-        <v>251</v>
-      </c>
-      <c r="F45" t="s">
-        <v>246</v>
-      </c>
-      <c r="G45">
-        <v>4301.1409000000003</v>
-      </c>
-      <c r="H45">
-        <v>1</v>
-      </c>
-      <c r="I45" s="1">
-        <v>4.7</v>
-      </c>
-      <c r="J45" s="1">
+      <c r="A45" s="5"/>
+      <c r="B45" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="G45" s="5">
+        <v>181</v>
+      </c>
+      <c r="H45" s="14">
+        <v>2</v>
+      </c>
+      <c r="I45" s="16">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="J45" s="16">
         <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>4.7</v>
-      </c>
-      <c r="Q45"/>
+        <v>19.899999999999999</v>
+      </c>
+      <c r="P45" s="2"/>
       <c r="R45"/>
     </row>
     <row r="46" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>341</v>
-      </c>
-      <c r="B46" t="s">
-        <v>249</v>
-      </c>
-      <c r="C46" t="s">
-        <v>270</v>
-      </c>
-      <c r="D46" t="s">
-        <v>19</v>
-      </c>
-      <c r="E46" t="s">
-        <v>252</v>
-      </c>
-      <c r="F46" t="s">
-        <v>246</v>
-      </c>
-      <c r="G46">
-        <v>34.3127</v>
-      </c>
-      <c r="H46">
-        <v>1</v>
-      </c>
-      <c r="I46" s="1">
-        <v>0.44</v>
-      </c>
-      <c r="J46" s="1">
+      <c r="A46" s="5"/>
+      <c r="B46" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F46" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="G46" s="5">
+        <v>292</v>
+      </c>
+      <c r="H46" s="14">
+        <v>2</v>
+      </c>
+      <c r="I46" s="16">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="J46" s="16">
         <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>0.44</v>
-      </c>
-      <c r="Q46"/>
-      <c r="R46"/>
+        <v>19.899999999999999</v>
+      </c>
     </row>
     <row r="47" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="B47" t="s">
-        <v>335</v>
-      </c>
-      <c r="C47" t="s">
-        <v>270</v>
-      </c>
-      <c r="D47" t="s">
-        <v>19</v>
-      </c>
-      <c r="E47" t="s">
-        <v>333</v>
-      </c>
-      <c r="F47" t="s">
-        <v>305</v>
-      </c>
-      <c r="G47" t="s">
-        <v>334</v>
-      </c>
-      <c r="H47">
-        <v>1</v>
-      </c>
-      <c r="I47" s="1">
-        <v>4.99</v>
-      </c>
-      <c r="J47" s="2">
-        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>4.99</v>
-      </c>
-      <c r="Q47"/>
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="6">
+        <f>SUBTOTAL(109,TableExtruder[Total Price])</f>
+        <v>2248.0899999999997</v>
+      </c>
+      <c r="P47" s="2"/>
       <c r="R47"/>
     </row>
     <row r="48" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>304</v>
-      </c>
       <c r="B48" t="s">
-        <v>335</v>
-      </c>
-      <c r="C48" t="s">
-        <v>271</v>
-      </c>
-      <c r="D48" t="s">
-        <v>101</v>
-      </c>
-      <c r="E48">
-        <v>3311</v>
-      </c>
-      <c r="H48">
-        <v>1</v>
-      </c>
-      <c r="I48" s="1">
-        <v>5.95</v>
-      </c>
-      <c r="J48" s="1" t="str">
-        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v/>
-      </c>
-      <c r="Q48"/>
+        <v>245</v>
+      </c>
+      <c r="P48" s="2"/>
       <c r="R48"/>
     </row>
-    <row r="49" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
-        <v>281</v>
-      </c>
+    <row r="49" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>164</v>
-      </c>
-      <c r="C49" t="s">
-        <v>270</v>
+        <v>72</v>
       </c>
       <c r="D49" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="E49" t="s">
-        <v>63</v>
-      </c>
-      <c r="F49" t="s">
-        <v>64</v>
-      </c>
-      <c r="G49" t="s">
-        <v>163</v>
+        <v>73</v>
       </c>
       <c r="H49">
-        <v>2</v>
-      </c>
-      <c r="I49" s="2">
-        <v>0.51</v>
-      </c>
-      <c r="J49" s="2">
-        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>1.02</v>
-      </c>
-      <c r="Q49"/>
+        <v>1</v>
+      </c>
+      <c r="I49">
+        <v>43.8</v>
+      </c>
+      <c r="P49" s="2"/>
       <c r="R49"/>
     </row>
-    <row r="50" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
-      <c r="C50" t="s">
-        <v>270</v>
-      </c>
-      <c r="G50" t="s">
-        <v>353</v>
+    <row r="50" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>99</v>
+      </c>
+      <c r="D50" t="s">
+        <v>16</v>
+      </c>
+      <c r="E50" t="s">
+        <v>100</v>
       </c>
       <c r="H50">
-        <v>4</v>
-      </c>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1">
-        <f>IF(TableExtruder[[#This Row],[Preference]] &lt;&gt; "Alternate", TableExtruder[[#This Row],[Quantity]]*TableExtruder[[#This Row],[Unit Price]], "")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I50">
+        <v>43.82</v>
       </c>
       <c r="P50" s="2"/>
       <c r="R50"/>
     </row>
-    <row r="51" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
-      <c r="H51" s="5"/>
-      <c r="I51" s="5"/>
-      <c r="J51" s="6">
-        <f>SUBTOTAL(109,TableExtruder[Total Price])</f>
-        <v>2224.2599999999993</v>
+    <row r="51" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>241</v>
+      </c>
+      <c r="D51" t="s">
+        <v>16</v>
+      </c>
+      <c r="E51" t="s">
+        <v>19</v>
+      </c>
+      <c r="F51" t="s">
+        <v>20</v>
+      </c>
+      <c r="G51" t="s">
+        <v>116</v>
+      </c>
+      <c r="H51">
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <v>20.25</v>
       </c>
       <c r="P51" s="2"/>
       <c r="R51"/>
     </row>
-    <row r="52" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
-      <c r="I52" s="5"/>
-      <c r="J52" s="6"/>
+    <row r="52" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P52" s="2"/>
       <c r="R52"/>
     </row>
-    <row r="53" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="5"/>
-      <c r="I53" s="5"/>
-      <c r="J53" s="6"/>
-    </row>
-    <row r="54" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
-      <c r="I54" s="5"/>
-      <c r="J54" s="6"/>
-    </row>
-    <row r="55" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>261</v>
-      </c>
+    <row r="53" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>242</v>
+      </c>
+      <c r="P53" s="2"/>
+      <c r="R53"/>
+    </row>
+    <row r="54" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>108</v>
+      </c>
+      <c r="D54" t="s">
+        <v>16</v>
+      </c>
+      <c r="E54" t="s">
+        <v>15</v>
+      </c>
+      <c r="F54" t="s">
+        <v>17</v>
+      </c>
+      <c r="G54" t="s">
+        <v>115</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>19.54</v>
+      </c>
+      <c r="P54" s="2"/>
+      <c r="R54"/>
+    </row>
+    <row r="55" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P55" s="2"/>
       <c r="R55"/>
     </row>
-    <row r="56" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>79</v>
-      </c>
-      <c r="D56" t="s">
-        <v>69</v>
-      </c>
-      <c r="E56" t="s">
-        <v>80</v>
-      </c>
-      <c r="H56">
-        <v>1</v>
-      </c>
-      <c r="I56">
-        <v>43.8</v>
-      </c>
-      <c r="P56" s="2"/>
-      <c r="R56"/>
-    </row>
-    <row r="57" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="57" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>108</v>
+        <v>216</v>
       </c>
       <c r="D57" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E57" t="s">
-        <v>109</v>
+        <v>12</v>
+      </c>
+      <c r="F57" t="s">
+        <v>14</v>
+      </c>
+      <c r="G57" t="s">
+        <v>12</v>
       </c>
       <c r="H57">
         <v>1</v>
       </c>
       <c r="I57">
-        <v>43.82</v>
-      </c>
-      <c r="P57" s="2"/>
-      <c r="R57"/>
-    </row>
-    <row r="58" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>257</v>
-      </c>
-      <c r="D58" t="s">
-        <v>19</v>
-      </c>
-      <c r="E58" t="s">
-        <v>22</v>
-      </c>
-      <c r="F58" t="s">
-        <v>23</v>
-      </c>
-      <c r="G58" t="s">
-        <v>127</v>
-      </c>
-      <c r="H58">
-        <v>1</v>
-      </c>
-      <c r="I58">
-        <v>20.25</v>
-      </c>
-      <c r="P58" s="2"/>
-      <c r="R58"/>
-    </row>
-    <row r="59" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P59" s="2"/>
-      <c r="R59"/>
-    </row>
-    <row r="60" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="59" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="60" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>258</v>
-      </c>
-      <c r="P60" s="2"/>
-      <c r="R60"/>
-    </row>
-    <row r="61" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+      <c r="F60" t="s">
+        <v>205</v>
+      </c>
+      <c r="G60" t="s">
+        <v>251</v>
+      </c>
+      <c r="H60">
+        <v>1</v>
+      </c>
+      <c r="I60">
+        <v>19.32</v>
+      </c>
+    </row>
+    <row r="61" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>118</v>
+        <v>287</v>
       </c>
       <c r="D61" t="s">
-        <v>19</v>
+        <v>201</v>
       </c>
       <c r="E61" t="s">
-        <v>18</v>
+        <v>286</v>
       </c>
       <c r="F61" t="s">
-        <v>20</v>
+        <v>289</v>
       </c>
       <c r="G61" t="s">
-        <v>126</v>
+        <v>288</v>
       </c>
       <c r="H61">
         <v>1</v>
       </c>
       <c r="I61">
-        <v>19.54</v>
-      </c>
-      <c r="P61" s="2"/>
-      <c r="R61"/>
-    </row>
-    <row r="62" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P62" s="2"/>
-      <c r="R62"/>
-    </row>
-    <row r="63" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>254</v>
-      </c>
-      <c r="P63" s="2"/>
-      <c r="R63"/>
-    </row>
-    <row r="64" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>232</v>
-      </c>
-      <c r="D64" t="s">
-        <v>16</v>
-      </c>
-      <c r="E64" t="s">
-        <v>15</v>
-      </c>
-      <c r="F64" t="s">
-        <v>17</v>
-      </c>
-      <c r="G64" t="s">
-        <v>15</v>
-      </c>
-      <c r="H64">
-        <v>1</v>
-      </c>
-      <c r="I64">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="66" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="67" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>268</v>
-      </c>
-      <c r="F67" t="s">
-        <v>221</v>
-      </c>
-      <c r="G67" t="s">
-        <v>267</v>
-      </c>
-      <c r="H67">
-        <v>1</v>
-      </c>
-      <c r="I67">
-        <v>19.32</v>
-      </c>
-    </row>
-    <row r="68" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>309</v>
-      </c>
-      <c r="D68" t="s">
-        <v>217</v>
-      </c>
-      <c r="E68" t="s">
-        <v>308</v>
-      </c>
-      <c r="F68" t="s">
-        <v>311</v>
-      </c>
-      <c r="G68" t="s">
-        <v>310</v>
-      </c>
-      <c r="H68">
-        <v>1</v>
-      </c>
-      <c r="I68">
         <v>14.65</v>
       </c>
     </row>
@@ -3983,13 +3640,10 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Unit Price" prompt="Price per part" sqref="I1" xr:uid="{333F752F-542B-4332-A90F-F9290A7923E6}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total Price" prompt="Quantity * Unit Price" sqref="J1" xr:uid="{34FED5B6-934B-4D29-85D8-FB3294449BDF}"/>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="E22" r:id="rId1" xr:uid="{C773AB1E-DDC5-490E-8A13-59B58C73755C}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -3998,7 +3652,7 @@
           <x14:formula1>
             <xm:f>Helper!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C50</xm:sqref>
+          <xm:sqref>C2:C47</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4011,7 +3665,7 @@
   <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="I23" sqref="A23:I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4030,25 +3684,25 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="B1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>272</v>
+        <v>256</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="H1" t="s">
         <v>0</v>
@@ -4057,27 +3711,27 @@
         <v>1</v>
       </c>
       <c r="J1" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>212</v>
+        <v>353</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="C2" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -4092,22 +3746,22 @@
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="B3" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G3" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -4122,19 +3776,19 @@
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
         <v>6</v>
       </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
       <c r="G4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -4149,22 +3803,22 @@
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>359</v>
+        <v>334</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G5" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="H5">
         <v>2</v>
@@ -4179,22 +3833,22 @@
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>360</v>
+        <v>335</v>
       </c>
       <c r="B6" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G6" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -4209,13 +3863,13 @@
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>361</v>
+        <v>336</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="F7" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="G7">
         <v>3985</v>
@@ -4233,19 +3887,19 @@
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>362</v>
+        <v>337</v>
       </c>
       <c r="B8" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="G8">
         <v>4540</v>
@@ -4263,16 +3917,16 @@
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>363</v>
+        <v>338</v>
       </c>
       <c r="B9" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="F9" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="G9" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -4282,22 +3936,22 @@
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>350</v>
+        <v>326</v>
       </c>
       <c r="B10" t="s">
-        <v>352</v>
+        <v>328</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G10" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="H10">
         <v>7</v>
@@ -4312,22 +3966,22 @@
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="B11" t="s">
-        <v>351</v>
+        <v>327</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>348</v>
+        <v>324</v>
       </c>
       <c r="F11" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="G11" t="s">
-        <v>346</v>
+        <v>322</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1">
@@ -4337,22 +3991,22 @@
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>364</v>
+        <v>339</v>
       </c>
       <c r="B12" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G12" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -4367,22 +4021,22 @@
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>365</v>
+        <v>340</v>
       </c>
       <c r="B13" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E13" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F13" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G13" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -4397,22 +4051,22 @@
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>366</v>
+        <v>341</v>
       </c>
       <c r="B14" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E14" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F14" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G14" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="H14">
         <v>5</v>
@@ -4427,22 +4081,22 @@
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>367</v>
+        <v>342</v>
       </c>
       <c r="B15" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E15" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F15" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G15" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="H15">
         <v>7</v>
@@ -4457,22 +4111,22 @@
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>368</v>
+        <v>343</v>
       </c>
       <c r="B16" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E16" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F16" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G16" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="H16">
         <v>7</v>
@@ -4487,22 +4141,22 @@
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>369</v>
+        <v>344</v>
       </c>
       <c r="B17" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E17" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F17" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G17" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="H17">
         <v>4</v>
@@ -4517,22 +4171,22 @@
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>370</v>
+        <v>345</v>
       </c>
       <c r="B18" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="D18" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F18" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G18" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="H18">
         <v>4</v>
@@ -4547,22 +4201,22 @@
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>371</v>
+        <v>346</v>
       </c>
       <c r="B19" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E19" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F19" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G19" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="H19">
         <v>4</v>
@@ -4577,22 +4231,22 @@
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>372</v>
+        <v>347</v>
       </c>
       <c r="B20" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="D20" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E20" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F20" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G20" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="H20">
         <v>4</v>
@@ -4607,22 +4261,22 @@
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>373</v>
+        <v>348</v>
       </c>
       <c r="B21" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="D21" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F21" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G21" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="H21">
         <v>2</v>
@@ -4637,22 +4291,22 @@
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>374</v>
+        <v>349</v>
       </c>
       <c r="B22" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="D22" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E22" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F22" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G22" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="H22">
         <v>2</v>
@@ -4667,16 +4321,16 @@
     </row>
     <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>375</v>
+        <v>350</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F23" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -4691,10 +4345,10 @@
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>338</v>
+        <v>314</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -4716,7 +4370,7 @@
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
@@ -4729,27 +4383,27 @@
     </row>
     <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>377</v>
+        <v>352</v>
       </c>
       <c r="B27" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="D27" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E27" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="F27" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="G27" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="H27">
         <v>2</v>
@@ -4760,24 +4414,24 @@
     </row>
     <row r="29" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D30" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E30" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="F30" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="G30" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="H30">
         <v>3</v>
@@ -4788,13 +4442,13 @@
     </row>
     <row r="31" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="F31" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G31" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="H31">
         <v>1</v>
@@ -4805,16 +4459,16 @@
     </row>
     <row r="32" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="D32" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E32" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F32" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="G32">
         <v>4685</v>
@@ -4828,24 +4482,24 @@
     </row>
     <row r="34" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
     </row>
     <row r="35" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="D35" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E35" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F35" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="G35" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="H35">
         <v>2</v>
@@ -4856,24 +4510,24 @@
     </row>
     <row r="37" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
     </row>
     <row r="38" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="D38" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E38" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="F38" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="G38" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H38">
         <v>1</v>
@@ -4884,13 +4538,13 @@
     </row>
     <row r="39" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="D39" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E39" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="H39">
         <v>1</v>
@@ -4936,7 +4590,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4955,25 +4609,25 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="B1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>272</v>
+        <v>256</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="H1" t="s">
         <v>0</v>
@@ -4982,25 +4636,25 @@
         <v>1</v>
       </c>
       <c r="J1" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="G2" s="4">
         <v>181</v>
@@ -5018,19 +4672,19 @@
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="G3">
         <v>292</v>
@@ -5048,19 +4702,19 @@
     </row>
     <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="H4">
         <v>5</v>
@@ -5076,19 +4730,19 @@
     <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
         <v>27</v>
       </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="H5">
         <v>4</v>
@@ -5104,17 +4758,17 @@
     <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -5129,25 +4783,25 @@
     </row>
     <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>354</v>
+        <v>329</v>
       </c>
       <c r="B7" t="s">
-        <v>358</v>
+        <v>333</v>
       </c>
       <c r="C7" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>355</v>
+        <v>330</v>
       </c>
       <c r="F7" t="s">
-        <v>356</v>
+        <v>331</v>
       </c>
       <c r="G7" t="s">
-        <v>357</v>
+        <v>332</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -5164,7 +4818,7 @@
     </row>
     <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="J8" s="2">
         <f>SUBTOTAL(109,TableController[Total Price])</f>
@@ -5175,26 +4829,26 @@
     </row>
     <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
     </row>
     <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F10" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="G10" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -5205,19 +4859,19 @@
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G11" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -5228,24 +4882,24 @@
     </row>
     <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>260</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="D14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G14" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -5256,13 +4910,13 @@
     </row>
     <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="F15" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="G15" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -5273,19 +4927,19 @@
     </row>
     <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F16" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G16" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="H16">
         <v>2</v>
@@ -5296,19 +4950,19 @@
     </row>
     <row r="17" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E17" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F17" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G17" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -5362,22 +5016,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>273</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>271</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>